<commit_message>
Fix bug superhost e nomenclatura
</commit_message>
<xml_diff>
--- a/araruama_stats.xlsx
+++ b/araruama_stats.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="124">
   <si>
     <t>title</t>
   </si>
@@ -31,30 +31,30 @@
     <t>rating</t>
   </si>
   <si>
-    <t>is_superhost</t>
+    <t>superhost</t>
   </si>
   <si>
     <t>Casa em Araruama</t>
   </si>
   <si>
+    <t>Casa em Parque Hotel</t>
+  </si>
+  <si>
     <t>Apartamento em Araruama</t>
   </si>
   <si>
-    <t>Casa em Parque Hotel</t>
-  </si>
-  <si>
     <t>Casa em Fazendinha</t>
   </si>
   <si>
     <t>Casa de campo em Praia Seca</t>
   </si>
   <si>
+    <t>Chalé em Coqueiral</t>
+  </si>
+  <si>
     <t>Casa de campo em Outeiro</t>
   </si>
   <si>
-    <t>Chalé em Coqueiral</t>
-  </si>
-  <si>
     <t>Quarto privativo em Araruama</t>
   </si>
   <si>
@@ -70,22 +70,25 @@
     <t>Região dos lagos - Araruama - Saquarema - Arraial</t>
   </si>
   <si>
+    <t>Aconchegante Casa - Quintal &amp; Garagem</t>
+  </si>
+  <si>
     <t>Casa em Araruama 1</t>
   </si>
   <si>
     <t>Pedacinho do Céu</t>
   </si>
   <si>
+    <t>Recanto para curtir e relaxar em Araruama</t>
+  </si>
+  <si>
+    <t>Apartamento em frente a lagoa de Araruama</t>
+  </si>
+  <si>
     <t>Casa tranquila, bem localizada Ar opcional Tv wifi</t>
   </si>
   <si>
-    <t>Apartamento em frente a lagoa de Araruama</t>
-  </si>
-  <si>
-    <t>Recanto para curtir e relaxar em Araruama</t>
-  </si>
-  <si>
-    <t>Aconchegante Casa - Quintal &amp; Garagem</t>
+    <t>loft &lt;SPA&lt; onde você descansa relaxa e se renova</t>
   </si>
   <si>
     <t>Meu aconchego</t>
@@ -97,40 +100,37 @@
     <t>Casa Maravilhosa com Lagoa privativa</t>
   </si>
   <si>
-    <t>Casa recanto Coqueiral</t>
+    <t>Chalé Recantinho da Lagoa, Araruama,Rj</t>
   </si>
   <si>
     <t>Casa com piscina no Condomínio Sonho de Vida</t>
   </si>
   <si>
-    <t>loft &lt;SPA&lt; onde você descansa relaxa e se renova</t>
-  </si>
-  <si>
-    <t>Chalé Recantinho da Lagoa, Araruama,Rj</t>
+    <t>Apto na Região dos lagos. Aconchegante e central.</t>
+  </si>
+  <si>
+    <t>Suíte aconchegante no centro de Praia Seca.</t>
+  </si>
+  <si>
+    <t>Curta o melhor de Araruama e Região dos Lagos</t>
+  </si>
+  <si>
+    <t>VEM! Casa Rodrigues - Praia Seca, Araruama</t>
+  </si>
+  <si>
+    <t>Aluguel por temporada com piscina privativa</t>
+  </si>
+  <si>
+    <t>Casarão com Piscina poucos passos do Mar (PRAIA)</t>
+  </si>
+  <si>
+    <t>Praia pertinho! 4 suítes, Piscina e Churrasqueira</t>
+  </si>
+  <si>
+    <t>Apartamento à beira da orla de Araruama</t>
   </si>
   <si>
     <t>Loft agradável em Araruama.</t>
-  </si>
-  <si>
-    <t>VEM! Casa Rodrigues - Praia Seca, Araruama</t>
-  </si>
-  <si>
-    <t>Apto na Região dos lagos. Aconchegante e central.</t>
-  </si>
-  <si>
-    <t>Aluguel por temporada com piscina privativa</t>
-  </si>
-  <si>
-    <t>Curta o melhor de Araruama e Região dos Lagos</t>
-  </si>
-  <si>
-    <t>Praia pertinho! 4 suítes, Piscina e Churrasqueira</t>
-  </si>
-  <si>
-    <t>Casarão com Piscina poucos passos do Mar (PRAIA)</t>
-  </si>
-  <si>
-    <t>Apartamento à beira da orla de Araruama</t>
   </si>
   <si>
     <t>Casa em praia seca com piscina e um belo jardim</t>
@@ -168,36 +168,36 @@
     <t>2 camas de casal</t>
   </si>
   <si>
+    <t>1 cama queen</t>
+  </si>
+  <si>
     <t>4 camas</t>
   </si>
   <si>
     <t>1 cama de casal</t>
   </si>
   <si>
+    <t>3 camas</t>
+  </si>
+  <si>
     <t>2 camas</t>
   </si>
   <si>
-    <t>3 camas</t>
-  </si>
-  <si>
-    <t>1 cama queen</t>
-  </si>
-  <si>
     <t>9 camas</t>
   </si>
   <si>
     <t>3 camas de casal</t>
   </si>
   <si>
+    <t>5 camas</t>
+  </si>
+  <si>
+    <t>10 camas</t>
+  </si>
+  <si>
     <t>1 cama</t>
   </si>
   <si>
-    <t>10 camas</t>
-  </si>
-  <si>
-    <t>5 camas</t>
-  </si>
-  <si>
     <t>13 camas</t>
   </si>
   <si>
@@ -207,22 +207,25 @@
     <t>R$110 por noite</t>
   </si>
   <si>
+    <t>R$137 por noite</t>
+  </si>
+  <si>
     <t>R$106 por noite</t>
   </si>
   <si>
     <t>R$96 por noite</t>
   </si>
   <si>
+    <t>R$210 por noite</t>
+  </si>
+  <si>
+    <t>R$173 por noite, originalmente R$211</t>
+  </si>
+  <si>
     <t>R$118 por noite</t>
   </si>
   <si>
-    <t>R$173 por noite, originalmente R$211</t>
-  </si>
-  <si>
-    <t>R$210 por noite</t>
-  </si>
-  <si>
-    <t>R$137 por noite</t>
+    <t>R$189 por noite, originalmente R$302</t>
   </si>
   <si>
     <t>R$187 por noite, originalmente R$235</t>
@@ -231,42 +234,39 @@
     <t>R$117 por noite</t>
   </si>
   <si>
-    <t>R$345 por noite</t>
+    <t>R$91 por noite</t>
   </si>
   <si>
     <t>R$290 por noite, originalmente R$352</t>
   </si>
   <si>
-    <t>R$189 por noite, originalmente R$302</t>
-  </si>
-  <si>
-    <t>R$91 por noite</t>
+    <t>R$140 por noite</t>
+  </si>
+  <si>
+    <t>R$136 por noite, originalmente R$166</t>
+  </si>
+  <si>
+    <t>R$133 por noite</t>
+  </si>
+  <si>
+    <t>R$116 por noite, originalmente R$137</t>
+  </si>
+  <si>
+    <t>R$315 por noite</t>
+  </si>
+  <si>
+    <t>R$599 por noite</t>
+  </si>
+  <si>
+    <t>R$326 por noite, originalmente R$358</t>
+  </si>
+  <si>
+    <t>R$228 por noite</t>
   </si>
   <si>
     <t>R$136 por noite</t>
   </si>
   <si>
-    <t>R$116 por noite, originalmente R$137</t>
-  </si>
-  <si>
-    <t>R$140 por noite</t>
-  </si>
-  <si>
-    <t>R$315 por noite</t>
-  </si>
-  <si>
-    <t>R$133 por noite</t>
-  </si>
-  <si>
-    <t>R$326 por noite, originalmente R$358</t>
-  </si>
-  <si>
-    <t>R$599 por noite</t>
-  </si>
-  <si>
-    <t>R$228 por noite</t>
-  </si>
-  <si>
     <t>R$314 por noite</t>
   </si>
   <si>
@@ -300,22 +300,25 @@
     <t>4,79 (282)</t>
   </si>
   <si>
+    <t>4,89 (46)</t>
+  </si>
+  <si>
     <t>4,97 (158)</t>
   </si>
   <si>
     <t>4,92 (12)</t>
   </si>
   <si>
+    <t>5,0 (29)</t>
+  </si>
+  <si>
+    <t>4,85 (26)</t>
+  </si>
+  <si>
     <t>4,9 (21)</t>
   </si>
   <si>
-    <t>4,85 (26)</t>
-  </si>
-  <si>
-    <t>5,0 (29)</t>
-  </si>
-  <si>
-    <t>4,89 (46)</t>
+    <t>5,0 (9)</t>
   </si>
   <si>
     <t>4,89 (9)</t>
@@ -327,39 +330,39 @@
     <t>4,75 (20)</t>
   </si>
   <si>
+    <t>4,84 (75)</t>
+  </si>
+  <si>
+    <t>5,0 (21)</t>
+  </si>
+  <si>
+    <t>4,71 (7)</t>
+  </si>
+  <si>
+    <t>5,0 (11)</t>
+  </si>
+  <si>
+    <t>4,89 (28)</t>
+  </si>
+  <si>
+    <t>4,92 (173)</t>
+  </si>
+  <si>
+    <t>4,97 (66)</t>
+  </si>
+  <si>
+    <t>5,0 (16)</t>
+  </si>
+  <si>
+    <t>4,74 (70)</t>
+  </si>
+  <si>
+    <t>4,44 (9)</t>
+  </si>
+  <si>
     <t>Novo</t>
   </si>
   <si>
-    <t>5,0 (21)</t>
-  </si>
-  <si>
-    <t>5,0 (9)</t>
-  </si>
-  <si>
-    <t>4,84 (75)</t>
-  </si>
-  <si>
-    <t>4,92 (173)</t>
-  </si>
-  <si>
-    <t>4,71 (7)</t>
-  </si>
-  <si>
-    <t>4,97 (66)</t>
-  </si>
-  <si>
-    <t>4,89 (28)</t>
-  </si>
-  <si>
-    <t>4,74 (70)</t>
-  </si>
-  <si>
-    <t>5,0 (16)</t>
-  </si>
-  <si>
-    <t>4,44 (9)</t>
-  </si>
-  <si>
     <t>4,97 (37)</t>
   </si>
   <si>
@@ -384,7 +387,7 @@
     <t>4,95 (73)</t>
   </si>
   <si>
-    <t>&lt;div class="t1mwk1n0 dir dir-ltr"&gt;Superhost&lt;/div&gt;</t>
+    <t>Superhost</t>
   </si>
 </sst>
 </file>
@@ -787,7 +790,7 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B3" t="s">
         <v>18</v>
@@ -802,7 +805,7 @@
         <v>94</v>
       </c>
       <c r="F3" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -822,7 +825,7 @@
         <v>95</v>
       </c>
       <c r="F4" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -842,18 +845,18 @@
         <v>96</v>
       </c>
       <c r="F5" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B6" t="s">
         <v>21</v>
       </c>
       <c r="C6" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D6" t="s">
         <v>66</v>
@@ -861,16 +864,19 @@
       <c r="E6" t="s">
         <v>97</v>
       </c>
+      <c r="F6" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B7" t="s">
         <v>22</v>
       </c>
       <c r="C7" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D7" t="s">
         <v>67</v>
@@ -878,13 +884,10 @@
       <c r="E7" t="s">
         <v>98</v>
       </c>
-      <c r="F7" t="s">
-        <v>122</v>
-      </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B8" t="s">
         <v>23</v>
@@ -899,7 +902,7 @@
         <v>99</v>
       </c>
       <c r="F8" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -910,7 +913,7 @@
         <v>24</v>
       </c>
       <c r="C9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D9" t="s">
         <v>69</v>
@@ -918,53 +921,56 @@
       <c r="E9" t="s">
         <v>100</v>
       </c>
+      <c r="F9" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B10" t="s">
         <v>25</v>
       </c>
       <c r="C10" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="D10" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="E10" t="s">
         <v>101</v>
       </c>
-      <c r="F10" t="s">
-        <v>122</v>
-      </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11" t="s">
         <v>26</v>
       </c>
       <c r="C11" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="D11" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E11" t="s">
         <v>102</v>
       </c>
+      <c r="F11" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B12" t="s">
         <v>27</v>
       </c>
       <c r="C12" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="D12" t="s">
         <v>71</v>
@@ -981,7 +987,7 @@
         <v>28</v>
       </c>
       <c r="C13" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="D13" t="s">
         <v>72</v>
@@ -989,19 +995,16 @@
       <c r="E13" t="s">
         <v>104</v>
       </c>
-      <c r="F13" t="s">
-        <v>122</v>
-      </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B14" t="s">
         <v>29</v>
       </c>
       <c r="C14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D14" t="s">
         <v>73</v>
@@ -1010,18 +1013,18 @@
         <v>105</v>
       </c>
       <c r="F14" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B15" t="s">
         <v>30</v>
       </c>
       <c r="C15" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D15" t="s">
         <v>74</v>
@@ -1032,24 +1035,27 @@
     </row>
     <row r="16" spans="1:6">
       <c r="A16" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="B16" t="s">
         <v>31</v>
       </c>
       <c r="C16" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="D16" t="s">
         <v>75</v>
       </c>
       <c r="E16" t="s">
-        <v>103</v>
+        <v>107</v>
+      </c>
+      <c r="F16" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B17" t="s">
         <v>32</v>
@@ -1061,15 +1067,15 @@
         <v>76</v>
       </c>
       <c r="E17" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="F17" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="B18" t="s">
         <v>33</v>
@@ -1081,7 +1087,10 @@
         <v>77</v>
       </c>
       <c r="E18" t="s">
-        <v>108</v>
+        <v>109</v>
+      </c>
+      <c r="F18" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -1098,30 +1107,30 @@
         <v>78</v>
       </c>
       <c r="E19" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="F19" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B20" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C20" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D20" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="E20" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="F20" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -1129,36 +1138,36 @@
         <v>6</v>
       </c>
       <c r="B21" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C21" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D21" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E21" t="s">
         <v>111</v>
       </c>
+      <c r="F21" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" t="s">
         <v>6</v>
       </c>
       <c r="B22" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C22" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D22" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E22" t="s">
         <v>112</v>
-      </c>
-      <c r="F22" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -1166,13 +1175,13 @@
         <v>14</v>
       </c>
       <c r="B23" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C23" t="s">
         <v>53</v>
       </c>
       <c r="D23" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E23" t="s">
         <v>113</v>
@@ -1183,19 +1192,19 @@
         <v>6</v>
       </c>
       <c r="B24" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="C24" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D24" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="E24" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="F24" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -1203,73 +1212,73 @@
         <v>6</v>
       </c>
       <c r="B25" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="C25" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D25" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="E25" t="s">
-        <v>103</v>
+        <v>114</v>
       </c>
     </row>
     <row r="26" spans="1:6">
       <c r="A26" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B26" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C26" t="s">
         <v>53</v>
       </c>
       <c r="D26" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E26" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="27" spans="1:6">
       <c r="A27" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="B27" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="C27" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="D27" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="E27" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="F27" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="28" spans="1:6">
       <c r="A28" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="B28" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="C28" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="D28" t="s">
-        <v>76</v>
+        <v>83</v>
       </c>
       <c r="E28" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
       <c r="F28" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -1286,10 +1295,10 @@
         <v>84</v>
       </c>
       <c r="E29" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="F29" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -1300,13 +1309,13 @@
         <v>41</v>
       </c>
       <c r="C30" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D30" t="s">
         <v>85</v>
       </c>
       <c r="E30" t="s">
-        <v>103</v>
+        <v>114</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -1323,7 +1332,7 @@
         <v>86</v>
       </c>
       <c r="E31" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="32" spans="1:6">
@@ -1340,24 +1349,24 @@
         <v>87</v>
       </c>
       <c r="E32" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="33" spans="1:6">
       <c r="A33" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B33" t="s">
         <v>44</v>
       </c>
       <c r="C33" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D33" t="s">
         <v>88</v>
       </c>
       <c r="E33" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="34" spans="1:6">
@@ -1368,13 +1377,13 @@
         <v>45</v>
       </c>
       <c r="C34" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D34" t="s">
         <v>89</v>
       </c>
       <c r="E34" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="35" spans="1:6">
@@ -1385,13 +1394,13 @@
         <v>46</v>
       </c>
       <c r="C35" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D35" t="s">
         <v>90</v>
       </c>
       <c r="E35" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="36" spans="1:6">
@@ -1402,36 +1411,36 @@
         <v>47</v>
       </c>
       <c r="C36" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D36" t="s">
         <v>91</v>
       </c>
       <c r="E36" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="F36" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="37" spans="1:6">
       <c r="A37" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B37" t="s">
         <v>48</v>
       </c>
       <c r="C37" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D37" t="s">
         <v>92</v>
       </c>
       <c r="E37" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="F37" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adicionado mais 3 páginas de WebScraping.
</commit_message>
<xml_diff>
--- a/araruama_stats.xlsx
+++ b/araruama_stats.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:U37"/>
+  <dimension ref="A1:U91"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -577,13 +577,13 @@
       <c r="R2" t="inlineStr"/>
       <c r="S2" t="inlineStr">
         <is>
-          <t>R$ 189.17</t>
+          <t>R$ 239.19</t>
         </is>
       </c>
       <c r="T2" t="inlineStr"/>
       <c r="U2" t="inlineStr">
         <is>
-          <t>27/04/2023 15:00:13</t>
+          <t>27/04/2023 15:23:27</t>
         </is>
       </c>
     </row>
@@ -597,7 +597,7 @@
       <c r="C3" t="inlineStr"/>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Casa em Araruama 1</t>
+          <t>Pedacinho do Céu</t>
         </is>
       </c>
       <c r="E3" t="inlineStr"/>
@@ -606,13 +606,13 @@
       <c r="H3" t="inlineStr"/>
       <c r="I3" t="inlineStr">
         <is>
-          <t>4 camas</t>
+          <t>1 cama de casal</t>
         </is>
       </c>
       <c r="J3" t="inlineStr"/>
       <c r="K3" t="inlineStr">
         <is>
-          <t>R$106 por noite</t>
+          <t>R$85 por noite, originalmente R$93</t>
         </is>
       </c>
       <c r="L3" t="inlineStr"/>
@@ -620,7 +620,7 @@
       <c r="N3" t="inlineStr"/>
       <c r="O3" t="inlineStr">
         <is>
-          <t>4,97 (159)</t>
+          <t>4,92 (12)</t>
         </is>
       </c>
       <c r="P3" t="inlineStr"/>
@@ -632,27 +632,27 @@
       <c r="R3" t="inlineStr"/>
       <c r="S3" t="inlineStr">
         <is>
-          <t>R$ 189.17</t>
+          <t>R$ 239.19</t>
         </is>
       </c>
       <c r="T3" t="inlineStr"/>
       <c r="U3" t="inlineStr">
         <is>
-          <t>27/04/2023 15:00:13</t>
+          <t>27/04/2023 15:23:27</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Casa em Araruama</t>
+          <t>Casa em Parque Hotel</t>
         </is>
       </c>
       <c r="B4" t="inlineStr"/>
       <c r="C4" t="inlineStr"/>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Pedacinho do Céu</t>
+          <t>Aconchegante Casa - Quintal &amp; Garagem</t>
         </is>
       </c>
       <c r="E4" t="inlineStr"/>
@@ -661,13 +661,13 @@
       <c r="H4" t="inlineStr"/>
       <c r="I4" t="inlineStr">
         <is>
-          <t>1 cama de casal</t>
+          <t>1 cama queen</t>
         </is>
       </c>
       <c r="J4" t="inlineStr"/>
       <c r="K4" t="inlineStr">
         <is>
-          <t>R$85 por noite, originalmente R$93</t>
+          <t>R$137 por noite</t>
         </is>
       </c>
       <c r="L4" t="inlineStr"/>
@@ -675,7 +675,7 @@
       <c r="N4" t="inlineStr"/>
       <c r="O4" t="inlineStr">
         <is>
-          <t>4,92 (12)</t>
+          <t>4,89 (46)</t>
         </is>
       </c>
       <c r="P4" t="inlineStr"/>
@@ -687,27 +687,27 @@
       <c r="R4" t="inlineStr"/>
       <c r="S4" t="inlineStr">
         <is>
-          <t>R$ 189.17</t>
+          <t>R$ 239.19</t>
         </is>
       </c>
       <c r="T4" t="inlineStr"/>
       <c r="U4" t="inlineStr">
         <is>
-          <t>27/04/2023 15:00:13</t>
+          <t>27/04/2023 15:23:27</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Apartamento em Araruama</t>
+          <t>Casa em Fazendinha</t>
         </is>
       </c>
       <c r="B5" t="inlineStr"/>
       <c r="C5" t="inlineStr"/>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Apartamento em frente a lagoa de Araruama</t>
+          <t>Casa em Araruama 2</t>
         </is>
       </c>
       <c r="E5" t="inlineStr"/>
@@ -716,13 +716,13 @@
       <c r="H5" t="inlineStr"/>
       <c r="I5" t="inlineStr">
         <is>
-          <t>2 camas</t>
+          <t>4 camas</t>
         </is>
       </c>
       <c r="J5" t="inlineStr"/>
       <c r="K5" t="inlineStr">
         <is>
-          <t>R$173 por noite, originalmente R$211</t>
+          <t>R$98 por noite, originalmente R$109</t>
         </is>
       </c>
       <c r="L5" t="inlineStr"/>
@@ -730,21 +730,25 @@
       <c r="N5" t="inlineStr"/>
       <c r="O5" t="inlineStr">
         <is>
-          <t>4,85 (26)</t>
+          <t>5,0 (27)</t>
         </is>
       </c>
       <c r="P5" t="inlineStr"/>
-      <c r="Q5" t="inlineStr"/>
+      <c r="Q5" t="inlineStr">
+        <is>
+          <t>Superhost</t>
+        </is>
+      </c>
       <c r="R5" t="inlineStr"/>
       <c r="S5" t="inlineStr">
         <is>
-          <t>R$ 189.17</t>
+          <t>R$ 239.19</t>
         </is>
       </c>
       <c r="T5" t="inlineStr"/>
       <c r="U5" t="inlineStr">
         <is>
-          <t>27/04/2023 15:00:13</t>
+          <t>27/04/2023 15:23:27</t>
         </is>
       </c>
     </row>
@@ -758,7 +762,7 @@
       <c r="C6" t="inlineStr"/>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Meu aconchego</t>
+          <t>Casa em Araruama 1</t>
         </is>
       </c>
       <c r="E6" t="inlineStr"/>
@@ -767,13 +771,13 @@
       <c r="H6" t="inlineStr"/>
       <c r="I6" t="inlineStr">
         <is>
-          <t>9 camas</t>
+          <t>4 camas</t>
         </is>
       </c>
       <c r="J6" t="inlineStr"/>
       <c r="K6" t="inlineStr">
         <is>
-          <t>R$202 por noite, originalmente R$222</t>
+          <t>R$106 por noite</t>
         </is>
       </c>
       <c r="L6" t="inlineStr"/>
@@ -781,35 +785,39 @@
       <c r="N6" t="inlineStr"/>
       <c r="O6" t="inlineStr">
         <is>
-          <t>4,9 (10)</t>
+          <t>4,97 (159)</t>
         </is>
       </c>
       <c r="P6" t="inlineStr"/>
-      <c r="Q6" t="inlineStr"/>
+      <c r="Q6" t="inlineStr">
+        <is>
+          <t>Superhost</t>
+        </is>
+      </c>
       <c r="R6" t="inlineStr"/>
       <c r="S6" t="inlineStr">
         <is>
-          <t>R$ 189.17</t>
+          <t>R$ 239.19</t>
         </is>
       </c>
       <c r="T6" t="inlineStr"/>
       <c r="U6" t="inlineStr">
         <is>
-          <t>27/04/2023 15:00:13</t>
+          <t>27/04/2023 15:23:27</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Casa em Parque Hotel</t>
+          <t>Casa em Araruama</t>
         </is>
       </c>
       <c r="B7" t="inlineStr"/>
       <c r="C7" t="inlineStr"/>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Aconchegante Casa - Quintal &amp; Garagem</t>
+          <t>Meu aconchego</t>
         </is>
       </c>
       <c r="E7" t="inlineStr"/>
@@ -818,13 +826,13 @@
       <c r="H7" t="inlineStr"/>
       <c r="I7" t="inlineStr">
         <is>
-          <t>1 cama queen</t>
+          <t>9 camas</t>
         </is>
       </c>
       <c r="J7" t="inlineStr"/>
       <c r="K7" t="inlineStr">
         <is>
-          <t>R$137 por noite</t>
+          <t>R$202 por noite, originalmente R$222</t>
         </is>
       </c>
       <c r="L7" t="inlineStr"/>
@@ -832,39 +840,35 @@
       <c r="N7" t="inlineStr"/>
       <c r="O7" t="inlineStr">
         <is>
-          <t>4,89 (46)</t>
+          <t>4,9 (10)</t>
         </is>
       </c>
       <c r="P7" t="inlineStr"/>
-      <c r="Q7" t="inlineStr">
-        <is>
-          <t>Superhost</t>
-        </is>
-      </c>
+      <c r="Q7" t="inlineStr"/>
       <c r="R7" t="inlineStr"/>
       <c r="S7" t="inlineStr">
         <is>
-          <t>R$ 189.17</t>
+          <t>R$ 239.19</t>
         </is>
       </c>
       <c r="T7" t="inlineStr"/>
       <c r="U7" t="inlineStr">
         <is>
-          <t>27/04/2023 15:00:13</t>
+          <t>27/04/2023 15:23:27</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Casa em Fazendinha</t>
+          <t>Apartamento em Araruama</t>
         </is>
       </c>
       <c r="B8" t="inlineStr"/>
       <c r="C8" t="inlineStr"/>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Casa em Araruama 2</t>
+          <t>Apartamento em frente a lagoa de Araruama</t>
         </is>
       </c>
       <c r="E8" t="inlineStr"/>
@@ -873,13 +877,13 @@
       <c r="H8" t="inlineStr"/>
       <c r="I8" t="inlineStr">
         <is>
-          <t>4 camas</t>
+          <t>2 camas</t>
         </is>
       </c>
       <c r="J8" t="inlineStr"/>
       <c r="K8" t="inlineStr">
         <is>
-          <t>R$98 por noite, originalmente R$109</t>
+          <t>R$173 por noite, originalmente R$211</t>
         </is>
       </c>
       <c r="L8" t="inlineStr"/>
@@ -887,25 +891,21 @@
       <c r="N8" t="inlineStr"/>
       <c r="O8" t="inlineStr">
         <is>
-          <t>5,0 (27)</t>
+          <t>4,85 (26)</t>
         </is>
       </c>
       <c r="P8" t="inlineStr"/>
-      <c r="Q8" t="inlineStr">
-        <is>
-          <t>Superhost</t>
-        </is>
-      </c>
+      <c r="Q8" t="inlineStr"/>
       <c r="R8" t="inlineStr"/>
       <c r="S8" t="inlineStr">
         <is>
-          <t>R$ 189.17</t>
+          <t>R$ 239.19</t>
         </is>
       </c>
       <c r="T8" t="inlineStr"/>
       <c r="U8" t="inlineStr">
         <is>
-          <t>27/04/2023 15:00:13</t>
+          <t>27/04/2023 15:23:27</t>
         </is>
       </c>
     </row>
@@ -954,27 +954,27 @@
       <c r="R9" t="inlineStr"/>
       <c r="S9" t="inlineStr">
         <is>
-          <t>R$ 189.17</t>
+          <t>R$ 239.19</t>
         </is>
       </c>
       <c r="T9" t="inlineStr"/>
       <c r="U9" t="inlineStr">
         <is>
-          <t>27/04/2023 15:00:13</t>
+          <t>27/04/2023 15:23:27</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Casa de campo em Praia Seca</t>
+          <t>Casa em Araruama</t>
         </is>
       </c>
       <c r="B10" t="inlineStr"/>
       <c r="C10" t="inlineStr"/>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Casa Maravilhosa com Lagoa privativa</t>
+          <t>loft &lt;SPA&lt; onde você descansa relaxa e se renova</t>
         </is>
       </c>
       <c r="E10" t="inlineStr"/>
@@ -983,13 +983,13 @@
       <c r="H10" t="inlineStr"/>
       <c r="I10" t="inlineStr">
         <is>
-          <t>3 camas de casal</t>
+          <t>2 camas</t>
         </is>
       </c>
       <c r="J10" t="inlineStr"/>
       <c r="K10" t="inlineStr">
         <is>
-          <t>R$117 por noite</t>
+          <t>R$189 por noite, originalmente R$302</t>
         </is>
       </c>
       <c r="L10" t="inlineStr"/>
@@ -997,21 +997,25 @@
       <c r="N10" t="inlineStr"/>
       <c r="O10" t="inlineStr">
         <is>
-          <t>4,77 (22)</t>
+          <t>5,0 (9)</t>
         </is>
       </c>
       <c r="P10" t="inlineStr"/>
-      <c r="Q10" t="inlineStr"/>
+      <c r="Q10" t="inlineStr">
+        <is>
+          <t>Superhost</t>
+        </is>
+      </c>
       <c r="R10" t="inlineStr"/>
       <c r="S10" t="inlineStr">
         <is>
-          <t>R$ 189.17</t>
+          <t>R$ 239.19</t>
         </is>
       </c>
       <c r="T10" t="inlineStr"/>
       <c r="U10" t="inlineStr">
         <is>
-          <t>27/04/2023 15:00:13</t>
+          <t>27/04/2023 15:23:27</t>
         </is>
       </c>
     </row>
@@ -1025,7 +1029,7 @@
       <c r="C11" t="inlineStr"/>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Aluguel por temporada com piscina privativa</t>
+          <t>Loft completo para temporada</t>
         </is>
       </c>
       <c r="E11" t="inlineStr"/>
@@ -1034,13 +1038,13 @@
       <c r="H11" t="inlineStr"/>
       <c r="I11" t="inlineStr">
         <is>
-          <t>3 camas</t>
+          <t>2 camas</t>
         </is>
       </c>
       <c r="J11" t="inlineStr"/>
       <c r="K11" t="inlineStr">
         <is>
-          <t>R$315 por noite</t>
+          <t>R$296 por noite</t>
         </is>
       </c>
       <c r="L11" t="inlineStr"/>
@@ -1048,39 +1052,35 @@
       <c r="N11" t="inlineStr"/>
       <c r="O11" t="inlineStr">
         <is>
-          <t>4,97 (67)</t>
+          <t>4,92 (25)</t>
         </is>
       </c>
       <c r="P11" t="inlineStr"/>
-      <c r="Q11" t="inlineStr">
-        <is>
-          <t>Superhost</t>
-        </is>
-      </c>
+      <c r="Q11" t="inlineStr"/>
       <c r="R11" t="inlineStr"/>
       <c r="S11" t="inlineStr">
         <is>
-          <t>R$ 189.17</t>
+          <t>R$ 239.19</t>
         </is>
       </c>
       <c r="T11" t="inlineStr"/>
       <c r="U11" t="inlineStr">
         <is>
-          <t>27/04/2023 15:00:13</t>
+          <t>27/04/2023 15:23:27</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Apartamento em Araruama</t>
+          <t>Casa em Araruama</t>
         </is>
       </c>
       <c r="B12" t="inlineStr"/>
       <c r="C12" t="inlineStr"/>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Apto na Região dos lagos. Aconchegante e central.</t>
+          <t>Aluguel por temporada com piscina privativa</t>
         </is>
       </c>
       <c r="E12" t="inlineStr"/>
@@ -1089,13 +1089,13 @@
       <c r="H12" t="inlineStr"/>
       <c r="I12" t="inlineStr">
         <is>
-          <t>2 camas</t>
+          <t>3 camas</t>
         </is>
       </c>
       <c r="J12" t="inlineStr"/>
       <c r="K12" t="inlineStr">
         <is>
-          <t>R$140 por noite</t>
+          <t>R$315 por noite</t>
         </is>
       </c>
       <c r="L12" t="inlineStr"/>
@@ -1103,35 +1103,39 @@
       <c r="N12" t="inlineStr"/>
       <c r="O12" t="inlineStr">
         <is>
-          <t>4,71 (7)</t>
+          <t>4,97 (67)</t>
         </is>
       </c>
       <c r="P12" t="inlineStr"/>
-      <c r="Q12" t="inlineStr"/>
+      <c r="Q12" t="inlineStr">
+        <is>
+          <t>Superhost</t>
+        </is>
+      </c>
       <c r="R12" t="inlineStr"/>
       <c r="S12" t="inlineStr">
         <is>
-          <t>R$ 189.17</t>
+          <t>R$ 239.19</t>
         </is>
       </c>
       <c r="T12" t="inlineStr"/>
       <c r="U12" t="inlineStr">
         <is>
-          <t>27/04/2023 15:00:13</t>
+          <t>27/04/2023 15:23:27</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Chalé em Coqueiral</t>
+          <t>Apartamento em Araruama</t>
         </is>
       </c>
       <c r="B13" t="inlineStr"/>
       <c r="C13" t="inlineStr"/>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Chalé Recantinho da Lagoa, Araruama,Rj</t>
+          <t>Apto na Região dos lagos. Aconchegante e central.</t>
         </is>
       </c>
       <c r="E13" t="inlineStr"/>
@@ -1140,13 +1144,13 @@
       <c r="H13" t="inlineStr"/>
       <c r="I13" t="inlineStr">
         <is>
-          <t>3 camas</t>
+          <t>2 camas</t>
         </is>
       </c>
       <c r="J13" t="inlineStr"/>
       <c r="K13" t="inlineStr">
         <is>
-          <t>R$91 por noite</t>
+          <t>R$140 por noite</t>
         </is>
       </c>
       <c r="L13" t="inlineStr"/>
@@ -1154,7 +1158,7 @@
       <c r="N13" t="inlineStr"/>
       <c r="O13" t="inlineStr">
         <is>
-          <t>4,84 (75)</t>
+          <t>4,71 (7)</t>
         </is>
       </c>
       <c r="P13" t="inlineStr"/>
@@ -1162,27 +1166,27 @@
       <c r="R13" t="inlineStr"/>
       <c r="S13" t="inlineStr">
         <is>
-          <t>R$ 189.17</t>
+          <t>R$ 239.19</t>
         </is>
       </c>
       <c r="T13" t="inlineStr"/>
       <c r="U13" t="inlineStr">
         <is>
-          <t>27/04/2023 15:00:13</t>
+          <t>27/04/2023 15:23:27</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Casa em Parque Hotel</t>
+          <t>Casa de campo em Praia Seca</t>
         </is>
       </c>
       <c r="B14" t="inlineStr"/>
       <c r="C14" t="inlineStr"/>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Curta o melhor de Araruama e Região dos Lagos</t>
+          <t>Casa Maravilhosa com Lagoa privativa</t>
         </is>
       </c>
       <c r="E14" t="inlineStr"/>
@@ -1191,13 +1195,13 @@
       <c r="H14" t="inlineStr"/>
       <c r="I14" t="inlineStr">
         <is>
-          <t>4 camas</t>
+          <t>3 camas de casal</t>
         </is>
       </c>
       <c r="J14" t="inlineStr"/>
       <c r="K14" t="inlineStr">
         <is>
-          <t>R$133 por noite</t>
+          <t>R$117 por noite</t>
         </is>
       </c>
       <c r="L14" t="inlineStr"/>
@@ -1205,25 +1209,21 @@
       <c r="N14" t="inlineStr"/>
       <c r="O14" t="inlineStr">
         <is>
-          <t>4,9 (29)</t>
+          <t>4,77 (22)</t>
         </is>
       </c>
       <c r="P14" t="inlineStr"/>
-      <c r="Q14" t="inlineStr">
-        <is>
-          <t>Superhost</t>
-        </is>
-      </c>
+      <c r="Q14" t="inlineStr"/>
       <c r="R14" t="inlineStr"/>
       <c r="S14" t="inlineStr">
         <is>
-          <t>R$ 189.17</t>
+          <t>R$ 239.19</t>
         </is>
       </c>
       <c r="T14" t="inlineStr"/>
       <c r="U14" t="inlineStr">
         <is>
-          <t>27/04/2023 15:00:13</t>
+          <t>27/04/2023 15:23:27</t>
         </is>
       </c>
     </row>
@@ -1268,27 +1268,27 @@
       <c r="R15" t="inlineStr"/>
       <c r="S15" t="inlineStr">
         <is>
-          <t>R$ 189.17</t>
+          <t>R$ 239.19</t>
         </is>
       </c>
       <c r="T15" t="inlineStr"/>
       <c r="U15" t="inlineStr">
         <is>
-          <t>27/04/2023 15:00:13</t>
+          <t>27/04/2023 15:23:27</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Casa em Araruama</t>
+          <t>Casa de hóspedes em Pontinha</t>
         </is>
       </c>
       <c r="B16" t="inlineStr"/>
       <c r="C16" t="inlineStr"/>
       <c r="D16" t="inlineStr">
         <is>
-          <t>loft &lt;SPA&lt; onde você descansa relaxa e se renova</t>
+          <t>Casa do Alto da Pontinha</t>
         </is>
       </c>
       <c r="E16" t="inlineStr"/>
@@ -1303,7 +1303,7 @@
       <c r="J16" t="inlineStr"/>
       <c r="K16" t="inlineStr">
         <is>
-          <t>R$189 por noite, originalmente R$302</t>
+          <t>R$72 por noite</t>
         </is>
       </c>
       <c r="L16" t="inlineStr"/>
@@ -1311,7 +1311,7 @@
       <c r="N16" t="inlineStr"/>
       <c r="O16" t="inlineStr">
         <is>
-          <t>5,0 (9)</t>
+          <t>4,83 (18)</t>
         </is>
       </c>
       <c r="P16" t="inlineStr"/>
@@ -1323,29 +1323,27 @@
       <c r="R16" t="inlineStr"/>
       <c r="S16" t="inlineStr">
         <is>
-          <t>R$ 189.17</t>
+          <t>R$ 239.19</t>
         </is>
       </c>
       <c r="T16" t="inlineStr"/>
       <c r="U16" t="inlineStr">
         <is>
-          <t>27/04/2023 15:00:13</t>
+          <t>27/04/2023 15:23:27</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Apartamento em Araruama</t>
+          <t>Casa de campo em Outeiro</t>
         </is>
       </c>
       <c r="B17" t="inlineStr"/>
       <c r="C17" t="inlineStr"/>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Kitinete em Araruama/RJ!
-Centro!
-Perto da Praia!</t>
+          <t>Casa com piscina no Condomínio Sonho de Vida</t>
         </is>
       </c>
       <c r="E17" t="inlineStr"/>
@@ -1354,13 +1352,13 @@
       <c r="H17" t="inlineStr"/>
       <c r="I17" t="inlineStr">
         <is>
-          <t>2 camas</t>
+          <t>4 camas</t>
         </is>
       </c>
       <c r="J17" t="inlineStr"/>
       <c r="K17" t="inlineStr">
         <is>
-          <t>R$198 por noite</t>
+          <t>R$290 por noite, originalmente R$352</t>
         </is>
       </c>
       <c r="L17" t="inlineStr"/>
@@ -1368,35 +1366,41 @@
       <c r="N17" t="inlineStr"/>
       <c r="O17" t="inlineStr">
         <is>
-          <t>4,8 (10)</t>
+          <t>5,0 (22)</t>
         </is>
       </c>
       <c r="P17" t="inlineStr"/>
-      <c r="Q17" t="inlineStr"/>
+      <c r="Q17" t="inlineStr">
+        <is>
+          <t>Superhost</t>
+        </is>
+      </c>
       <c r="R17" t="inlineStr"/>
       <c r="S17" t="inlineStr">
         <is>
-          <t>R$ 189.17</t>
+          <t>R$ 239.19</t>
         </is>
       </c>
       <c r="T17" t="inlineStr"/>
       <c r="U17" t="inlineStr">
         <is>
-          <t>27/04/2023 15:00:13</t>
+          <t>27/04/2023 15:23:27</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Casa de campo em Outeiro</t>
+          <t>Apartamento em Araruama</t>
         </is>
       </c>
       <c r="B18" t="inlineStr"/>
       <c r="C18" t="inlineStr"/>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Casa com piscina no Condomínio Sonho de Vida</t>
+          <t>Kitinete em Araruama/RJ!
+Centro!
+Perto da Praia!</t>
         </is>
       </c>
       <c r="E18" t="inlineStr"/>
@@ -1405,13 +1409,13 @@
       <c r="H18" t="inlineStr"/>
       <c r="I18" t="inlineStr">
         <is>
-          <t>4 camas</t>
+          <t>2 camas</t>
         </is>
       </c>
       <c r="J18" t="inlineStr"/>
       <c r="K18" t="inlineStr">
         <is>
-          <t>R$290 por noite, originalmente R$352</t>
+          <t>R$198 por noite</t>
         </is>
       </c>
       <c r="L18" t="inlineStr"/>
@@ -1419,39 +1423,35 @@
       <c r="N18" t="inlineStr"/>
       <c r="O18" t="inlineStr">
         <is>
-          <t>5,0 (22)</t>
+          <t>4,8 (10)</t>
         </is>
       </c>
       <c r="P18" t="inlineStr"/>
-      <c r="Q18" t="inlineStr">
-        <is>
-          <t>Superhost</t>
-        </is>
-      </c>
+      <c r="Q18" t="inlineStr"/>
       <c r="R18" t="inlineStr"/>
       <c r="S18" t="inlineStr">
         <is>
-          <t>R$ 189.17</t>
+          <t>R$ 239.19</t>
         </is>
       </c>
       <c r="T18" t="inlineStr"/>
       <c r="U18" t="inlineStr">
         <is>
-          <t>27/04/2023 15:00:13</t>
+          <t>27/04/2023 15:23:27</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Casa de campo em Araruama</t>
+          <t>Apartamento em Parque Hotel</t>
         </is>
       </c>
       <c r="B19" t="inlineStr"/>
       <c r="C19" t="inlineStr"/>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Casa de Praia agradável com piscina em Praia Seca</t>
+          <t>Apartamento na Lagoa de Araruama</t>
         </is>
       </c>
       <c r="E19" t="inlineStr"/>
@@ -1460,13 +1460,13 @@
       <c r="H19" t="inlineStr"/>
       <c r="I19" t="inlineStr">
         <is>
-          <t>5 camas</t>
+          <t>3 camas</t>
         </is>
       </c>
       <c r="J19" t="inlineStr"/>
       <c r="K19" t="inlineStr">
         <is>
-          <t>R$257 por noite, originalmente R$326</t>
+          <t>R$208 por noite</t>
         </is>
       </c>
       <c r="L19" t="inlineStr"/>
@@ -1474,21 +1474,25 @@
       <c r="N19" t="inlineStr"/>
       <c r="O19" t="inlineStr">
         <is>
-          <t>5,0 (9)</t>
+          <t>4,94 (17)</t>
         </is>
       </c>
       <c r="P19" t="inlineStr"/>
-      <c r="Q19" t="inlineStr"/>
+      <c r="Q19" t="inlineStr">
+        <is>
+          <t>Superhost</t>
+        </is>
+      </c>
       <c r="R19" t="inlineStr"/>
       <c r="S19" t="inlineStr">
         <is>
-          <t>R$ 189.17</t>
+          <t>R$ 239.19</t>
         </is>
       </c>
       <c r="T19" t="inlineStr"/>
       <c r="U19" t="inlineStr">
         <is>
-          <t>27/04/2023 15:00:13</t>
+          <t>27/04/2023 15:23:27</t>
         </is>
       </c>
     </row>
@@ -1537,13 +1541,13 @@
       <c r="R20" t="inlineStr"/>
       <c r="S20" t="inlineStr">
         <is>
-          <t>R$ 189.17</t>
+          <t>R$ 239.19</t>
         </is>
       </c>
       <c r="T20" t="inlineStr"/>
       <c r="U20" t="inlineStr">
         <is>
-          <t>27/04/2023 15:00:13</t>
+          <t>27/04/2023 15:23:27</t>
         </is>
       </c>
     </row>
@@ -1592,13 +1596,13 @@
       <c r="R21" t="inlineStr"/>
       <c r="S21" t="inlineStr">
         <is>
-          <t>R$ 189.17</t>
+          <t>R$ 239.19</t>
         </is>
       </c>
       <c r="T21" t="inlineStr"/>
       <c r="U21" t="inlineStr">
         <is>
-          <t>27/04/2023 15:00:13</t>
+          <t>27/04/2023 15:23:27</t>
         </is>
       </c>
     </row>
@@ -1643,13 +1647,13 @@
       <c r="R22" t="inlineStr"/>
       <c r="S22" t="inlineStr">
         <is>
-          <t>R$ 189.17</t>
+          <t>R$ 239.19</t>
         </is>
       </c>
       <c r="T22" t="inlineStr"/>
       <c r="U22" t="inlineStr">
         <is>
-          <t>27/04/2023 15:00:13</t>
+          <t>27/04/2023 15:23:27</t>
         </is>
       </c>
     </row>
@@ -1694,13 +1698,13 @@
       <c r="R23" t="inlineStr"/>
       <c r="S23" t="inlineStr">
         <is>
-          <t>R$ 189.17</t>
+          <t>R$ 239.19</t>
         </is>
       </c>
       <c r="T23" t="inlineStr"/>
       <c r="U23" t="inlineStr">
         <is>
-          <t>27/04/2023 15:00:13</t>
+          <t>27/04/2023 15:23:27</t>
         </is>
       </c>
     </row>
@@ -1749,13 +1753,13 @@
       <c r="R24" t="inlineStr"/>
       <c r="S24" t="inlineStr">
         <is>
-          <t>R$ 189.17</t>
+          <t>R$ 239.19</t>
         </is>
       </c>
       <c r="T24" t="inlineStr"/>
       <c r="U24" t="inlineStr">
         <is>
-          <t>27/04/2023 15:00:13</t>
+          <t>27/04/2023 15:23:27</t>
         </is>
       </c>
     </row>
@@ -1804,13 +1808,13 @@
       <c r="R25" t="inlineStr"/>
       <c r="S25" t="inlineStr">
         <is>
-          <t>R$ 189.17</t>
+          <t>R$ 239.19</t>
         </is>
       </c>
       <c r="T25" t="inlineStr"/>
       <c r="U25" t="inlineStr">
         <is>
-          <t>27/04/2023 15:00:13</t>
+          <t>27/04/2023 15:23:27</t>
         </is>
       </c>
     </row>
@@ -1855,13 +1859,13 @@
       <c r="R26" t="inlineStr"/>
       <c r="S26" t="inlineStr">
         <is>
-          <t>R$ 189.17</t>
+          <t>R$ 239.19</t>
         </is>
       </c>
       <c r="T26" t="inlineStr"/>
       <c r="U26" t="inlineStr">
         <is>
-          <t>27/04/2023 15:00:13</t>
+          <t>27/04/2023 15:23:27</t>
         </is>
       </c>
     </row>
@@ -1910,13 +1914,13 @@
       <c r="R27" t="inlineStr"/>
       <c r="S27" t="inlineStr">
         <is>
-          <t>R$ 189.17</t>
+          <t>R$ 239.19</t>
         </is>
       </c>
       <c r="T27" t="inlineStr"/>
       <c r="U27" t="inlineStr">
         <is>
-          <t>27/04/2023 15:00:13</t>
+          <t>27/04/2023 15:23:27</t>
         </is>
       </c>
     </row>
@@ -1965,13 +1969,13 @@
       <c r="R28" t="inlineStr"/>
       <c r="S28" t="inlineStr">
         <is>
-          <t>R$ 189.17</t>
+          <t>R$ 239.19</t>
         </is>
       </c>
       <c r="T28" t="inlineStr"/>
       <c r="U28" t="inlineStr">
         <is>
-          <t>27/04/2023 15:00:13</t>
+          <t>27/04/2023 15:23:27</t>
         </is>
       </c>
     </row>
@@ -2021,13 +2025,13 @@
       <c r="R29" t="inlineStr"/>
       <c r="S29" t="inlineStr">
         <is>
-          <t>R$ 189.17</t>
+          <t>R$ 239.19</t>
         </is>
       </c>
       <c r="T29" t="inlineStr"/>
       <c r="U29" t="inlineStr">
         <is>
-          <t>27/04/2023 15:00:13</t>
+          <t>27/04/2023 15:23:27</t>
         </is>
       </c>
     </row>
@@ -2076,13 +2080,13 @@
       <c r="R30" t="inlineStr"/>
       <c r="S30" t="inlineStr">
         <is>
-          <t>R$ 189.17</t>
+          <t>R$ 239.19</t>
         </is>
       </c>
       <c r="T30" t="inlineStr"/>
       <c r="U30" t="inlineStr">
         <is>
-          <t>27/04/2023 15:00:13</t>
+          <t>27/04/2023 15:23:27</t>
         </is>
       </c>
     </row>
@@ -2131,13 +2135,13 @@
       <c r="R31" t="inlineStr"/>
       <c r="S31" t="inlineStr">
         <is>
-          <t>R$ 189.17</t>
+          <t>R$ 239.19</t>
         </is>
       </c>
       <c r="T31" t="inlineStr"/>
       <c r="U31" t="inlineStr">
         <is>
-          <t>27/04/2023 15:00:13</t>
+          <t>27/04/2023 15:23:27</t>
         </is>
       </c>
     </row>
@@ -2182,13 +2186,13 @@
       <c r="R32" t="inlineStr"/>
       <c r="S32" t="inlineStr">
         <is>
-          <t>R$ 189.17</t>
+          <t>R$ 239.19</t>
         </is>
       </c>
       <c r="T32" t="inlineStr"/>
       <c r="U32" t="inlineStr">
         <is>
-          <t>27/04/2023 15:00:13</t>
+          <t>27/04/2023 15:23:27</t>
         </is>
       </c>
     </row>
@@ -2233,13 +2237,13 @@
       <c r="R33" t="inlineStr"/>
       <c r="S33" t="inlineStr">
         <is>
-          <t>R$ 189.17</t>
+          <t>R$ 239.19</t>
         </is>
       </c>
       <c r="T33" t="inlineStr"/>
       <c r="U33" t="inlineStr">
         <is>
-          <t>27/04/2023 15:00:13</t>
+          <t>27/04/2023 15:23:27</t>
         </is>
       </c>
     </row>
@@ -2288,13 +2292,13 @@
       <c r="R34" t="inlineStr"/>
       <c r="S34" t="inlineStr">
         <is>
-          <t>R$ 189.17</t>
+          <t>R$ 239.19</t>
         </is>
       </c>
       <c r="T34" t="inlineStr"/>
       <c r="U34" t="inlineStr">
         <is>
-          <t>27/04/2023 15:00:13</t>
+          <t>27/04/2023 15:23:27</t>
         </is>
       </c>
     </row>
@@ -2343,13 +2347,13 @@
       <c r="R35" t="inlineStr"/>
       <c r="S35" t="inlineStr">
         <is>
-          <t>R$ 189.17</t>
+          <t>R$ 239.19</t>
         </is>
       </c>
       <c r="T35" t="inlineStr"/>
       <c r="U35" t="inlineStr">
         <is>
-          <t>27/04/2023 15:00:13</t>
+          <t>27/04/2023 15:23:27</t>
         </is>
       </c>
     </row>
@@ -2394,13 +2398,13 @@
       <c r="R36" t="inlineStr"/>
       <c r="S36" t="inlineStr">
         <is>
-          <t>R$ 189.17</t>
+          <t>R$ 239.19</t>
         </is>
       </c>
       <c r="T36" t="inlineStr"/>
       <c r="U36" t="inlineStr">
         <is>
-          <t>27/04/2023 15:00:13</t>
+          <t>27/04/2023 15:23:27</t>
         </is>
       </c>
     </row>
@@ -2445,13 +2449,2856 @@
       <c r="R37" t="inlineStr"/>
       <c r="S37" t="inlineStr">
         <is>
-          <t>R$ 189.17</t>
+          <t>R$ 239.19</t>
         </is>
       </c>
       <c r="T37" t="inlineStr"/>
       <c r="U37" t="inlineStr">
         <is>
-          <t>27/04/2023 15:00:13</t>
+          <t>27/04/2023 15:23:27</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>Apartamento em Araruama</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr"/>
+      <c r="C38" t="inlineStr"/>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>apartamento super confortável</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr"/>
+      <c r="F38" t="inlineStr"/>
+      <c r="G38" t="inlineStr"/>
+      <c r="H38" t="inlineStr"/>
+      <c r="I38" t="inlineStr">
+        <is>
+          <t>2 camas</t>
+        </is>
+      </c>
+      <c r="J38" t="inlineStr"/>
+      <c r="K38" t="inlineStr">
+        <is>
+          <t>R$175 por noite, originalmente R$214</t>
+        </is>
+      </c>
+      <c r="L38" t="inlineStr"/>
+      <c r="M38" t="inlineStr"/>
+      <c r="N38" t="inlineStr"/>
+      <c r="O38" t="inlineStr">
+        <is>
+          <t>Novo</t>
+        </is>
+      </c>
+      <c r="P38" t="inlineStr"/>
+      <c r="Q38" t="inlineStr"/>
+      <c r="R38" t="inlineStr"/>
+      <c r="S38" t="inlineStr">
+        <is>
+          <t>R$ 239.19</t>
+        </is>
+      </c>
+      <c r="T38" t="inlineStr"/>
+      <c r="U38" t="inlineStr">
+        <is>
+          <t>27/04/2023 15:23:27</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>Casa em Araruama</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr"/>
+      <c r="C39" t="inlineStr"/>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>loft Peniel lugar tranquilo</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr"/>
+      <c r="F39" t="inlineStr"/>
+      <c r="G39" t="inlineStr"/>
+      <c r="H39" t="inlineStr"/>
+      <c r="I39" t="inlineStr">
+        <is>
+          <t>2 camas</t>
+        </is>
+      </c>
+      <c r="J39" t="inlineStr"/>
+      <c r="K39" t="inlineStr">
+        <is>
+          <t>R$217 por noite</t>
+        </is>
+      </c>
+      <c r="L39" t="inlineStr"/>
+      <c r="M39" t="inlineStr"/>
+      <c r="N39" t="inlineStr"/>
+      <c r="O39" t="inlineStr">
+        <is>
+          <t>4,89 (9)</t>
+        </is>
+      </c>
+      <c r="P39" t="inlineStr"/>
+      <c r="Q39" t="inlineStr">
+        <is>
+          <t>Superhost</t>
+        </is>
+      </c>
+      <c r="R39" t="inlineStr"/>
+      <c r="S39" t="inlineStr">
+        <is>
+          <t>R$ 239.19</t>
+        </is>
+      </c>
+      <c r="T39" t="inlineStr"/>
+      <c r="U39" t="inlineStr">
+        <is>
+          <t>27/04/2023 15:23:27</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>Casa em Araruama</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr"/>
+      <c r="C40" t="inlineStr"/>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>Excelente casa na orla da lagoa em Praia Seca/RJ</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr"/>
+      <c r="F40" t="inlineStr"/>
+      <c r="G40" t="inlineStr"/>
+      <c r="H40" t="inlineStr"/>
+      <c r="I40" t="inlineStr">
+        <is>
+          <t>5 camas</t>
+        </is>
+      </c>
+      <c r="J40" t="inlineStr"/>
+      <c r="K40" t="inlineStr">
+        <is>
+          <t>R$258 por noite</t>
+        </is>
+      </c>
+      <c r="L40" t="inlineStr"/>
+      <c r="M40" t="inlineStr"/>
+      <c r="N40" t="inlineStr"/>
+      <c r="O40" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="P40" t="inlineStr"/>
+      <c r="Q40" t="inlineStr"/>
+      <c r="R40" t="inlineStr"/>
+      <c r="S40" t="inlineStr">
+        <is>
+          <t>R$ 239.19</t>
+        </is>
+      </c>
+      <c r="T40" t="inlineStr"/>
+      <c r="U40" t="inlineStr">
+        <is>
+          <t>27/04/2023 15:23:27</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>Casa em Araruama</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr"/>
+      <c r="C41" t="inlineStr"/>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>Casa aconchegante !</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr"/>
+      <c r="F41" t="inlineStr"/>
+      <c r="G41" t="inlineStr"/>
+      <c r="H41" t="inlineStr"/>
+      <c r="I41" t="inlineStr">
+        <is>
+          <t>6 camas</t>
+        </is>
+      </c>
+      <c r="J41" t="inlineStr"/>
+      <c r="K41" t="inlineStr">
+        <is>
+          <t>R$151 por noite, originalmente R$184</t>
+        </is>
+      </c>
+      <c r="L41" t="inlineStr"/>
+      <c r="M41" t="inlineStr"/>
+      <c r="N41" t="inlineStr"/>
+      <c r="O41" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="P41" t="inlineStr"/>
+      <c r="Q41" t="inlineStr"/>
+      <c r="R41" t="inlineStr"/>
+      <c r="S41" t="inlineStr">
+        <is>
+          <t>R$ 239.19</t>
+        </is>
+      </c>
+      <c r="T41" t="inlineStr"/>
+      <c r="U41" t="inlineStr">
+        <is>
+          <t>27/04/2023 15:23:27</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>Casa em Araruama</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr"/>
+      <c r="C42" t="inlineStr"/>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>Refúgio na laguna</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr"/>
+      <c r="F42" t="inlineStr"/>
+      <c r="G42" t="inlineStr"/>
+      <c r="H42" t="inlineStr"/>
+      <c r="I42" t="inlineStr">
+        <is>
+          <t>4 camas</t>
+        </is>
+      </c>
+      <c r="J42" t="inlineStr"/>
+      <c r="K42" t="inlineStr">
+        <is>
+          <t>R$283 por noite</t>
+        </is>
+      </c>
+      <c r="L42" t="inlineStr"/>
+      <c r="M42" t="inlineStr"/>
+      <c r="N42" t="inlineStr"/>
+      <c r="O42" t="inlineStr">
+        <is>
+          <t>4,95 (20)</t>
+        </is>
+      </c>
+      <c r="P42" t="inlineStr"/>
+      <c r="Q42" t="inlineStr">
+        <is>
+          <t>Superhost</t>
+        </is>
+      </c>
+      <c r="R42" t="inlineStr"/>
+      <c r="S42" t="inlineStr">
+        <is>
+          <t>R$ 239.19</t>
+        </is>
+      </c>
+      <c r="T42" t="inlineStr"/>
+      <c r="U42" t="inlineStr">
+        <is>
+          <t>27/04/2023 15:23:27</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>Casa de veraneio em Araruama</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr"/>
+      <c r="C43" t="inlineStr"/>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>Praia Seca Araruama Rj</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr"/>
+      <c r="F43" t="inlineStr"/>
+      <c r="G43" t="inlineStr"/>
+      <c r="H43" t="inlineStr"/>
+      <c r="I43" t="inlineStr">
+        <is>
+          <t>4 camas</t>
+        </is>
+      </c>
+      <c r="J43" t="inlineStr"/>
+      <c r="K43" t="inlineStr">
+        <is>
+          <t>R$371 por noite</t>
+        </is>
+      </c>
+      <c r="L43" t="inlineStr"/>
+      <c r="M43" t="inlineStr"/>
+      <c r="N43" t="inlineStr"/>
+      <c r="O43" t="inlineStr">
+        <is>
+          <t>5,0 (4)</t>
+        </is>
+      </c>
+      <c r="P43" t="inlineStr"/>
+      <c r="Q43" t="inlineStr"/>
+      <c r="R43" t="inlineStr"/>
+      <c r="S43" t="inlineStr">
+        <is>
+          <t>R$ 239.19</t>
+        </is>
+      </c>
+      <c r="T43" t="inlineStr"/>
+      <c r="U43" t="inlineStr">
+        <is>
+          <t>27/04/2023 15:23:27</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>Casa em Araruama</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr"/>
+      <c r="C44" t="inlineStr"/>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>Excelente Casa Cond. Ocean Park</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr"/>
+      <c r="F44" t="inlineStr"/>
+      <c r="G44" t="inlineStr"/>
+      <c r="H44" t="inlineStr"/>
+      <c r="I44" t="inlineStr">
+        <is>
+          <t>4 camas</t>
+        </is>
+      </c>
+      <c r="J44" t="inlineStr"/>
+      <c r="K44" t="inlineStr">
+        <is>
+          <t>R$178 por noite, originalmente R$217</t>
+        </is>
+      </c>
+      <c r="L44" t="inlineStr"/>
+      <c r="M44" t="inlineStr"/>
+      <c r="N44" t="inlineStr"/>
+      <c r="O44" t="inlineStr">
+        <is>
+          <t>Novo</t>
+        </is>
+      </c>
+      <c r="P44" t="inlineStr"/>
+      <c r="Q44" t="inlineStr"/>
+      <c r="R44" t="inlineStr"/>
+      <c r="S44" t="inlineStr">
+        <is>
+          <t>R$ 239.19</t>
+        </is>
+      </c>
+      <c r="T44" t="inlineStr"/>
+      <c r="U44" t="inlineStr">
+        <is>
+          <t>27/04/2023 15:23:27</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>Casa em Araruama</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr"/>
+      <c r="C45" t="inlineStr"/>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>#Hospedagem Nota 10 Araruama!</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr"/>
+      <c r="F45" t="inlineStr"/>
+      <c r="G45" t="inlineStr"/>
+      <c r="H45" t="inlineStr"/>
+      <c r="I45" t="inlineStr">
+        <is>
+          <t>6 camas</t>
+        </is>
+      </c>
+      <c r="J45" t="inlineStr"/>
+      <c r="K45" t="inlineStr">
+        <is>
+          <t>R$471 por noite</t>
+        </is>
+      </c>
+      <c r="L45" t="inlineStr"/>
+      <c r="M45" t="inlineStr"/>
+      <c r="N45" t="inlineStr"/>
+      <c r="O45" t="inlineStr">
+        <is>
+          <t>5,0 (7)</t>
+        </is>
+      </c>
+      <c r="P45" t="inlineStr"/>
+      <c r="Q45" t="inlineStr"/>
+      <c r="R45" t="inlineStr"/>
+      <c r="S45" t="inlineStr">
+        <is>
+          <t>R$ 239.19</t>
+        </is>
+      </c>
+      <c r="T45" t="inlineStr"/>
+      <c r="U45" t="inlineStr">
+        <is>
+          <t>27/04/2023 15:23:27</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>Casa em Ponte dos Leites</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr"/>
+      <c r="C46" t="inlineStr"/>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>Casa com piscina em condomínio e segurança 24hrs</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr"/>
+      <c r="F46" t="inlineStr"/>
+      <c r="G46" t="inlineStr"/>
+      <c r="H46" t="inlineStr"/>
+      <c r="I46" t="inlineStr">
+        <is>
+          <t>7 camas</t>
+        </is>
+      </c>
+      <c r="J46" t="inlineStr"/>
+      <c r="K46" t="inlineStr">
+        <is>
+          <t>R$257 por noite</t>
+        </is>
+      </c>
+      <c r="L46" t="inlineStr"/>
+      <c r="M46" t="inlineStr"/>
+      <c r="N46" t="inlineStr"/>
+      <c r="O46" t="inlineStr">
+        <is>
+          <t>4,88 (97)</t>
+        </is>
+      </c>
+      <c r="P46" t="inlineStr"/>
+      <c r="Q46" t="inlineStr"/>
+      <c r="R46" t="inlineStr"/>
+      <c r="S46" t="inlineStr">
+        <is>
+          <t>R$ 239.19</t>
+        </is>
+      </c>
+      <c r="T46" t="inlineStr"/>
+      <c r="U46" t="inlineStr">
+        <is>
+          <t>27/04/2023 15:23:27</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>Casa em Araruama</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr"/>
+      <c r="C47" t="inlineStr"/>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>Excelente Casa Cond. AlphaBeach</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr"/>
+      <c r="F47" t="inlineStr"/>
+      <c r="G47" t="inlineStr"/>
+      <c r="H47" t="inlineStr"/>
+      <c r="I47" t="inlineStr">
+        <is>
+          <t>5 camas</t>
+        </is>
+      </c>
+      <c r="J47" t="inlineStr"/>
+      <c r="K47" t="inlineStr">
+        <is>
+          <t>R$365 por noite</t>
+        </is>
+      </c>
+      <c r="L47" t="inlineStr"/>
+      <c r="M47" t="inlineStr"/>
+      <c r="N47" t="inlineStr"/>
+      <c r="O47" t="inlineStr">
+        <is>
+          <t>Novo</t>
+        </is>
+      </c>
+      <c r="P47" t="inlineStr"/>
+      <c r="Q47" t="inlineStr"/>
+      <c r="R47" t="inlineStr"/>
+      <c r="S47" t="inlineStr">
+        <is>
+          <t>R$ 239.19</t>
+        </is>
+      </c>
+      <c r="T47" t="inlineStr"/>
+      <c r="U47" t="inlineStr">
+        <is>
+          <t>27/04/2023 15:23:27</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>Casa em Salinas</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr"/>
+      <c r="C48" t="inlineStr"/>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>Casa em condomínio junto a lagoa, em Praia Seca</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr"/>
+      <c r="F48" t="inlineStr"/>
+      <c r="G48" t="inlineStr"/>
+      <c r="H48" t="inlineStr"/>
+      <c r="I48" t="inlineStr">
+        <is>
+          <t>4 camas</t>
+        </is>
+      </c>
+      <c r="J48" t="inlineStr"/>
+      <c r="K48" t="inlineStr">
+        <is>
+          <t>R$290 por noite</t>
+        </is>
+      </c>
+      <c r="L48" t="inlineStr"/>
+      <c r="M48" t="inlineStr"/>
+      <c r="N48" t="inlineStr"/>
+      <c r="O48" t="inlineStr">
+        <is>
+          <t>5,0 (24)</t>
+        </is>
+      </c>
+      <c r="P48" t="inlineStr"/>
+      <c r="Q48" t="inlineStr"/>
+      <c r="R48" t="inlineStr"/>
+      <c r="S48" t="inlineStr">
+        <is>
+          <t>R$ 239.19</t>
+        </is>
+      </c>
+      <c r="T48" t="inlineStr"/>
+      <c r="U48" t="inlineStr">
+        <is>
+          <t>27/04/2023 15:23:27</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>Casa em Araruama</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr"/>
+      <c r="C49" t="inlineStr"/>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>Ampla casa com quintal e garagem - Araruama/RJ</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr"/>
+      <c r="F49" t="inlineStr"/>
+      <c r="G49" t="inlineStr"/>
+      <c r="H49" t="inlineStr"/>
+      <c r="I49" t="inlineStr">
+        <is>
+          <t>2 camas</t>
+        </is>
+      </c>
+      <c r="J49" t="inlineStr"/>
+      <c r="K49" t="inlineStr">
+        <is>
+          <t>R$154 por noite</t>
+        </is>
+      </c>
+      <c r="L49" t="inlineStr"/>
+      <c r="M49" t="inlineStr"/>
+      <c r="N49" t="inlineStr"/>
+      <c r="O49" t="inlineStr">
+        <is>
+          <t>4,77 (65)</t>
+        </is>
+      </c>
+      <c r="P49" t="inlineStr"/>
+      <c r="Q49" t="inlineStr">
+        <is>
+          <t>Superhost</t>
+        </is>
+      </c>
+      <c r="R49" t="inlineStr"/>
+      <c r="S49" t="inlineStr">
+        <is>
+          <t>R$ 239.19</t>
+        </is>
+      </c>
+      <c r="T49" t="inlineStr"/>
+      <c r="U49" t="inlineStr">
+        <is>
+          <t>27/04/2023 15:23:27</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>Quarto privativo em Alto da Boa Vista</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr"/>
+      <c r="C50" t="inlineStr"/>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>Suíte em Araruama - Praça da bandeira</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr"/>
+      <c r="F50" t="inlineStr"/>
+      <c r="G50" t="inlineStr"/>
+      <c r="H50" t="inlineStr"/>
+      <c r="I50" t="inlineStr">
+        <is>
+          <t>1 cama de casal</t>
+        </is>
+      </c>
+      <c r="J50" t="inlineStr"/>
+      <c r="K50" t="inlineStr">
+        <is>
+          <t>R$115 por noite</t>
+        </is>
+      </c>
+      <c r="L50" t="inlineStr"/>
+      <c r="M50" t="inlineStr"/>
+      <c r="N50" t="inlineStr"/>
+      <c r="O50" t="inlineStr">
+        <is>
+          <t>4,63 (19)</t>
+        </is>
+      </c>
+      <c r="P50" t="inlineStr"/>
+      <c r="Q50" t="inlineStr"/>
+      <c r="R50" t="inlineStr"/>
+      <c r="S50" t="inlineStr">
+        <is>
+          <t>R$ 239.19</t>
+        </is>
+      </c>
+      <c r="T50" t="inlineStr"/>
+      <c r="U50" t="inlineStr">
+        <is>
+          <t>27/04/2023 15:23:27</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>Casa em Araruama</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr"/>
+      <c r="C51" t="inlineStr"/>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>Casa Pé na Areia Praia Seca</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr"/>
+      <c r="F51" t="inlineStr"/>
+      <c r="G51" t="inlineStr"/>
+      <c r="H51" t="inlineStr"/>
+      <c r="I51" t="inlineStr">
+        <is>
+          <t>5 camas</t>
+        </is>
+      </c>
+      <c r="J51" t="inlineStr"/>
+      <c r="K51" t="inlineStr">
+        <is>
+          <t>R$260 por noite, originalmente R$302</t>
+        </is>
+      </c>
+      <c r="L51" t="inlineStr"/>
+      <c r="M51" t="inlineStr"/>
+      <c r="N51" t="inlineStr"/>
+      <c r="O51" t="inlineStr">
+        <is>
+          <t>5,0 (3)</t>
+        </is>
+      </c>
+      <c r="P51" t="inlineStr"/>
+      <c r="Q51" t="inlineStr"/>
+      <c r="R51" t="inlineStr"/>
+      <c r="S51" t="inlineStr">
+        <is>
+          <t>R$ 239.19</t>
+        </is>
+      </c>
+      <c r="T51" t="inlineStr"/>
+      <c r="U51" t="inlineStr">
+        <is>
+          <t>27/04/2023 15:23:27</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>Quarto privativo em Alto da Boa Vista</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr"/>
+      <c r="C52" t="inlineStr"/>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>Lugar de Sossego e muita Natureza.</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr"/>
+      <c r="F52" t="inlineStr"/>
+      <c r="G52" t="inlineStr"/>
+      <c r="H52" t="inlineStr"/>
+      <c r="I52" t="inlineStr">
+        <is>
+          <t>1 cama de casal</t>
+        </is>
+      </c>
+      <c r="J52" t="inlineStr"/>
+      <c r="K52" t="inlineStr">
+        <is>
+          <t>R$184 por noite</t>
+        </is>
+      </c>
+      <c r="L52" t="inlineStr"/>
+      <c r="M52" t="inlineStr"/>
+      <c r="N52" t="inlineStr"/>
+      <c r="O52" t="inlineStr">
+        <is>
+          <t>4,94 (48)</t>
+        </is>
+      </c>
+      <c r="P52" t="inlineStr"/>
+      <c r="Q52" t="inlineStr">
+        <is>
+          <t>Superhost</t>
+        </is>
+      </c>
+      <c r="R52" t="inlineStr"/>
+      <c r="S52" t="inlineStr">
+        <is>
+          <t>R$ 239.19</t>
+        </is>
+      </c>
+      <c r="T52" t="inlineStr"/>
+      <c r="U52" t="inlineStr">
+        <is>
+          <t>27/04/2023 15:23:27</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>Quarto privativo em Araruama</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr"/>
+      <c r="C53" t="inlineStr"/>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>Acomodação suíte no centro de Praia Seca.</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr"/>
+      <c r="F53" t="inlineStr"/>
+      <c r="G53" t="inlineStr"/>
+      <c r="H53" t="inlineStr"/>
+      <c r="I53" t="inlineStr">
+        <is>
+          <t>1 cama</t>
+        </is>
+      </c>
+      <c r="J53" t="inlineStr"/>
+      <c r="K53" t="inlineStr">
+        <is>
+          <t>R$147 por noite</t>
+        </is>
+      </c>
+      <c r="L53" t="inlineStr"/>
+      <c r="M53" t="inlineStr"/>
+      <c r="N53" t="inlineStr"/>
+      <c r="O53" t="inlineStr">
+        <is>
+          <t>5,0 (9)</t>
+        </is>
+      </c>
+      <c r="P53" t="inlineStr"/>
+      <c r="Q53" t="inlineStr">
+        <is>
+          <t>Superhost</t>
+        </is>
+      </c>
+      <c r="R53" t="inlineStr"/>
+      <c r="S53" t="inlineStr">
+        <is>
+          <t>R$ 239.19</t>
+        </is>
+      </c>
+      <c r="T53" t="inlineStr"/>
+      <c r="U53" t="inlineStr">
+        <is>
+          <t>27/04/2023 15:23:27</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>Casa em Praia Linda</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr"/>
+      <c r="C54" t="inlineStr"/>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>Recanto dos Canários</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr"/>
+      <c r="F54" t="inlineStr"/>
+      <c r="G54" t="inlineStr"/>
+      <c r="H54" t="inlineStr"/>
+      <c r="I54" t="inlineStr">
+        <is>
+          <t>4 camas</t>
+        </is>
+      </c>
+      <c r="J54" t="inlineStr"/>
+      <c r="K54" t="inlineStr">
+        <is>
+          <t>R$87 por noite</t>
+        </is>
+      </c>
+      <c r="L54" t="inlineStr"/>
+      <c r="M54" t="inlineStr"/>
+      <c r="N54" t="inlineStr"/>
+      <c r="O54" t="inlineStr">
+        <is>
+          <t>4,95 (74)</t>
+        </is>
+      </c>
+      <c r="P54" t="inlineStr"/>
+      <c r="Q54" t="inlineStr">
+        <is>
+          <t>Superhost</t>
+        </is>
+      </c>
+      <c r="R54" t="inlineStr"/>
+      <c r="S54" t="inlineStr">
+        <is>
+          <t>R$ 239.19</t>
+        </is>
+      </c>
+      <c r="T54" t="inlineStr"/>
+      <c r="U54" t="inlineStr">
+        <is>
+          <t>27/04/2023 15:23:27</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>Casa em Atlantico</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr"/>
+      <c r="C55" t="inlineStr"/>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>Casa aconchegante, piscina. Praia Seca - Araruama.</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr"/>
+      <c r="F55" t="inlineStr"/>
+      <c r="G55" t="inlineStr"/>
+      <c r="H55" t="inlineStr"/>
+      <c r="I55" t="inlineStr">
+        <is>
+          <t>9 camas</t>
+        </is>
+      </c>
+      <c r="J55" t="inlineStr"/>
+      <c r="K55" t="inlineStr">
+        <is>
+          <t>R$291 por noite</t>
+        </is>
+      </c>
+      <c r="L55" t="inlineStr"/>
+      <c r="M55" t="inlineStr"/>
+      <c r="N55" t="inlineStr"/>
+      <c r="O55" t="inlineStr">
+        <is>
+          <t>5,0 (16)</t>
+        </is>
+      </c>
+      <c r="P55" t="inlineStr"/>
+      <c r="Q55" t="inlineStr">
+        <is>
+          <t>Superhost</t>
+        </is>
+      </c>
+      <c r="R55" t="inlineStr"/>
+      <c r="S55" t="inlineStr">
+        <is>
+          <t>R$ 239.19</t>
+        </is>
+      </c>
+      <c r="T55" t="inlineStr"/>
+      <c r="U55" t="inlineStr">
+        <is>
+          <t>27/04/2023 15:23:27</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>Casa em Araruama</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr"/>
+      <c r="C56" t="inlineStr"/>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>Casa em praia seca com piscina e um belo jardim</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr"/>
+      <c r="F56" t="inlineStr"/>
+      <c r="G56" t="inlineStr"/>
+      <c r="H56" t="inlineStr"/>
+      <c r="I56" t="inlineStr">
+        <is>
+          <t>13 camas</t>
+        </is>
+      </c>
+      <c r="J56" t="inlineStr"/>
+      <c r="K56" t="inlineStr">
+        <is>
+          <t>R$314 por noite</t>
+        </is>
+      </c>
+      <c r="L56" t="inlineStr"/>
+      <c r="M56" t="inlineStr"/>
+      <c r="N56" t="inlineStr"/>
+      <c r="O56" t="inlineStr">
+        <is>
+          <t>4,97 (38)</t>
+        </is>
+      </c>
+      <c r="P56" t="inlineStr"/>
+      <c r="Q56" t="inlineStr">
+        <is>
+          <t>Superhost</t>
+        </is>
+      </c>
+      <c r="R56" t="inlineStr"/>
+      <c r="S56" t="inlineStr">
+        <is>
+          <t>R$ 239.19</t>
+        </is>
+      </c>
+      <c r="T56" t="inlineStr"/>
+      <c r="U56" t="inlineStr">
+        <is>
+          <t>27/04/2023 15:23:27</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>Bangalô em Saquarema</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr"/>
+      <c r="C57" t="inlineStr"/>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>Bangalô com Piscina Privativa - @myweekend.brasil</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr"/>
+      <c r="F57" t="inlineStr"/>
+      <c r="G57" t="inlineStr"/>
+      <c r="H57" t="inlineStr"/>
+      <c r="I57" t="inlineStr">
+        <is>
+          <t>2 camas</t>
+        </is>
+      </c>
+      <c r="J57" t="inlineStr"/>
+      <c r="K57" t="inlineStr">
+        <is>
+          <t>R$1.123 por noite</t>
+        </is>
+      </c>
+      <c r="L57" t="inlineStr"/>
+      <c r="M57" t="inlineStr"/>
+      <c r="N57" t="inlineStr"/>
+      <c r="O57" t="inlineStr">
+        <is>
+          <t>5,0 (4)</t>
+        </is>
+      </c>
+      <c r="P57" t="inlineStr"/>
+      <c r="Q57" t="inlineStr"/>
+      <c r="R57" t="inlineStr"/>
+      <c r="S57" t="inlineStr">
+        <is>
+          <t>R$ 239.19</t>
+        </is>
+      </c>
+      <c r="T57" t="inlineStr"/>
+      <c r="U57" t="inlineStr">
+        <is>
+          <t>27/04/2023 15:23:27</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>Quarto privativo em Araruama</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr"/>
+      <c r="C58" t="inlineStr"/>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>Conjugado em Araruama</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr"/>
+      <c r="F58" t="inlineStr"/>
+      <c r="G58" t="inlineStr"/>
+      <c r="H58" t="inlineStr"/>
+      <c r="I58" t="inlineStr">
+        <is>
+          <t>1 cama</t>
+        </is>
+      </c>
+      <c r="J58" t="inlineStr"/>
+      <c r="K58" t="inlineStr">
+        <is>
+          <t>R$103 por noite</t>
+        </is>
+      </c>
+      <c r="L58" t="inlineStr"/>
+      <c r="M58" t="inlineStr"/>
+      <c r="N58" t="inlineStr"/>
+      <c r="O58" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="P58" t="inlineStr"/>
+      <c r="Q58" t="inlineStr"/>
+      <c r="R58" t="inlineStr"/>
+      <c r="S58" t="inlineStr">
+        <is>
+          <t>R$ 239.19</t>
+        </is>
+      </c>
+      <c r="T58" t="inlineStr"/>
+      <c r="U58" t="inlineStr">
+        <is>
+          <t>27/04/2023 15:23:27</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>Casa em Arraial do Cabo</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr"/>
+      <c r="C59" t="inlineStr"/>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>Casa la Duna</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr"/>
+      <c r="F59" t="inlineStr"/>
+      <c r="G59" t="inlineStr"/>
+      <c r="H59" t="inlineStr"/>
+      <c r="I59" t="inlineStr">
+        <is>
+          <t>4 camas</t>
+        </is>
+      </c>
+      <c r="J59" t="inlineStr"/>
+      <c r="K59" t="inlineStr">
+        <is>
+          <t>R$221 por noite</t>
+        </is>
+      </c>
+      <c r="L59" t="inlineStr"/>
+      <c r="M59" t="inlineStr"/>
+      <c r="N59" t="inlineStr"/>
+      <c r="O59" t="inlineStr">
+        <is>
+          <t>4,73 (40)</t>
+        </is>
+      </c>
+      <c r="P59" t="inlineStr"/>
+      <c r="Q59" t="inlineStr">
+        <is>
+          <t>Superhost</t>
+        </is>
+      </c>
+      <c r="R59" t="inlineStr"/>
+      <c r="S59" t="inlineStr">
+        <is>
+          <t>R$ 239.19</t>
+        </is>
+      </c>
+      <c r="T59" t="inlineStr"/>
+      <c r="U59" t="inlineStr">
+        <is>
+          <t>27/04/2023 15:23:27</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>Condomínio em Iguaba Grande</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr"/>
+      <c r="C60" t="inlineStr"/>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>Apto Lindo de Frente para Lagoa</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr"/>
+      <c r="F60" t="inlineStr"/>
+      <c r="G60" t="inlineStr"/>
+      <c r="H60" t="inlineStr"/>
+      <c r="I60" t="inlineStr">
+        <is>
+          <t>4 camas</t>
+        </is>
+      </c>
+      <c r="J60" t="inlineStr"/>
+      <c r="K60" t="inlineStr">
+        <is>
+          <t>R$103 por noite</t>
+        </is>
+      </c>
+      <c r="L60" t="inlineStr"/>
+      <c r="M60" t="inlineStr"/>
+      <c r="N60" t="inlineStr"/>
+      <c r="O60" t="inlineStr">
+        <is>
+          <t>4,8 (61)</t>
+        </is>
+      </c>
+      <c r="P60" t="inlineStr"/>
+      <c r="Q60" t="inlineStr"/>
+      <c r="R60" t="inlineStr"/>
+      <c r="S60" t="inlineStr">
+        <is>
+          <t>R$ 239.19</t>
+        </is>
+      </c>
+      <c r="T60" t="inlineStr"/>
+      <c r="U60" t="inlineStr">
+        <is>
+          <t>27/04/2023 15:23:27</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>Casa em Araruama</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr"/>
+      <c r="C61" t="inlineStr"/>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>Chalé de Madeira em condomínio fechado</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr"/>
+      <c r="F61" t="inlineStr"/>
+      <c r="G61" t="inlineStr"/>
+      <c r="H61" t="inlineStr"/>
+      <c r="I61" t="inlineStr">
+        <is>
+          <t>2 camas</t>
+        </is>
+      </c>
+      <c r="J61" t="inlineStr"/>
+      <c r="K61" t="inlineStr">
+        <is>
+          <t>R$139 por noite</t>
+        </is>
+      </c>
+      <c r="L61" t="inlineStr"/>
+      <c r="M61" t="inlineStr"/>
+      <c r="N61" t="inlineStr"/>
+      <c r="O61" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="P61" t="inlineStr"/>
+      <c r="Q61" t="inlineStr"/>
+      <c r="R61" t="inlineStr"/>
+      <c r="S61" t="inlineStr">
+        <is>
+          <t>R$ 239.19</t>
+        </is>
+      </c>
+      <c r="T61" t="inlineStr"/>
+      <c r="U61" t="inlineStr">
+        <is>
+          <t>27/04/2023 15:23:27</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>Casa em Centro</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr"/>
+      <c r="C62" t="inlineStr"/>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>Casa1. Centro Araruama,Wify, perto Rodoviá   Lagoa</t>
+        </is>
+      </c>
+      <c r="E62" t="inlineStr"/>
+      <c r="F62" t="inlineStr"/>
+      <c r="G62" t="inlineStr"/>
+      <c r="H62" t="inlineStr"/>
+      <c r="I62" t="inlineStr">
+        <is>
+          <t>4 camas</t>
+        </is>
+      </c>
+      <c r="J62" t="inlineStr"/>
+      <c r="K62" t="inlineStr">
+        <is>
+          <t>R$177 por noite</t>
+        </is>
+      </c>
+      <c r="L62" t="inlineStr"/>
+      <c r="M62" t="inlineStr"/>
+      <c r="N62" t="inlineStr"/>
+      <c r="O62" t="inlineStr">
+        <is>
+          <t>4,45 (11)</t>
+        </is>
+      </c>
+      <c r="P62" t="inlineStr"/>
+      <c r="Q62" t="inlineStr">
+        <is>
+          <t>Superhost</t>
+        </is>
+      </c>
+      <c r="R62" t="inlineStr"/>
+      <c r="S62" t="inlineStr">
+        <is>
+          <t>R$ 239.19</t>
+        </is>
+      </c>
+      <c r="T62" t="inlineStr"/>
+      <c r="U62" t="inlineStr">
+        <is>
+          <t>27/04/2023 15:23:27</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>Loft em Araruama</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr"/>
+      <c r="C63" t="inlineStr"/>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>Loft  Caeté</t>
+        </is>
+      </c>
+      <c r="E63" t="inlineStr"/>
+      <c r="F63" t="inlineStr"/>
+      <c r="G63" t="inlineStr"/>
+      <c r="H63" t="inlineStr"/>
+      <c r="I63" t="inlineStr">
+        <is>
+          <t>2 camas</t>
+        </is>
+      </c>
+      <c r="J63" t="inlineStr"/>
+      <c r="K63" t="inlineStr">
+        <is>
+          <t>R$320 por noite</t>
+        </is>
+      </c>
+      <c r="L63" t="inlineStr"/>
+      <c r="M63" t="inlineStr"/>
+      <c r="N63" t="inlineStr"/>
+      <c r="O63" t="inlineStr">
+        <is>
+          <t>4,89 (19)</t>
+        </is>
+      </c>
+      <c r="P63" t="inlineStr"/>
+      <c r="Q63" t="inlineStr"/>
+      <c r="R63" t="inlineStr"/>
+      <c r="S63" t="inlineStr">
+        <is>
+          <t>R$ 239.19</t>
+        </is>
+      </c>
+      <c r="T63" t="inlineStr"/>
+      <c r="U63" t="inlineStr">
+        <is>
+          <t>27/04/2023 15:23:27</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>Casa em Mutirão</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr"/>
+      <c r="C64" t="inlineStr"/>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>Casa com Piscina (16 pessoas) - Araruama, RJ</t>
+        </is>
+      </c>
+      <c r="E64" t="inlineStr"/>
+      <c r="F64" t="inlineStr"/>
+      <c r="G64" t="inlineStr"/>
+      <c r="H64" t="inlineStr"/>
+      <c r="I64" t="inlineStr">
+        <is>
+          <t>8 camas de casal</t>
+        </is>
+      </c>
+      <c r="J64" t="inlineStr"/>
+      <c r="K64" t="inlineStr">
+        <is>
+          <t>R$952 por noite</t>
+        </is>
+      </c>
+      <c r="L64" t="inlineStr"/>
+      <c r="M64" t="inlineStr"/>
+      <c r="N64" t="inlineStr"/>
+      <c r="O64" t="inlineStr">
+        <is>
+          <t>4,92 (24)</t>
+        </is>
+      </c>
+      <c r="P64" t="inlineStr"/>
+      <c r="Q64" t="inlineStr"/>
+      <c r="R64" t="inlineStr"/>
+      <c r="S64" t="inlineStr">
+        <is>
+          <t>R$ 239.19</t>
+        </is>
+      </c>
+      <c r="T64" t="inlineStr"/>
+      <c r="U64" t="inlineStr">
+        <is>
+          <t>27/04/2023 15:23:27</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>Casa em Parque Hotel</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr"/>
+      <c r="C65" t="inlineStr"/>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>Excelente casa Parque Hotel - Araruama</t>
+        </is>
+      </c>
+      <c r="E65" t="inlineStr"/>
+      <c r="F65" t="inlineStr"/>
+      <c r="G65" t="inlineStr"/>
+      <c r="H65" t="inlineStr"/>
+      <c r="I65" t="inlineStr">
+        <is>
+          <t>3 camas</t>
+        </is>
+      </c>
+      <c r="J65" t="inlineStr"/>
+      <c r="K65" t="inlineStr">
+        <is>
+          <t>R$138 por noite</t>
+        </is>
+      </c>
+      <c r="L65" t="inlineStr"/>
+      <c r="M65" t="inlineStr"/>
+      <c r="N65" t="inlineStr"/>
+      <c r="O65" t="inlineStr">
+        <is>
+          <t>5,0 (14)</t>
+        </is>
+      </c>
+      <c r="P65" t="inlineStr"/>
+      <c r="Q65" t="inlineStr"/>
+      <c r="R65" t="inlineStr"/>
+      <c r="S65" t="inlineStr">
+        <is>
+          <t>R$ 239.19</t>
+        </is>
+      </c>
+      <c r="T65" t="inlineStr"/>
+      <c r="U65" t="inlineStr">
+        <is>
+          <t>27/04/2023 15:23:27</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>Casa em Ponte dos Leites</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr"/>
+      <c r="C66" t="inlineStr"/>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>Casa com piscina em condomínio e segurança 24hrs</t>
+        </is>
+      </c>
+      <c r="E66" t="inlineStr"/>
+      <c r="F66" t="inlineStr"/>
+      <c r="G66" t="inlineStr"/>
+      <c r="H66" t="inlineStr"/>
+      <c r="I66" t="inlineStr">
+        <is>
+          <t>7 camas</t>
+        </is>
+      </c>
+      <c r="J66" t="inlineStr"/>
+      <c r="K66" t="inlineStr">
+        <is>
+          <t>R$257 por noite</t>
+        </is>
+      </c>
+      <c r="L66" t="inlineStr"/>
+      <c r="M66" t="inlineStr"/>
+      <c r="N66" t="inlineStr"/>
+      <c r="O66" t="inlineStr">
+        <is>
+          <t>4,88 (97)</t>
+        </is>
+      </c>
+      <c r="P66" t="inlineStr"/>
+      <c r="Q66" t="inlineStr"/>
+      <c r="R66" t="inlineStr"/>
+      <c r="S66" t="inlineStr">
+        <is>
+          <t>R$ 239.19</t>
+        </is>
+      </c>
+      <c r="T66" t="inlineStr"/>
+      <c r="U66" t="inlineStr">
+        <is>
+          <t>27/04/2023 15:23:27</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>Casa em Atlantico</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr"/>
+      <c r="C67" t="inlineStr"/>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>Casa aconchegante, piscina. Praia Seca - Araruama.</t>
+        </is>
+      </c>
+      <c r="E67" t="inlineStr"/>
+      <c r="F67" t="inlineStr"/>
+      <c r="G67" t="inlineStr"/>
+      <c r="H67" t="inlineStr"/>
+      <c r="I67" t="inlineStr">
+        <is>
+          <t>9 camas</t>
+        </is>
+      </c>
+      <c r="J67" t="inlineStr"/>
+      <c r="K67" t="inlineStr">
+        <is>
+          <t>R$291 por noite</t>
+        </is>
+      </c>
+      <c r="L67" t="inlineStr"/>
+      <c r="M67" t="inlineStr"/>
+      <c r="N67" t="inlineStr"/>
+      <c r="O67" t="inlineStr">
+        <is>
+          <t>5,0 (16)</t>
+        </is>
+      </c>
+      <c r="P67" t="inlineStr"/>
+      <c r="Q67" t="inlineStr">
+        <is>
+          <t>Superhost</t>
+        </is>
+      </c>
+      <c r="R67" t="inlineStr"/>
+      <c r="S67" t="inlineStr">
+        <is>
+          <t>R$ 239.19</t>
+        </is>
+      </c>
+      <c r="T67" t="inlineStr"/>
+      <c r="U67" t="inlineStr">
+        <is>
+          <t>27/04/2023 15:23:27</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>Apartamento em Parque Hotel</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr"/>
+      <c r="C68" t="inlineStr"/>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>Apto 2 quartos 5 min. Praia da Pontinha Araruama</t>
+        </is>
+      </c>
+      <c r="E68" t="inlineStr"/>
+      <c r="F68" t="inlineStr"/>
+      <c r="G68" t="inlineStr"/>
+      <c r="H68" t="inlineStr"/>
+      <c r="I68" t="inlineStr">
+        <is>
+          <t>2 camas de casal</t>
+        </is>
+      </c>
+      <c r="J68" t="inlineStr"/>
+      <c r="K68" t="inlineStr">
+        <is>
+          <t>R$243 por noite</t>
+        </is>
+      </c>
+      <c r="L68" t="inlineStr"/>
+      <c r="M68" t="inlineStr"/>
+      <c r="N68" t="inlineStr"/>
+      <c r="O68" t="inlineStr">
+        <is>
+          <t>4,67 (3)</t>
+        </is>
+      </c>
+      <c r="P68" t="inlineStr"/>
+      <c r="Q68" t="inlineStr"/>
+      <c r="R68" t="inlineStr"/>
+      <c r="S68" t="inlineStr">
+        <is>
+          <t>R$ 239.19</t>
+        </is>
+      </c>
+      <c r="T68" t="inlineStr"/>
+      <c r="U68" t="inlineStr">
+        <is>
+          <t>27/04/2023 15:23:27</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>Casa em Araruama</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr"/>
+      <c r="C69" t="inlineStr"/>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>Casa recanto Coqueiral</t>
+        </is>
+      </c>
+      <c r="E69" t="inlineStr"/>
+      <c r="F69" t="inlineStr"/>
+      <c r="G69" t="inlineStr"/>
+      <c r="H69" t="inlineStr"/>
+      <c r="I69" t="inlineStr">
+        <is>
+          <t>2 camas</t>
+        </is>
+      </c>
+      <c r="J69" t="inlineStr"/>
+      <c r="K69" t="inlineStr">
+        <is>
+          <t>R$356 por noite</t>
+        </is>
+      </c>
+      <c r="L69" t="inlineStr"/>
+      <c r="M69" t="inlineStr"/>
+      <c r="N69" t="inlineStr"/>
+      <c r="O69" t="inlineStr">
+        <is>
+          <t>Novo</t>
+        </is>
+      </c>
+      <c r="P69" t="inlineStr"/>
+      <c r="Q69" t="inlineStr"/>
+      <c r="R69" t="inlineStr"/>
+      <c r="S69" t="inlineStr">
+        <is>
+          <t>R$ 239.19</t>
+        </is>
+      </c>
+      <c r="T69" t="inlineStr"/>
+      <c r="U69" t="inlineStr">
+        <is>
+          <t>27/04/2023 15:23:27</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>Microcasa em Vilatur</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr"/>
+      <c r="C70" t="inlineStr"/>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>Villa cactus microcasa 2</t>
+        </is>
+      </c>
+      <c r="E70" t="inlineStr"/>
+      <c r="F70" t="inlineStr"/>
+      <c r="G70" t="inlineStr"/>
+      <c r="H70" t="inlineStr"/>
+      <c r="I70" t="inlineStr">
+        <is>
+          <t>2 camas</t>
+        </is>
+      </c>
+      <c r="J70" t="inlineStr"/>
+      <c r="K70" t="inlineStr">
+        <is>
+          <t>R$194 por noite</t>
+        </is>
+      </c>
+      <c r="L70" t="inlineStr"/>
+      <c r="M70" t="inlineStr"/>
+      <c r="N70" t="inlineStr"/>
+      <c r="O70" t="inlineStr">
+        <is>
+          <t>4,94 (49)</t>
+        </is>
+      </c>
+      <c r="P70" t="inlineStr"/>
+      <c r="Q70" t="inlineStr">
+        <is>
+          <t>Superhost</t>
+        </is>
+      </c>
+      <c r="R70" t="inlineStr"/>
+      <c r="S70" t="inlineStr">
+        <is>
+          <t>R$ 239.19</t>
+        </is>
+      </c>
+      <c r="T70" t="inlineStr"/>
+      <c r="U70" t="inlineStr">
+        <is>
+          <t>27/04/2023 15:23:27</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>Casa em Araruama</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr"/>
+      <c r="C71" t="inlineStr"/>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>Araruama piscina, churrasqueira, sinuca, pulápula</t>
+        </is>
+      </c>
+      <c r="E71" t="inlineStr"/>
+      <c r="F71" t="inlineStr"/>
+      <c r="G71" t="inlineStr"/>
+      <c r="H71" t="inlineStr"/>
+      <c r="I71" t="inlineStr">
+        <is>
+          <t>6 camas</t>
+        </is>
+      </c>
+      <c r="J71" t="inlineStr"/>
+      <c r="K71" t="inlineStr">
+        <is>
+          <t>R$804 por noite</t>
+        </is>
+      </c>
+      <c r="L71" t="inlineStr"/>
+      <c r="M71" t="inlineStr"/>
+      <c r="N71" t="inlineStr"/>
+      <c r="O71" t="inlineStr">
+        <is>
+          <t>4,94 (51)</t>
+        </is>
+      </c>
+      <c r="P71" t="inlineStr"/>
+      <c r="Q71" t="inlineStr">
+        <is>
+          <t>Superhost</t>
+        </is>
+      </c>
+      <c r="R71" t="inlineStr"/>
+      <c r="S71" t="inlineStr">
+        <is>
+          <t>R$ 239.19</t>
+        </is>
+      </c>
+      <c r="T71" t="inlineStr"/>
+      <c r="U71" t="inlineStr">
+        <is>
+          <t>27/04/2023 15:23:27</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>Casa em Areal</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr"/>
+      <c r="C72" t="inlineStr"/>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>Casa Lagoa Terraço</t>
+        </is>
+      </c>
+      <c r="E72" t="inlineStr"/>
+      <c r="F72" t="inlineStr"/>
+      <c r="G72" t="inlineStr"/>
+      <c r="H72" t="inlineStr"/>
+      <c r="I72" t="inlineStr">
+        <is>
+          <t>1 cama de casal</t>
+        </is>
+      </c>
+      <c r="J72" t="inlineStr"/>
+      <c r="K72" t="inlineStr">
+        <is>
+          <t>R$148 por noite</t>
+        </is>
+      </c>
+      <c r="L72" t="inlineStr"/>
+      <c r="M72" t="inlineStr"/>
+      <c r="N72" t="inlineStr"/>
+      <c r="O72" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="P72" t="inlineStr"/>
+      <c r="Q72" t="inlineStr">
+        <is>
+          <t>Superhost</t>
+        </is>
+      </c>
+      <c r="R72" t="inlineStr"/>
+      <c r="S72" t="inlineStr">
+        <is>
+          <t>R$ 239.19</t>
+        </is>
+      </c>
+      <c r="T72" t="inlineStr"/>
+      <c r="U72" t="inlineStr">
+        <is>
+          <t>27/04/2023 15:23:27</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>Casa em Vilatur</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr"/>
+      <c r="C73" t="inlineStr"/>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>Kitnet mobiliada em Saquarema.</t>
+        </is>
+      </c>
+      <c r="E73" t="inlineStr"/>
+      <c r="F73" t="inlineStr"/>
+      <c r="G73" t="inlineStr"/>
+      <c r="H73" t="inlineStr"/>
+      <c r="I73" t="inlineStr">
+        <is>
+          <t>6 camas</t>
+        </is>
+      </c>
+      <c r="J73" t="inlineStr"/>
+      <c r="K73" t="inlineStr">
+        <is>
+          <t>R$93 por noite, originalmente R$104</t>
+        </is>
+      </c>
+      <c r="L73" t="inlineStr"/>
+      <c r="M73" t="inlineStr"/>
+      <c r="N73" t="inlineStr"/>
+      <c r="O73" t="inlineStr">
+        <is>
+          <t>4,86 (69)</t>
+        </is>
+      </c>
+      <c r="P73" t="inlineStr"/>
+      <c r="Q73" t="inlineStr">
+        <is>
+          <t>Superhost</t>
+        </is>
+      </c>
+      <c r="R73" t="inlineStr"/>
+      <c r="S73" t="inlineStr">
+        <is>
+          <t>R$ 239.19</t>
+        </is>
+      </c>
+      <c r="T73" t="inlineStr"/>
+      <c r="U73" t="inlineStr">
+        <is>
+          <t>27/04/2023 15:23:27</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>Quarto privativo em Alto da Boa Vista</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr"/>
+      <c r="C74" t="inlineStr"/>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>Lugar de Sossego e muita Natureza.</t>
+        </is>
+      </c>
+      <c r="E74" t="inlineStr"/>
+      <c r="F74" t="inlineStr"/>
+      <c r="G74" t="inlineStr"/>
+      <c r="H74" t="inlineStr"/>
+      <c r="I74" t="inlineStr">
+        <is>
+          <t>1 cama de casal</t>
+        </is>
+      </c>
+      <c r="J74" t="inlineStr"/>
+      <c r="K74" t="inlineStr">
+        <is>
+          <t>R$184 por noite</t>
+        </is>
+      </c>
+      <c r="L74" t="inlineStr"/>
+      <c r="M74" t="inlineStr"/>
+      <c r="N74" t="inlineStr"/>
+      <c r="O74" t="inlineStr">
+        <is>
+          <t>4,94 (48)</t>
+        </is>
+      </c>
+      <c r="P74" t="inlineStr"/>
+      <c r="Q74" t="inlineStr">
+        <is>
+          <t>Superhost</t>
+        </is>
+      </c>
+      <c r="R74" t="inlineStr"/>
+      <c r="S74" t="inlineStr">
+        <is>
+          <t>R$ 239.19</t>
+        </is>
+      </c>
+      <c r="T74" t="inlineStr"/>
+      <c r="U74" t="inlineStr">
+        <is>
+          <t>27/04/2023 15:23:27</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>Quarto privativo em Araruama</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr"/>
+      <c r="C75" t="inlineStr"/>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>Acomodação suíte no centro de Praia Seca.</t>
+        </is>
+      </c>
+      <c r="E75" t="inlineStr"/>
+      <c r="F75" t="inlineStr"/>
+      <c r="G75" t="inlineStr"/>
+      <c r="H75" t="inlineStr"/>
+      <c r="I75" t="inlineStr">
+        <is>
+          <t>1 cama</t>
+        </is>
+      </c>
+      <c r="J75" t="inlineStr"/>
+      <c r="K75" t="inlineStr">
+        <is>
+          <t>R$147 por noite</t>
+        </is>
+      </c>
+      <c r="L75" t="inlineStr"/>
+      <c r="M75" t="inlineStr"/>
+      <c r="N75" t="inlineStr"/>
+      <c r="O75" t="inlineStr">
+        <is>
+          <t>5,0 (9)</t>
+        </is>
+      </c>
+      <c r="P75" t="inlineStr"/>
+      <c r="Q75" t="inlineStr">
+        <is>
+          <t>Superhost</t>
+        </is>
+      </c>
+      <c r="R75" t="inlineStr"/>
+      <c r="S75" t="inlineStr">
+        <is>
+          <t>R$ 239.19</t>
+        </is>
+      </c>
+      <c r="T75" t="inlineStr"/>
+      <c r="U75" t="inlineStr">
+        <is>
+          <t>27/04/2023 15:23:27</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>Casa em Salinas</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr"/>
+      <c r="C76" t="inlineStr"/>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>Casa em condomínio junto a lagoa, em Praia Seca</t>
+        </is>
+      </c>
+      <c r="E76" t="inlineStr"/>
+      <c r="F76" t="inlineStr"/>
+      <c r="G76" t="inlineStr"/>
+      <c r="H76" t="inlineStr"/>
+      <c r="I76" t="inlineStr">
+        <is>
+          <t>4 camas</t>
+        </is>
+      </c>
+      <c r="J76" t="inlineStr"/>
+      <c r="K76" t="inlineStr">
+        <is>
+          <t>R$290 por noite</t>
+        </is>
+      </c>
+      <c r="L76" t="inlineStr"/>
+      <c r="M76" t="inlineStr"/>
+      <c r="N76" t="inlineStr"/>
+      <c r="O76" t="inlineStr">
+        <is>
+          <t>5,0 (24)</t>
+        </is>
+      </c>
+      <c r="P76" t="inlineStr"/>
+      <c r="Q76" t="inlineStr"/>
+      <c r="R76" t="inlineStr"/>
+      <c r="S76" t="inlineStr">
+        <is>
+          <t>R$ 239.19</t>
+        </is>
+      </c>
+      <c r="T76" t="inlineStr"/>
+      <c r="U76" t="inlineStr">
+        <is>
+          <t>27/04/2023 15:23:27</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>Chalé em Iguaba Grande</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr"/>
+      <c r="C77" t="inlineStr"/>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>Chalé Mágico de Iguaba Grande</t>
+        </is>
+      </c>
+      <c r="E77" t="inlineStr"/>
+      <c r="F77" t="inlineStr"/>
+      <c r="G77" t="inlineStr"/>
+      <c r="H77" t="inlineStr"/>
+      <c r="I77" t="inlineStr">
+        <is>
+          <t>4 camas</t>
+        </is>
+      </c>
+      <c r="J77" t="inlineStr"/>
+      <c r="K77" t="inlineStr">
+        <is>
+          <t>R$238 por noite</t>
+        </is>
+      </c>
+      <c r="L77" t="inlineStr"/>
+      <c r="M77" t="inlineStr"/>
+      <c r="N77" t="inlineStr"/>
+      <c r="O77" t="inlineStr">
+        <is>
+          <t>Novo</t>
+        </is>
+      </c>
+      <c r="P77" t="inlineStr"/>
+      <c r="Q77" t="inlineStr"/>
+      <c r="R77" t="inlineStr"/>
+      <c r="S77" t="inlineStr">
+        <is>
+          <t>R$ 239.19</t>
+        </is>
+      </c>
+      <c r="T77" t="inlineStr"/>
+      <c r="U77" t="inlineStr">
+        <is>
+          <t>27/04/2023 15:23:27</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>Casa em Coqueiral</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr"/>
+      <c r="C78" t="inlineStr"/>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>Casa Espaçosa Privada c/ Piscina e Churrasqueira</t>
+        </is>
+      </c>
+      <c r="E78" t="inlineStr"/>
+      <c r="F78" t="inlineStr"/>
+      <c r="G78" t="inlineStr"/>
+      <c r="H78" t="inlineStr"/>
+      <c r="I78" t="inlineStr">
+        <is>
+          <t>15 camas</t>
+        </is>
+      </c>
+      <c r="J78" t="inlineStr"/>
+      <c r="K78" t="inlineStr">
+        <is>
+          <t>R$336 por noite</t>
+        </is>
+      </c>
+      <c r="L78" t="inlineStr"/>
+      <c r="M78" t="inlineStr"/>
+      <c r="N78" t="inlineStr"/>
+      <c r="O78" t="inlineStr">
+        <is>
+          <t>4,82 (11)</t>
+        </is>
+      </c>
+      <c r="P78" t="inlineStr"/>
+      <c r="Q78" t="inlineStr"/>
+      <c r="R78" t="inlineStr"/>
+      <c r="S78" t="inlineStr">
+        <is>
+          <t>R$ 239.19</t>
+        </is>
+      </c>
+      <c r="T78" t="inlineStr"/>
+      <c r="U78" t="inlineStr">
+        <is>
+          <t>27/04/2023 15:23:27</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>Casa de veraneio em Iguaba Grande</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr"/>
+      <c r="C79" t="inlineStr"/>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>Casinha Grega com vista para Lagoa!</t>
+        </is>
+      </c>
+      <c r="E79" t="inlineStr"/>
+      <c r="F79" t="inlineStr"/>
+      <c r="G79" t="inlineStr"/>
+      <c r="H79" t="inlineStr"/>
+      <c r="I79" t="inlineStr">
+        <is>
+          <t>4 camas</t>
+        </is>
+      </c>
+      <c r="J79" t="inlineStr"/>
+      <c r="K79" t="inlineStr">
+        <is>
+          <t>R$151 por noite</t>
+        </is>
+      </c>
+      <c r="L79" t="inlineStr"/>
+      <c r="M79" t="inlineStr"/>
+      <c r="N79" t="inlineStr"/>
+      <c r="O79" t="inlineStr">
+        <is>
+          <t>4,94 (53)</t>
+        </is>
+      </c>
+      <c r="P79" t="inlineStr"/>
+      <c r="Q79" t="inlineStr">
+        <is>
+          <t>Superhost</t>
+        </is>
+      </c>
+      <c r="R79" t="inlineStr"/>
+      <c r="S79" t="inlineStr">
+        <is>
+          <t>R$ 239.19</t>
+        </is>
+      </c>
+      <c r="T79" t="inlineStr"/>
+      <c r="U79" t="inlineStr">
+        <is>
+          <t>27/04/2023 15:23:27</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>Casa em Araruama</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr"/>
+      <c r="C80" t="inlineStr"/>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>Linda Casa em local tranquilo próximo à Lagoa</t>
+        </is>
+      </c>
+      <c r="E80" t="inlineStr"/>
+      <c r="F80" t="inlineStr"/>
+      <c r="G80" t="inlineStr"/>
+      <c r="H80" t="inlineStr"/>
+      <c r="I80" t="inlineStr">
+        <is>
+          <t>6 camas</t>
+        </is>
+      </c>
+      <c r="J80" t="inlineStr"/>
+      <c r="K80" t="inlineStr">
+        <is>
+          <t>R$650 por noite</t>
+        </is>
+      </c>
+      <c r="L80" t="inlineStr"/>
+      <c r="M80" t="inlineStr"/>
+      <c r="N80" t="inlineStr"/>
+      <c r="O80" t="inlineStr">
+        <is>
+          <t>4,93 (29)</t>
+        </is>
+      </c>
+      <c r="P80" t="inlineStr"/>
+      <c r="Q80" t="inlineStr">
+        <is>
+          <t>Superhost</t>
+        </is>
+      </c>
+      <c r="R80" t="inlineStr"/>
+      <c r="S80" t="inlineStr">
+        <is>
+          <t>R$ 239.19</t>
+        </is>
+      </c>
+      <c r="T80" t="inlineStr"/>
+      <c r="U80" t="inlineStr">
+        <is>
+          <t>27/04/2023 15:23:27</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>Casa em Atlantico</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr"/>
+      <c r="C81" t="inlineStr"/>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>Casa de frente para o mar, paz e tranquilidade</t>
+        </is>
+      </c>
+      <c r="E81" t="inlineStr"/>
+      <c r="F81" t="inlineStr"/>
+      <c r="G81" t="inlineStr"/>
+      <c r="H81" t="inlineStr"/>
+      <c r="I81" t="inlineStr">
+        <is>
+          <t>3 camas de casal</t>
+        </is>
+      </c>
+      <c r="J81" t="inlineStr"/>
+      <c r="K81" t="inlineStr">
+        <is>
+          <t>R$452 por noite</t>
+        </is>
+      </c>
+      <c r="L81" t="inlineStr"/>
+      <c r="M81" t="inlineStr"/>
+      <c r="N81" t="inlineStr"/>
+      <c r="O81" t="inlineStr">
+        <is>
+          <t>4,9 (40)</t>
+        </is>
+      </c>
+      <c r="P81" t="inlineStr"/>
+      <c r="Q81" t="inlineStr">
+        <is>
+          <t>Superhost</t>
+        </is>
+      </c>
+      <c r="R81" t="inlineStr"/>
+      <c r="S81" t="inlineStr">
+        <is>
+          <t>R$ 239.19</t>
+        </is>
+      </c>
+      <c r="T81" t="inlineStr"/>
+      <c r="U81" t="inlineStr">
+        <is>
+          <t>27/04/2023 15:23:27</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>Casa em Araruama</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr"/>
+      <c r="C82" t="inlineStr"/>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>Casa recanto Coqueiral</t>
+        </is>
+      </c>
+      <c r="E82" t="inlineStr"/>
+      <c r="F82" t="inlineStr"/>
+      <c r="G82" t="inlineStr"/>
+      <c r="H82" t="inlineStr"/>
+      <c r="I82" t="inlineStr">
+        <is>
+          <t>2 camas</t>
+        </is>
+      </c>
+      <c r="J82" t="inlineStr"/>
+      <c r="K82" t="inlineStr">
+        <is>
+          <t>R$356 por noite</t>
+        </is>
+      </c>
+      <c r="L82" t="inlineStr"/>
+      <c r="M82" t="inlineStr"/>
+      <c r="N82" t="inlineStr"/>
+      <c r="O82" t="inlineStr">
+        <is>
+          <t>Novo</t>
+        </is>
+      </c>
+      <c r="P82" t="inlineStr"/>
+      <c r="Q82" t="inlineStr"/>
+      <c r="R82" t="inlineStr"/>
+      <c r="S82" t="inlineStr">
+        <is>
+          <t>R$ 239.19</t>
+        </is>
+      </c>
+      <c r="T82" t="inlineStr"/>
+      <c r="U82" t="inlineStr">
+        <is>
+          <t>27/04/2023 15:23:27</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>Casa em Mutirão</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr"/>
+      <c r="C83" t="inlineStr"/>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>Casa com Piscina (16 pessoas) - Araruama, RJ</t>
+        </is>
+      </c>
+      <c r="E83" t="inlineStr"/>
+      <c r="F83" t="inlineStr"/>
+      <c r="G83" t="inlineStr"/>
+      <c r="H83" t="inlineStr"/>
+      <c r="I83" t="inlineStr">
+        <is>
+          <t>8 camas de casal</t>
+        </is>
+      </c>
+      <c r="J83" t="inlineStr"/>
+      <c r="K83" t="inlineStr">
+        <is>
+          <t>R$952 por noite</t>
+        </is>
+      </c>
+      <c r="L83" t="inlineStr"/>
+      <c r="M83" t="inlineStr"/>
+      <c r="N83" t="inlineStr"/>
+      <c r="O83" t="inlineStr">
+        <is>
+          <t>4,92 (24)</t>
+        </is>
+      </c>
+      <c r="P83" t="inlineStr"/>
+      <c r="Q83" t="inlineStr"/>
+      <c r="R83" t="inlineStr"/>
+      <c r="S83" t="inlineStr">
+        <is>
+          <t>R$ 239.19</t>
+        </is>
+      </c>
+      <c r="T83" t="inlineStr"/>
+      <c r="U83" t="inlineStr">
+        <is>
+          <t>27/04/2023 15:23:27</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>Casa em Araruama</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr"/>
+      <c r="C84" t="inlineStr"/>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>Casa em Praia Seca entre o Mar e a Lagoa</t>
+        </is>
+      </c>
+      <c r="E84" t="inlineStr"/>
+      <c r="F84" t="inlineStr"/>
+      <c r="G84" t="inlineStr"/>
+      <c r="H84" t="inlineStr"/>
+      <c r="I84" t="inlineStr">
+        <is>
+          <t>5 camas</t>
+        </is>
+      </c>
+      <c r="J84" t="inlineStr"/>
+      <c r="K84" t="inlineStr">
+        <is>
+          <t>R$399 por noite</t>
+        </is>
+      </c>
+      <c r="L84" t="inlineStr"/>
+      <c r="M84" t="inlineStr"/>
+      <c r="N84" t="inlineStr"/>
+      <c r="O84" t="inlineStr">
+        <is>
+          <t>5,0 (10)</t>
+        </is>
+      </c>
+      <c r="P84" t="inlineStr"/>
+      <c r="Q84" t="inlineStr"/>
+      <c r="R84" t="inlineStr"/>
+      <c r="S84" t="inlineStr">
+        <is>
+          <t>R$ 239.19</t>
+        </is>
+      </c>
+      <c r="T84" t="inlineStr"/>
+      <c r="U84" t="inlineStr">
+        <is>
+          <t>27/04/2023 15:23:27</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>Condomínio em Saquarema</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr"/>
+      <c r="C85" t="inlineStr"/>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>Casinha Náutica II - Itaúna</t>
+        </is>
+      </c>
+      <c r="E85" t="inlineStr"/>
+      <c r="F85" t="inlineStr"/>
+      <c r="G85" t="inlineStr"/>
+      <c r="H85" t="inlineStr"/>
+      <c r="I85" t="inlineStr">
+        <is>
+          <t>3 camas</t>
+        </is>
+      </c>
+      <c r="J85" t="inlineStr"/>
+      <c r="K85" t="inlineStr">
+        <is>
+          <t>R$174 por noite</t>
+        </is>
+      </c>
+      <c r="L85" t="inlineStr"/>
+      <c r="M85" t="inlineStr"/>
+      <c r="N85" t="inlineStr"/>
+      <c r="O85" t="inlineStr">
+        <is>
+          <t>5,0 (3)</t>
+        </is>
+      </c>
+      <c r="P85" t="inlineStr"/>
+      <c r="Q85" t="inlineStr"/>
+      <c r="R85" t="inlineStr"/>
+      <c r="S85" t="inlineStr">
+        <is>
+          <t>R$ 239.19</t>
+        </is>
+      </c>
+      <c r="T85" t="inlineStr"/>
+      <c r="U85" t="inlineStr">
+        <is>
+          <t>27/04/2023 15:23:27</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>Casa em Araruama</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr"/>
+      <c r="C86" t="inlineStr"/>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t>Casa 3 qts com Piscina e jacuzzi 
+Araruama RJ</t>
+        </is>
+      </c>
+      <c r="E86" t="inlineStr"/>
+      <c r="F86" t="inlineStr"/>
+      <c r="G86" t="inlineStr"/>
+      <c r="H86" t="inlineStr"/>
+      <c r="I86" t="inlineStr">
+        <is>
+          <t>6 camas</t>
+        </is>
+      </c>
+      <c r="J86" t="inlineStr"/>
+      <c r="K86" t="inlineStr">
+        <is>
+          <t>R$198 por noite, originalmente R$299</t>
+        </is>
+      </c>
+      <c r="L86" t="inlineStr"/>
+      <c r="M86" t="inlineStr"/>
+      <c r="N86" t="inlineStr"/>
+      <c r="O86" t="inlineStr">
+        <is>
+          <t>4,25 (16)</t>
+        </is>
+      </c>
+      <c r="P86" t="inlineStr"/>
+      <c r="Q86" t="inlineStr"/>
+      <c r="R86" t="inlineStr"/>
+      <c r="S86" t="inlineStr">
+        <is>
+          <t>R$ 239.19</t>
+        </is>
+      </c>
+      <c r="T86" t="inlineStr"/>
+      <c r="U86" t="inlineStr">
+        <is>
+          <t>27/04/2023 15:23:27</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>Apartamento em Iguaba Grande</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr"/>
+      <c r="C87" t="inlineStr"/>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>Apartamento 2 quartos em frente a Lagoa</t>
+        </is>
+      </c>
+      <c r="E87" t="inlineStr"/>
+      <c r="F87" t="inlineStr"/>
+      <c r="G87" t="inlineStr"/>
+      <c r="H87" t="inlineStr"/>
+      <c r="I87" t="inlineStr">
+        <is>
+          <t>3 camas</t>
+        </is>
+      </c>
+      <c r="J87" t="inlineStr"/>
+      <c r="K87" t="inlineStr">
+        <is>
+          <t>R$175 por noite</t>
+        </is>
+      </c>
+      <c r="L87" t="inlineStr"/>
+      <c r="M87" t="inlineStr"/>
+      <c r="N87" t="inlineStr"/>
+      <c r="O87" t="inlineStr">
+        <is>
+          <t>4,79 (47)</t>
+        </is>
+      </c>
+      <c r="P87" t="inlineStr"/>
+      <c r="Q87" t="inlineStr">
+        <is>
+          <t>Superhost</t>
+        </is>
+      </c>
+      <c r="R87" t="inlineStr"/>
+      <c r="S87" t="inlineStr">
+        <is>
+          <t>R$ 239.19</t>
+        </is>
+      </c>
+      <c r="T87" t="inlineStr"/>
+      <c r="U87" t="inlineStr">
+        <is>
+          <t>27/04/2023 15:23:27</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>Casa em Araruama</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr"/>
+      <c r="C88" t="inlineStr"/>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>Linda casa ao lado da lagoa</t>
+        </is>
+      </c>
+      <c r="E88" t="inlineStr"/>
+      <c r="F88" t="inlineStr"/>
+      <c r="G88" t="inlineStr"/>
+      <c r="H88" t="inlineStr"/>
+      <c r="I88" t="inlineStr">
+        <is>
+          <t>1 – 6 de mai.</t>
+        </is>
+      </c>
+      <c r="J88" t="inlineStr"/>
+      <c r="K88" t="inlineStr">
+        <is>
+          <t>R$472 por noite</t>
+        </is>
+      </c>
+      <c r="L88" t="inlineStr"/>
+      <c r="M88" t="inlineStr"/>
+      <c r="N88" t="inlineStr"/>
+      <c r="O88" t="inlineStr">
+        <is>
+          <t>5,0 (3)</t>
+        </is>
+      </c>
+      <c r="P88" t="inlineStr"/>
+      <c r="Q88" t="inlineStr"/>
+      <c r="R88" t="inlineStr"/>
+      <c r="S88" t="inlineStr">
+        <is>
+          <t>R$ 239.19</t>
+        </is>
+      </c>
+      <c r="T88" t="inlineStr"/>
+      <c r="U88" t="inlineStr">
+        <is>
+          <t>27/04/2023 15:23:27</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>Casa em Araruama</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr"/>
+      <c r="C89" t="inlineStr"/>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>Chalé de Madeira em condomínio fechado</t>
+        </is>
+      </c>
+      <c r="E89" t="inlineStr"/>
+      <c r="F89" t="inlineStr"/>
+      <c r="G89" t="inlineStr"/>
+      <c r="H89" t="inlineStr"/>
+      <c r="I89" t="inlineStr">
+        <is>
+          <t>2 camas</t>
+        </is>
+      </c>
+      <c r="J89" t="inlineStr"/>
+      <c r="K89" t="inlineStr">
+        <is>
+          <t>R$139 por noite</t>
+        </is>
+      </c>
+      <c r="L89" t="inlineStr"/>
+      <c r="M89" t="inlineStr"/>
+      <c r="N89" t="inlineStr"/>
+      <c r="O89" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="P89" t="inlineStr"/>
+      <c r="Q89" t="inlineStr"/>
+      <c r="R89" t="inlineStr"/>
+      <c r="S89" t="inlineStr">
+        <is>
+          <t>R$ 239.19</t>
+        </is>
+      </c>
+      <c r="T89" t="inlineStr"/>
+      <c r="U89" t="inlineStr">
+        <is>
+          <t>27/04/2023 15:23:27</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>Casa em Praia Linda</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr"/>
+      <c r="C90" t="inlineStr"/>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>Recanto dos Canários</t>
+        </is>
+      </c>
+      <c r="E90" t="inlineStr"/>
+      <c r="F90" t="inlineStr"/>
+      <c r="G90" t="inlineStr"/>
+      <c r="H90" t="inlineStr"/>
+      <c r="I90" t="inlineStr">
+        <is>
+          <t>4 camas</t>
+        </is>
+      </c>
+      <c r="J90" t="inlineStr"/>
+      <c r="K90" t="inlineStr">
+        <is>
+          <t>R$87 por noite</t>
+        </is>
+      </c>
+      <c r="L90" t="inlineStr"/>
+      <c r="M90" t="inlineStr"/>
+      <c r="N90" t="inlineStr"/>
+      <c r="O90" t="inlineStr">
+        <is>
+          <t>4,95 (74)</t>
+        </is>
+      </c>
+      <c r="P90" t="inlineStr"/>
+      <c r="Q90" t="inlineStr">
+        <is>
+          <t>Superhost</t>
+        </is>
+      </c>
+      <c r="R90" t="inlineStr"/>
+      <c r="S90" t="inlineStr">
+        <is>
+          <t>R$ 239.19</t>
+        </is>
+      </c>
+      <c r="T90" t="inlineStr"/>
+      <c r="U90" t="inlineStr">
+        <is>
+          <t>27/04/2023 15:23:27</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>Casa em Araruama</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr"/>
+      <c r="C91" t="inlineStr"/>
+      <c r="D91" t="inlineStr">
+        <is>
+          <t>Casa Rústica (Tipo de Acampamento)</t>
+        </is>
+      </c>
+      <c r="E91" t="inlineStr"/>
+      <c r="F91" t="inlineStr"/>
+      <c r="G91" t="inlineStr"/>
+      <c r="H91" t="inlineStr"/>
+      <c r="I91" t="inlineStr">
+        <is>
+          <t>3 camas</t>
+        </is>
+      </c>
+      <c r="J91" t="inlineStr"/>
+      <c r="K91" t="inlineStr">
+        <is>
+          <t>R$114 por noite</t>
+        </is>
+      </c>
+      <c r="L91" t="inlineStr"/>
+      <c r="M91" t="inlineStr"/>
+      <c r="N91" t="inlineStr"/>
+      <c r="O91" t="inlineStr">
+        <is>
+          <t>Novo</t>
+        </is>
+      </c>
+      <c r="P91" t="inlineStr"/>
+      <c r="Q91" t="inlineStr"/>
+      <c r="R91" t="inlineStr"/>
+      <c r="S91" t="inlineStr">
+        <is>
+          <t>R$ 239.19</t>
+        </is>
+      </c>
+      <c r="T91" t="inlineStr"/>
+      <c r="U91" t="inlineStr">
+        <is>
+          <t>27/04/2023 15:23:27</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Correcao rating e adicao var dados
</commit_message>
<xml_diff>
--- a/araruama_stats.xlsx
+++ b/araruama_stats.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="687" uniqueCount="279">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="690" uniqueCount="295">
   <si>
     <t>title</t>
   </si>
@@ -79,28 +79,40 @@
     <t>Casa em Araruama</t>
   </si>
   <si>
-    <t>Casa em Village D Italia</t>
+    <t>Casa em Parque Hotel</t>
+  </si>
+  <si>
+    <t>Apartamento em Araruama</t>
+  </si>
+  <si>
+    <t>Casa de campo em Araruama</t>
+  </si>
+  <si>
+    <t>Casa em Fonte Limpa</t>
+  </si>
+  <si>
+    <t>Chalé em Coqueiral</t>
+  </si>
+  <si>
+    <t>Condomínio em Araruama</t>
+  </si>
+  <si>
+    <t>Apartamento em Parque Hotel</t>
+  </si>
+  <si>
+    <t>Casa de hóspedes em Araruama</t>
   </si>
   <si>
     <t>Casa em Ponte dos Leites</t>
   </si>
   <si>
-    <t>Casa de campo em Araruama</t>
-  </si>
-  <si>
-    <t>Casa em Parque Hotel</t>
-  </si>
-  <si>
-    <t>Apartamento em Araruama</t>
-  </si>
-  <si>
-    <t>Condomínio em Araruama</t>
-  </si>
-  <si>
     <t>Casa de campo em Praia Seca</t>
   </si>
   <si>
-    <t>Casa em Fonte Limpa</t>
+    <t>Vila em Fazendinha</t>
+  </si>
+  <si>
+    <t>Quarto em Alto da Boa Vista</t>
   </si>
   <si>
     <t>Casa em Atlantico</t>
@@ -109,121 +121,136 @@
     <t>Casa de hóspedes em Pontinha</t>
   </si>
   <si>
+    <t>Quarto em Araruama</t>
+  </si>
+  <si>
+    <t>Casa em Coqueiral</t>
+  </si>
+  <si>
+    <t>Casa de veraneio em Iguaba Grande</t>
+  </si>
+  <si>
+    <t>Casa em Praia Seca</t>
+  </si>
+  <si>
+    <t>Casa em Saquarema</t>
+  </si>
+  <si>
+    <t>Casa em Princess Park</t>
+  </si>
+  <si>
+    <t>Microcasa em Vilatur</t>
+  </si>
+  <si>
+    <t>Casa em Salinas</t>
+  </si>
+  <si>
+    <t>Lugar para ficar em Araruama</t>
+  </si>
+  <si>
+    <t>Casa em Arraial do Cabo</t>
+  </si>
+  <si>
+    <t>Casa em Porto da Roça I</t>
+  </si>
+  <si>
+    <t>Casa em Cabo Frio</t>
+  </si>
+  <si>
+    <t>Casa em Hospicio</t>
+  </si>
+  <si>
+    <t>Casa em Vilatur</t>
+  </si>
+  <si>
+    <t>Apartamento em Cabo Frio</t>
+  </si>
+  <si>
+    <t>Casa em Iguaba Pequena</t>
+  </si>
+  <si>
+    <t>Loft em Araruama</t>
+  </si>
+  <si>
+    <t>Casa em Ipitangas</t>
+  </si>
+  <si>
     <t>Casa em Praia Linda</t>
   </si>
   <si>
-    <t>Casa em Coqueiral</t>
-  </si>
-  <si>
-    <t>Loft em Araruama</t>
-  </si>
-  <si>
-    <t>Casa de veraneio em Iguaba Grande</t>
-  </si>
-  <si>
-    <t>Quarto em Alto da Boa Vista</t>
-  </si>
-  <si>
-    <t>Casa em Fazendinha</t>
-  </si>
-  <si>
-    <t>Casa de hóspedes em Araruama</t>
-  </si>
-  <si>
-    <t>Casa em Arraial do Cabo</t>
-  </si>
-  <si>
-    <t>Quarto em Araruama</t>
-  </si>
-  <si>
-    <t>Vila em Fazendinha</t>
-  </si>
-  <si>
-    <t>Casa em Cabo Frio</t>
-  </si>
-  <si>
-    <t>Casa em Vilatur</t>
-  </si>
-  <si>
-    <t>Casa em São Pedro da Aldeia</t>
-  </si>
-  <si>
-    <t>Casa em Hospicio</t>
-  </si>
-  <si>
-    <t>Apartamento em Cabo Frio</t>
-  </si>
-  <si>
-    <t>Casa em Iguaba Grande</t>
-  </si>
-  <si>
-    <t>Apartamento em Parque Hotel</t>
-  </si>
-  <si>
-    <t>Casa em Praia Seca</t>
-  </si>
-  <si>
-    <t>Casa de hóspedes em Parque Hotel</t>
-  </si>
-  <si>
-    <t>Casa em Salinas</t>
-  </si>
-  <si>
-    <t>Suíte de hóspedes em Arraial do Cabo</t>
+    <t>Casa em Célula Mater</t>
+  </si>
+  <si>
+    <t>Casa em Praia Grande</t>
+  </si>
+  <si>
+    <t>Região dos lagos - Araruama - Saquarema - Arraial</t>
+  </si>
+  <si>
+    <t>Casa tranquila, bem localizada Ar opcional Tv wifi</t>
+  </si>
+  <si>
+    <t>Pedacinho do Céu</t>
+  </si>
+  <si>
+    <t>Meu aconchego</t>
+  </si>
+  <si>
+    <t>loft &lt;SPA&lt; onde você descansa relaxa e se renova</t>
+  </si>
+  <si>
+    <t>Aconchegante Casa - Quintal &amp; Garagem</t>
+  </si>
+  <si>
+    <t>Apto na Região dos lagos. Aconchegante e central.</t>
+  </si>
+  <si>
+    <t>Loft completo para temporada</t>
+  </si>
+  <si>
+    <t>Casa de Praia agradável com piscina em Praia Seca</t>
+  </si>
+  <si>
+    <t>Ampla casa com quintal e garagem - Araruama/RJ</t>
+  </si>
+  <si>
+    <t>Araruama. Casa aconchegante com WiFi. Aceito Pet</t>
+  </si>
+  <si>
+    <t>Chalé Recantinho da Lagoa, Araruama,Rj</t>
+  </si>
+  <si>
+    <t>Apartamento à beira da orla de Araruama</t>
+  </si>
+  <si>
+    <t>Casa em Araruama 1</t>
+  </si>
+  <si>
+    <t>Apartamento na Lagoa de Araruama</t>
+  </si>
+  <si>
+    <t>VEM! Casa Rodrigues - Praia Seca, Araruama</t>
+  </si>
+  <si>
+    <t>Aluguel por temporada com piscina privativa</t>
+  </si>
+  <si>
+    <t>Casa com piscina em condomínio Sonho de Vida</t>
+  </si>
+  <si>
+    <t>Casa aconchegante em ótima localização em Araruama</t>
+  </si>
+  <si>
+    <t>Casa Maravilhosa com Lagoa privativa</t>
   </si>
   <si>
     <t>loft Peniel lugar tranquilo</t>
   </si>
   <si>
-    <t>Pedacinho do Céu</t>
-  </si>
-  <si>
-    <t>Região dos lagos - Araruama - Saquarema - Arraial</t>
-  </si>
-  <si>
-    <t>Chez Tonico_  Casa em Praia Seca, frente Lagoa.</t>
-  </si>
-  <si>
-    <t>Casa com piscina em condomínio Sonho de Vida</t>
-  </si>
-  <si>
-    <t>Casa de Praia agradável com piscina em Praia Seca</t>
-  </si>
-  <si>
-    <t>Casa espetacular! Piscina, sauna, churrasqueira…</t>
-  </si>
-  <si>
-    <t>Meu aconchego</t>
-  </si>
-  <si>
-    <t>Loft completo para temporada</t>
-  </si>
-  <si>
-    <t>Aconchegante Casa - Quintal &amp; Garagem</t>
-  </si>
-  <si>
-    <t>Aluguel por temporada com piscina privativa</t>
-  </si>
-  <si>
-    <t>Casa em Araruama 1</t>
-  </si>
-  <si>
-    <t>Apto na Região dos lagos. Aconchegante e central.</t>
-  </si>
-  <si>
-    <t>Apartamento à beira da orla de Araruama</t>
-  </si>
-  <si>
-    <t>Ampla casa com quintal e garagem - Araruama/RJ</t>
-  </si>
-  <si>
-    <t>Linda Casa em local tranquilo próximo à Lagoa</t>
-  </si>
-  <si>
-    <t>RECANTO MAJESTIC</t>
-  </si>
-  <si>
-    <t>Casa Maravilhosa com Lagoa privativa</t>
+    <t>Jms Recanto Região dos Lagos</t>
+  </si>
+  <si>
+    <t>casa em condomínio albatroz</t>
   </si>
   <si>
     <t>Kitinete em Araruama/RJ!
@@ -231,178 +258,182 @@
 Perto da Praia!</t>
   </si>
   <si>
-    <t>La Casa de Praia</t>
-  </si>
-  <si>
-    <t>Araruama. Casa aconchegante com WiFi. Aceito Pet</t>
+    <t>Curta o melhor de Araruama e Região dos Lagos</t>
+  </si>
+  <si>
+    <t>Casa em condominio com piscina e churrasqueira.</t>
+  </si>
+  <si>
+    <t>Suíte em Araruama - Praça da bandeira</t>
   </si>
   <si>
     <t>Casa aconchegante, piscina. Praia Seca - Araruama.</t>
   </si>
   <si>
+    <t>Casa do Alto da Pontinha</t>
+  </si>
+  <si>
+    <t>Acomodação suíte no centro de Praia Seca.</t>
+  </si>
+  <si>
+    <t>Suíte aconchegante no centro de Praia Seca.</t>
+  </si>
+  <si>
+    <t>Casa de Araruama com piscina, Coqueiral.</t>
+  </si>
+  <si>
+    <t>Linda kitnet em Iguaba Grande</t>
+  </si>
+  <si>
+    <t>Linda CASA Charmosa Duplex a 50M da Praia e Lagoa</t>
+  </si>
+  <si>
+    <t>Aconchegante casa com bastante espaço</t>
+  </si>
+  <si>
+    <t>Casa Espaçosa Privada c/ Piscina e Churrasqueira</t>
+  </si>
+  <si>
+    <t>RECANTO MAJESTIC</t>
+  </si>
+  <si>
+    <t>Espaço acolhedor para hóspedes na praia</t>
+  </si>
+  <si>
+    <t>Pedacinho do Céu 2</t>
+  </si>
+  <si>
+    <t>Casa do parque térrea a 100m da lagoa</t>
+  </si>
+  <si>
+    <t>Casa com piscina e parquinho em Vilatur, Saquarema</t>
+  </si>
+  <si>
+    <t>casa da vovó Luluca.</t>
+  </si>
+  <si>
+    <t>apartamento super confortável</t>
+  </si>
+  <si>
     <t>Casa na Região dos Lagos</t>
   </si>
   <si>
-    <t>Casa aconchegante em ótima localização em Araruama</t>
-  </si>
-  <si>
-    <t>Casa do Alto da Pontinha</t>
+    <t>Casa com piscina, sauna, campo, SPA, churrasqueira</t>
+  </si>
+  <si>
+    <t>Casa de praia - Região de Lagos</t>
+  </si>
+  <si>
+    <t>Casa aconchegante para lazer e descanso Araruama</t>
+  </si>
+  <si>
+    <t>Casa de Frente para o Mar</t>
+  </si>
+  <si>
+    <t>Villa cactus microcasa 2</t>
+  </si>
+  <si>
+    <t>Casa em condomínio junto a lagoa, em Praia Seca</t>
+  </si>
+  <si>
+    <t>Maju House</t>
+  </si>
+  <si>
+    <t>Belíssima casa em frente a Lagoa/Arraial do Cabo</t>
+  </si>
+  <si>
+    <t>casinha aconchegante com piscina</t>
+  </si>
+  <si>
+    <t>Loft Caeté com mezanino</t>
+  </si>
+  <si>
+    <t>Casa para temporada</t>
+  </si>
+  <si>
+    <t>Casa com churrasqueira perto da praia do Barbudo</t>
+  </si>
+  <si>
+    <t>Alugue por Temporada e Espaço para Eventos</t>
+  </si>
+  <si>
+    <t>Casa com piscina, perto da Lagoa</t>
+  </si>
+  <si>
+    <t>Flat Caminho de Búzios 3</t>
+  </si>
+  <si>
+    <t>Casa Blu (Santorini Experience) - Araruama</t>
+  </si>
+  <si>
+    <t>Casa Gran Canaria</t>
+  </si>
+  <si>
+    <t>Kitnet mobiliada em Saquarema.</t>
+  </si>
+  <si>
+    <t>Ap belíssimo em frente à lagoa</t>
+  </si>
+  <si>
+    <t>#Hospedagem Nota 10 Araruama!</t>
+  </si>
+  <si>
+    <t>Casa espetacular! Piscina, sauna, churrasqueira…</t>
+  </si>
+  <si>
+    <t>Cobertura na Praia do Forte</t>
+  </si>
+  <si>
+    <t>Casa de praia bem espaçosa. Próxima a lagoa.</t>
+  </si>
+  <si>
+    <t>Casa inteira com piscina</t>
+  </si>
+  <si>
+    <t>Araruama piscina, churrasqueira, sinuca, pulápula</t>
+  </si>
+  <si>
+    <t>Bonita casa em local agradável</t>
+  </si>
+  <si>
+    <t>Casa em praia seca</t>
+  </si>
+  <si>
+    <t>Conforto lagoa praia perto</t>
+  </si>
+  <si>
+    <t>Loft  Caeté</t>
+  </si>
+  <si>
+    <t>Paraíso Araruama
+Praia Seca</t>
+  </si>
+  <si>
+    <t>Casa de frente para o mar, paz e tranquilidade</t>
+  </si>
+  <si>
+    <t>Meu aconchego, paz e tranquilidade</t>
   </si>
   <si>
     <t>Recanto dos Canários</t>
   </si>
   <si>
-    <t>Casa de Araruama com piscina, Coqueiral.</t>
-  </si>
-  <si>
-    <t>Loft  Caeté</t>
-  </si>
-  <si>
-    <t>Linda kitnet em Iguaba Grande</t>
-  </si>
-  <si>
-    <t>Suíte em Araruama - Praça da bandeira</t>
-  </si>
-  <si>
-    <t>Pedacinho do Céu 2</t>
-  </si>
-  <si>
-    <t>Casa em Araruama 2</t>
-  </si>
-  <si>
-    <t>Jms Recanto Região dos Lagos</t>
-  </si>
-  <si>
-    <t>apartamento super confortável</t>
-  </si>
-  <si>
-    <t>Belíssima casa em frente a Lagoa/Arraial do Cabo</t>
-  </si>
-  <si>
-    <t>Acomodação suíte no centro de Praia Seca.</t>
-  </si>
-  <si>
-    <t>Casa em condominio com piscina e churrasqueira.</t>
+    <t>Apartamento em frente a lagoa de Araruama</t>
+  </si>
+  <si>
+    <t>Casa ampla e arejada, a 3 minutos da praia!</t>
+  </si>
+  <si>
+    <t>Casa agradável com piscina e churrasqueira</t>
   </si>
   <si>
     <t>Casinha Grega com vista para Lagoa!</t>
   </si>
   <si>
-    <t>Casa em Praia Seca entre o Mar e a Lagoa</t>
-  </si>
-  <si>
-    <t>Apartamento em Praia Seca</t>
-  </si>
-  <si>
-    <t>Casa recanto Coqueiral</t>
-  </si>
-  <si>
-    <t>Praia pertinho! 4 suítes, Piscina e Churrasqueira</t>
-  </si>
-  <si>
-    <t>Praia do Foguete/Casa 04</t>
-  </si>
-  <si>
-    <t>Refúgio na laguna</t>
-  </si>
-  <si>
-    <t>Excelente Casa Cond. AlphaBeach</t>
-  </si>
-  <si>
-    <t>Conforto lagoa praia perto</t>
-  </si>
-  <si>
-    <t>Apartamento em frente a lagoa de Araruama</t>
-  </si>
-  <si>
-    <t>Kitnet mobiliada em Saquarema.</t>
-  </si>
-  <si>
-    <t>Flat em São Pedro da Aldeia</t>
-  </si>
-  <si>
-    <t>Linda CASA Charmosa Duplex a 50M da Praia e Lagoa</t>
-  </si>
-  <si>
-    <t>Casa de Frente para o Mar</t>
-  </si>
-  <si>
-    <t>Casa Pé na Areia Praia Seca</t>
-  </si>
-  <si>
-    <t>Casa aconchegante para lazer e descanso Araruama</t>
-  </si>
-  <si>
-    <t>Casa aconchegante !</t>
-  </si>
-  <si>
-    <t>Casa com piscina condomínio Sonho de Vida</t>
-  </si>
-  <si>
-    <t>Casarão com Piscina poucos passos do Mar (PRAIA)</t>
-  </si>
-  <si>
-    <t>Alugue por Temporada e Espaço para Eventos</t>
-  </si>
-  <si>
-    <t>casa em condomínio albatroz</t>
-  </si>
-  <si>
-    <t>Suíte aconchegante no centro de Praia Seca.</t>
-  </si>
-  <si>
-    <t>Excelente casa piscina com hidro e área gourmet</t>
-  </si>
-  <si>
-    <t>Araruama piscina, churrasqueira, sinuca, pulápula</t>
-  </si>
-  <si>
-    <t>Cobertura na Praia do Forte</t>
-  </si>
-  <si>
-    <t>Praia Seca um paraíso escondido</t>
-  </si>
-  <si>
-    <t>Praia do Foguete/Casa 02</t>
-  </si>
-  <si>
-    <t>Casa Iguaba Grande espaçosa.</t>
-  </si>
-  <si>
-    <t>Recanto Tropical Araruama - Lindo Apto c/ Piscina</t>
-  </si>
-  <si>
-    <t>Casa em frente a lagoa iguabinha</t>
-  </si>
-  <si>
-    <t>Casa de frente para o mar, paz e tranquilidade</t>
-  </si>
-  <si>
-    <t>Casa Agradável em Arraial do Cabo - Condomínio</t>
-  </si>
-  <si>
-    <t>Casa Gran Canaria</t>
-  </si>
-  <si>
-    <t>Casa do parque térrea a 100m da lagoa</t>
-  </si>
-  <si>
-    <t>Casa completa c piscina/churrasqueira em Araruama</t>
-  </si>
-  <si>
-    <t>Casa em condomínio junto a lagoa, em Praia Seca</t>
-  </si>
-  <si>
-    <t>Casa Espaçosa Privada c/ Piscina e Churrasqueira</t>
-  </si>
-  <si>
-    <t>Casa em praia seca com piscina e um belo jardim</t>
-  </si>
-  <si>
-    <t>Casa de praia bem espaçosa. Próxima a lagoa.</t>
-  </si>
-  <si>
-    <t>Loft com vista pro mar e ar condicionado(Bromélia)</t>
+    <t>Excelente Casa Araruama 2100m2 área EXCLUSIVA</t>
+  </si>
+  <si>
+    <t>2 camas de casal</t>
   </si>
   <si>
     <t>2 camas</t>
@@ -411,448 +442,466 @@
     <t>1 cama de casal</t>
   </si>
   <si>
-    <t>2 camas de casal</t>
-  </si>
-  <si>
-    <t>10 camas</t>
+    <t>9 camas</t>
+  </si>
+  <si>
+    <t>1 cama queen</t>
+  </si>
+  <si>
+    <t>5 camas</t>
+  </si>
+  <si>
+    <t>4 camas</t>
+  </si>
+  <si>
+    <t>3 camas</t>
   </si>
   <si>
     <t>7 camas</t>
   </si>
   <si>
-    <t>5 camas</t>
-  </si>
-  <si>
-    <t>9 camas</t>
-  </si>
-  <si>
-    <t>1 cama queen</t>
-  </si>
-  <si>
-    <t>3 camas</t>
-  </si>
-  <si>
-    <t>4 camas</t>
+    <t>3 camas de casal</t>
+  </si>
+  <si>
+    <t>Hospede-se com Matheus Franceschi</t>
+  </si>
+  <si>
+    <t>Hospede-se com Lilian</t>
+  </si>
+  <si>
+    <t>8 camas</t>
+  </si>
+  <si>
+    <t>1 cama</t>
+  </si>
+  <si>
+    <t>15 camas</t>
   </si>
   <si>
     <t>6 camas</t>
   </si>
   <si>
-    <t>8 camas</t>
-  </si>
-  <si>
-    <t>3 camas de casal</t>
-  </si>
-  <si>
-    <t>Hospede-se com Matheus Franceschi</t>
-  </si>
-  <si>
-    <t>Hospede-se com Lilian</t>
-  </si>
-  <si>
-    <t>1 cama</t>
-  </si>
-  <si>
-    <t>15 camas</t>
-  </si>
-  <si>
-    <t>13 camas</t>
-  </si>
-  <si>
-    <t>R$185 por noite, originalmente R$226</t>
-  </si>
-  <si>
-    <t>R$84 por noite</t>
-  </si>
-  <si>
-    <t>R$107 por noite</t>
-  </si>
-  <si>
-    <t>R$531 por noite</t>
-  </si>
-  <si>
-    <t>R$222 por noite, originalmente R$252</t>
-  </si>
-  <si>
-    <t>R$234 por noite</t>
+    <t>27 camas</t>
+  </si>
+  <si>
+    <t>R$101 por noite</t>
+  </si>
+  <si>
+    <t>R$127 por noite</t>
+  </si>
+  <si>
+    <t>R$81 por noite, originalmente R$90</t>
+  </si>
+  <si>
+    <t>R$204 por noite</t>
+  </si>
+  <si>
+    <t>R$194 por noite</t>
+  </si>
+  <si>
+    <t>R$137 por noite</t>
+  </si>
+  <si>
+    <t>R$128 por noite</t>
+  </si>
+  <si>
+    <t>R$299 por noite</t>
+  </si>
+  <si>
+    <t>R$235 por noite</t>
+  </si>
+  <si>
+    <t>R$154 por noite</t>
+  </si>
+  <si>
+    <t>R$93 por noite</t>
+  </si>
+  <si>
+    <t>R$91 por noite</t>
+  </si>
+  <si>
+    <t>R$228 por noite</t>
+  </si>
+  <si>
+    <t>R$117 por noite</t>
+  </si>
+  <si>
+    <t>R$210 por noite</t>
+  </si>
+  <si>
+    <t>R$116 por noite</t>
+  </si>
+  <si>
+    <t>R$318 por noite</t>
+  </si>
+  <si>
+    <t>R$222 por noite, originalmente R$253</t>
+  </si>
+  <si>
+    <t>R$126 por noite</t>
+  </si>
+  <si>
+    <t>R$141 por noite</t>
+  </si>
+  <si>
+    <t>R$228 por noite, originalmente R$261</t>
+  </si>
+  <si>
+    <t>R$67 por noite</t>
+  </si>
+  <si>
+    <t>R$138 por noite</t>
+  </si>
+  <si>
+    <t>R$187 por noite</t>
+  </si>
+  <si>
+    <t>R$133 por noite</t>
+  </si>
+  <si>
+    <t>R$244 por noite, originalmente R$285</t>
+  </si>
+  <si>
+    <t xml:space="preserve">, </t>
+  </si>
+  <si>
+    <t>R$234 por noite, originalmente R$287</t>
+  </si>
+  <si>
+    <t>R$72 por noite</t>
+  </si>
+  <si>
+    <t>R$152 por noite</t>
+  </si>
+  <si>
+    <t>R$172 por noite</t>
+  </si>
+  <si>
+    <t>R$196 por noite</t>
+  </si>
+  <si>
+    <t>R$82 por noite, originalmente R$90</t>
+  </si>
+  <si>
+    <t>R$180 por noite</t>
+  </si>
+  <si>
+    <t>R$121 por noite</t>
+  </si>
+  <si>
+    <t>R$327 por noite</t>
+  </si>
+  <si>
+    <t>R$566 por noite</t>
+  </si>
+  <si>
+    <t>R$423 por noite, originalmente R$505</t>
+  </si>
+  <si>
+    <t>R$128 por noite, originalmente R$147</t>
+  </si>
+  <si>
+    <t>R$583 por noite, originalmente R$655</t>
+  </si>
+  <si>
+    <t>R$380 por noite</t>
+  </si>
+  <si>
+    <t>R$693 por noite</t>
+  </si>
+  <si>
+    <t>R$174 por noite, originalmente R$212</t>
+  </si>
+  <si>
+    <t>R$135 por noite, originalmente R$181</t>
+  </si>
+  <si>
+    <t>R$1.137 por noite</t>
+  </si>
+  <si>
+    <t>R$377 por noite, originalmente R$458</t>
+  </si>
+  <si>
+    <t>R$529 por noite</t>
+  </si>
+  <si>
+    <t>R$417 por noite</t>
+  </si>
+  <si>
+    <t>R$233 por noite</t>
+  </si>
+  <si>
+    <t>R$273 por noite, originalmente R$333</t>
+  </si>
+  <si>
+    <t>R$159 por noite, originalmente R$181</t>
+  </si>
+  <si>
+    <t>R$320 por noite</t>
+  </si>
+  <si>
+    <t>R$251 por noite</t>
+  </si>
+  <si>
+    <t>R$139 por noite, originalmente R$199</t>
+  </si>
+  <si>
+    <t>R$89 por noite</t>
+  </si>
+  <si>
+    <t>R$399 por noite</t>
+  </si>
+  <si>
+    <t>R$50 por noite, originalmente R$60</t>
+  </si>
+  <si>
+    <t>R$288 por noite, originalmente R$337</t>
+  </si>
+  <si>
+    <t>R$177 por noite</t>
+  </si>
+  <si>
+    <t>R$106 por noite</t>
+  </si>
+  <si>
+    <t>R$268 por noite</t>
+  </si>
+  <si>
+    <t>R$522 por noite</t>
   </si>
   <si>
     <t>R$1.138 por noite</t>
   </si>
   <si>
-    <t>R$229 por noite</t>
-  </si>
-  <si>
-    <t>R$299 por noite</t>
-  </si>
-  <si>
-    <t>R$137 por noite</t>
-  </si>
-  <si>
-    <t>R$318 por noite</t>
-  </si>
-  <si>
-    <t>R$117 por noite</t>
-  </si>
-  <si>
-    <t>R$115 por noite, originalmente R$126</t>
-  </si>
-  <si>
-    <t>R$228 por noite</t>
-  </si>
-  <si>
-    <t>R$355 por noite</t>
-  </si>
-  <si>
-    <t>R$154 por noite</t>
-  </si>
-  <si>
-    <t>R$628 por noite</t>
-  </si>
-  <si>
-    <t>R$566 por noite</t>
-  </si>
-  <si>
-    <t>R$127 por noite</t>
-  </si>
-  <si>
-    <t>R$187 por noite</t>
-  </si>
-  <si>
-    <t>R$255 por noite, originalmente R$310</t>
-  </si>
-  <si>
-    <t>R$93 por noite</t>
-  </si>
-  <si>
-    <t>R$234 por noite, originalmente R$286</t>
-  </si>
-  <si>
-    <t>R$132 por noite, originalmente R$175</t>
-  </si>
-  <si>
-    <t>R$80 por noite</t>
+    <t>R$1.301 por noite</t>
+  </si>
+  <si>
+    <t>R$334 por noite</t>
+  </si>
+  <si>
+    <t>R$344 por noite</t>
+  </si>
+  <si>
+    <t>R$804 por noite</t>
+  </si>
+  <si>
+    <t>R$173 por noite</t>
+  </si>
+  <si>
+    <t>R$730 por noite, originalmente R$890</t>
+  </si>
+  <si>
+    <t>R$281 por noite, originalmente R$343</t>
+  </si>
+  <si>
+    <t>R$931 por noite</t>
+  </si>
+  <si>
+    <t>R$418 por noite</t>
   </si>
   <si>
     <t>R$87 por noite</t>
   </si>
   <si>
-    <t>R$196 por noite</t>
-  </si>
-  <si>
-    <t>R$320 por noite</t>
-  </si>
-  <si>
-    <t>R$91 por noite</t>
-  </si>
-  <si>
-    <t xml:space="preserve">, </t>
-  </si>
-  <si>
-    <t>R$134 por noite, originalmente R$147</t>
-  </si>
-  <si>
-    <t>R$67 por noite</t>
-  </si>
-  <si>
-    <t>R$172 por noite, originalmente R$210</t>
-  </si>
-  <si>
-    <t>R$101 por noite</t>
-  </si>
-  <si>
-    <t>R$135 por noite, originalmente R$165</t>
-  </si>
-  <si>
-    <t>R$153 por noite</t>
-  </si>
-  <si>
-    <t>R$220 por noite</t>
-  </si>
-  <si>
-    <t>R$365 por noite</t>
-  </si>
-  <si>
-    <t>R$197 por noite</t>
-  </si>
-  <si>
-    <t>R$319 por noite, originalmente R$350</t>
-  </si>
-  <si>
-    <t>R$98 por noite</t>
-  </si>
-  <si>
-    <t>R$290 por noite, originalmente R$350</t>
-  </si>
-  <si>
-    <t>R$314 por noite</t>
-  </si>
-  <si>
-    <t>R$281 por noite, originalmente R$343</t>
-  </si>
-  <si>
     <t>R$217 por noite</t>
   </si>
   <si>
-    <t>R$94 por noite, originalmente R$105</t>
-  </si>
-  <si>
-    <t>R$98 por noite, originalmente R$107</t>
-  </si>
-  <si>
-    <t>R$179 por noite</t>
-  </si>
-  <si>
-    <t>R$462 por noite</t>
-  </si>
-  <si>
-    <t>R$255 por noite</t>
-  </si>
-  <si>
-    <t>R$529 por noite</t>
-  </si>
-  <si>
-    <t>R$151 por noite, originalmente R$184</t>
-  </si>
-  <si>
-    <t>R$304 por noite</t>
-  </si>
-  <si>
-    <t>R$468 por noite, originalmente R$558</t>
-  </si>
-  <si>
-    <t>R$89 por noite</t>
-  </si>
-  <si>
-    <t>R$138 por noite</t>
-  </si>
-  <si>
-    <t>R$169 por noite</t>
-  </si>
-  <si>
-    <t>R$459 por noite</t>
-  </si>
-  <si>
-    <t>R$804 por noite</t>
-  </si>
-  <si>
-    <t>R$1.301 por noite</t>
-  </si>
-  <si>
-    <t>R$410 por noite, originalmente R$500</t>
-  </si>
-  <si>
-    <t>R$94 por noite</t>
-  </si>
-  <si>
-    <t>R$144 por noite, originalmente R$158</t>
-  </si>
-  <si>
-    <t>R$285 por noite</t>
-  </si>
-  <si>
-    <t>R$417 por noite</t>
-  </si>
-  <si>
-    <t>R$514 por noite</t>
-  </si>
-  <si>
-    <t>R$139 por noite</t>
-  </si>
-  <si>
-    <t>R$549 por noite, originalmente R$657</t>
-  </si>
-  <si>
-    <t>R$173 por noite, originalmente R$212</t>
-  </si>
-  <si>
-    <t>R$233 por noite</t>
-  </si>
-  <si>
-    <t>R$249 por noite, originalmente R$287</t>
-  </si>
-  <si>
-    <t>R$387 por noite</t>
-  </si>
-  <si>
-    <t>R$334 por noite</t>
-  </si>
-  <si>
-    <t>R$67 por noite, originalmente R$172</t>
+    <t>R$426 por noite</t>
+  </si>
+  <si>
+    <t>R$576 por noite</t>
+  </si>
+  <si>
+    <t>R$479 por noite</t>
+  </si>
+  <si>
+    <t>4,79 (287)</t>
+  </si>
+  <si>
+    <t>4,93 (28)</t>
+  </si>
+  <si>
+    <t>4,86 (14)</t>
+  </si>
+  <si>
+    <t>4,93 (14)</t>
+  </si>
+  <si>
+    <t>5,0 (17)</t>
+  </si>
+  <si>
+    <t>4,9 (49)</t>
+  </si>
+  <si>
+    <t>4,78 (9)</t>
+  </si>
+  <si>
+    <t>4,93 (27)</t>
+  </si>
+  <si>
+    <t>5,0 (12)</t>
+  </si>
+  <si>
+    <t>4,77 (66)</t>
+  </si>
+  <si>
+    <t>4,9 (10)</t>
+  </si>
+  <si>
+    <t>4,8 (82)</t>
+  </si>
+  <si>
+    <t>4,55 (11)</t>
+  </si>
+  <si>
+    <t>4,98 (163)</t>
+  </si>
+  <si>
+    <t>4,94 (18)</t>
+  </si>
+  <si>
+    <t>4,92 (174)</t>
+  </si>
+  <si>
+    <t>4,97 (69)</t>
+  </si>
+  <si>
+    <t>4,88 (99)</t>
+  </si>
+  <si>
+    <t>5,0 (5)</t>
+  </si>
+  <si>
+    <t>4,78 (27)</t>
   </si>
   <si>
     <t>4,92 (12)</t>
   </si>
   <si>
-    <t>4,86 (14)</t>
-  </si>
-  <si>
-    <t>4,79 (287)</t>
-  </si>
-  <si>
-    <t>4,75 (63)</t>
-  </si>
-  <si>
-    <t>4,88 (99)</t>
-  </si>
-  <si>
-    <t>5,0 (12)</t>
+    <t>Novo</t>
+  </si>
+  <si>
+    <t>4,8 (10)</t>
+  </si>
+  <si>
+    <t>4,9 (30)</t>
+  </si>
+  <si>
+    <t>4,81 (16)</t>
+  </si>
+  <si>
+    <t>4,6 (20)</t>
+  </si>
+  <si>
+    <t>5,0 (18)</t>
+  </si>
+  <si>
+    <t>4,83 (18)</t>
+  </si>
+  <si>
+    <t>5,0 (11)</t>
+  </si>
+  <si>
+    <t>4,83 (24)</t>
+  </si>
+  <si>
+    <t>4,88 (8)</t>
+  </si>
+  <si>
+    <t>5,0 (10)</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>4,83 (12)</t>
+  </si>
+  <si>
+    <t>5,0 (46)</t>
+  </si>
+  <si>
+    <t>4,91 (107)</t>
+  </si>
+  <si>
+    <t>4,89 (18)</t>
+  </si>
+  <si>
+    <t>5,0 (6)</t>
+  </si>
+  <si>
+    <t>4,8 (69)</t>
+  </si>
+  <si>
+    <t>5,0 (21)</t>
+  </si>
+  <si>
+    <t>4,94 (51)</t>
+  </si>
+  <si>
+    <t>5,0 (24)</t>
+  </si>
+  <si>
+    <t>5,0 (3)</t>
+  </si>
+  <si>
+    <t>4,91 (45)</t>
+  </si>
+  <si>
+    <t>5,0 (4)</t>
+  </si>
+  <si>
+    <t>4,89 (37)</t>
+  </si>
+  <si>
+    <t>4,77 (44)</t>
+  </si>
+  <si>
+    <t>4,86 (72)</t>
   </si>
   <si>
     <t>5,0 (7)</t>
   </si>
   <si>
-    <t>4,93 (14)</t>
-  </si>
-  <si>
-    <t>4,93 (27)</t>
-  </si>
-  <si>
-    <t>4,9 (49)</t>
-  </si>
-  <si>
-    <t>4,97 (69)</t>
-  </si>
-  <si>
-    <t>4,98 (163)</t>
-  </si>
-  <si>
-    <t>4,78 (9)</t>
-  </si>
-  <si>
-    <t>4,55 (11)</t>
-  </si>
-  <si>
-    <t>5,0 (3)</t>
-  </si>
-  <si>
-    <t>4,77 (66)</t>
-  </si>
-  <si>
-    <t>4,93 (30)</t>
-  </si>
-  <si>
-    <t>4,9 (10)</t>
-  </si>
-  <si>
-    <t>4,78 (27)</t>
-  </si>
-  <si>
-    <t>4,8 (10)</t>
-  </si>
-  <si>
-    <t>Novo</t>
-  </si>
-  <si>
-    <t>5,0 (18)</t>
-  </si>
-  <si>
-    <t>5,0 (6)</t>
-  </si>
-  <si>
-    <t>5,0 (5)</t>
-  </si>
-  <si>
-    <t>4,83 (18)</t>
+    <t>4,97 (67)</t>
+  </si>
+  <si>
+    <t>4,8 (5)</t>
+  </si>
+  <si>
+    <t>4,94 (55)</t>
+  </si>
+  <si>
+    <t>4,89 (20)</t>
+  </si>
+  <si>
+    <t>4,9 (41)</t>
+  </si>
+  <si>
+    <t>4,9 (84)</t>
   </si>
   <si>
     <t>4,95 (76)</t>
   </si>
   <si>
-    <t>4,83 (24)</t>
-  </si>
-  <si>
-    <t>4,89 (20)</t>
-  </si>
-  <si>
-    <t>4,88 (8)</t>
-  </si>
-  <si>
-    <t>4,6 (20)</t>
-  </si>
-  <si>
-    <t>N/A</t>
-  </si>
-  <si>
-    <t>5,0 (30)</t>
-  </si>
-  <si>
-    <t>5,0 (11)</t>
-  </si>
-  <si>
-    <t>4,81 (16)</t>
+    <t>4,83 (30)</t>
+  </si>
+  <si>
+    <t>4,91 (11)</t>
   </si>
   <si>
     <t>4,95 (58)</t>
   </si>
   <si>
-    <t>4,66 (29)</t>
-  </si>
-  <si>
-    <t>4,75 (71)</t>
-  </si>
-  <si>
-    <t>4,95 (20)</t>
-  </si>
-  <si>
-    <t>4,83 (30)</t>
-  </si>
-  <si>
-    <t>4,86 (72)</t>
-  </si>
-  <si>
-    <t>5,0 (10)</t>
-  </si>
-  <si>
-    <t>4,83 (12)</t>
-  </si>
-  <si>
-    <t>5,0 (21)</t>
-  </si>
-  <si>
-    <t>4,91 (53)</t>
-  </si>
-  <si>
-    <t>4,84 (32)</t>
-  </si>
-  <si>
-    <t>4,94 (55)</t>
-  </si>
-  <si>
-    <t>4,97 (67)</t>
-  </si>
-  <si>
-    <t>4,6 (10)</t>
-  </si>
-  <si>
-    <t>4,9 (41)</t>
-  </si>
-  <si>
-    <t>4,77 (43)</t>
-  </si>
-  <si>
-    <t>4,91 (107)</t>
-  </si>
-  <si>
-    <t>5,0 (24)</t>
-  </si>
-  <si>
-    <t>4,97 (38)</t>
-  </si>
-  <si>
-    <t>4,8 (5)</t>
-  </si>
-  <si>
-    <t>4,88 (32)</t>
+    <t>4,76 (17)</t>
   </si>
   <si>
     <t>Superhost</t>
   </si>
   <si>
-    <t>R$ 237.46</t>
-  </si>
-  <si>
-    <t>31/05/2023 09:44:33</t>
+    <t>R$ 248.66</t>
+  </si>
+  <si>
+    <t>01/06/2023 08:43:19</t>
   </si>
 </sst>
 </file>
@@ -1284,25 +1333,22 @@
         <v>20</v>
       </c>
       <c r="D2" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="I2" t="s">
-        <v>129</v>
+        <v>138</v>
       </c>
       <c r="K2" t="s">
-        <v>147</v>
+        <v>155</v>
       </c>
       <c r="O2" t="s">
-        <v>221</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>276</v>
+        <v>232</v>
       </c>
       <c r="S2" t="s">
-        <v>277</v>
+        <v>293</v>
       </c>
       <c r="U2" t="s">
-        <v>278</v>
+        <v>294</v>
       </c>
     </row>
     <row r="3" spans="1:21">
@@ -1310,25 +1356,25 @@
         <v>20</v>
       </c>
       <c r="D3" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="I3" t="s">
-        <v>130</v>
+        <v>139</v>
       </c>
       <c r="K3" t="s">
-        <v>148</v>
+        <v>156</v>
       </c>
       <c r="O3" t="s">
-        <v>222</v>
+        <v>233</v>
       </c>
       <c r="Q3" t="s">
-        <v>276</v>
+        <v>292</v>
       </c>
       <c r="S3" t="s">
-        <v>277</v>
+        <v>293</v>
       </c>
       <c r="U3" t="s">
-        <v>278</v>
+        <v>294</v>
       </c>
     </row>
     <row r="4" spans="1:21">
@@ -1336,117 +1382,123 @@
         <v>20</v>
       </c>
       <c r="D4" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="I4" t="s">
-        <v>131</v>
+        <v>140</v>
       </c>
       <c r="K4" t="s">
-        <v>149</v>
+        <v>157</v>
       </c>
       <c r="O4" t="s">
-        <v>223</v>
+        <v>234</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>292</v>
       </c>
       <c r="S4" t="s">
-        <v>277</v>
+        <v>293</v>
       </c>
       <c r="U4" t="s">
-        <v>278</v>
+        <v>294</v>
       </c>
     </row>
     <row r="5" spans="1:21">
       <c r="A5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D5" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="I5" t="s">
-        <v>132</v>
+        <v>141</v>
       </c>
       <c r="K5" t="s">
-        <v>150</v>
+        <v>158</v>
       </c>
       <c r="O5" t="s">
-        <v>224</v>
+        <v>235</v>
       </c>
       <c r="S5" t="s">
-        <v>277</v>
+        <v>293</v>
       </c>
       <c r="U5" t="s">
-        <v>278</v>
+        <v>294</v>
       </c>
     </row>
     <row r="6" spans="1:21">
       <c r="A6" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D6" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="I6" t="s">
-        <v>133</v>
+        <v>139</v>
       </c>
       <c r="K6" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="O6" t="s">
-        <v>225</v>
+        <v>236</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>292</v>
       </c>
       <c r="S6" t="s">
-        <v>277</v>
+        <v>293</v>
       </c>
       <c r="U6" t="s">
-        <v>278</v>
+        <v>294</v>
       </c>
     </row>
     <row r="7" spans="1:21">
       <c r="A7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D7" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="I7" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
       <c r="K7" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
       <c r="O7" t="s">
-        <v>226</v>
+        <v>237</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>292</v>
       </c>
       <c r="S7" t="s">
-        <v>277</v>
+        <v>293</v>
       </c>
       <c r="U7" t="s">
-        <v>278</v>
+        <v>294</v>
       </c>
     </row>
     <row r="8" spans="1:21">
       <c r="A8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D8" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="I8" t="s">
-        <v>133</v>
+        <v>139</v>
       </c>
       <c r="K8" t="s">
-        <v>153</v>
+        <v>161</v>
       </c>
       <c r="O8" t="s">
-        <v>227</v>
-      </c>
-      <c r="Q8" t="s">
-        <v>276</v>
+        <v>238</v>
       </c>
       <c r="S8" t="s">
-        <v>277</v>
+        <v>293</v>
       </c>
       <c r="U8" t="s">
-        <v>278</v>
+        <v>294</v>
       </c>
     </row>
     <row r="9" spans="1:21">
@@ -1454,218 +1506,221 @@
         <v>20</v>
       </c>
       <c r="D9" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="I9" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="K9" t="s">
-        <v>154</v>
+        <v>162</v>
       </c>
       <c r="O9" t="s">
-        <v>228</v>
+        <v>239</v>
       </c>
       <c r="S9" t="s">
-        <v>277</v>
+        <v>293</v>
       </c>
       <c r="U9" t="s">
-        <v>278</v>
+        <v>294</v>
       </c>
     </row>
     <row r="10" spans="1:21">
       <c r="A10" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D10" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="I10" t="s">
-        <v>129</v>
+        <v>143</v>
       </c>
       <c r="K10" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="O10" t="s">
-        <v>229</v>
+        <v>240</v>
       </c>
       <c r="S10" t="s">
-        <v>277</v>
+        <v>293</v>
       </c>
       <c r="U10" t="s">
-        <v>278</v>
+        <v>294</v>
       </c>
     </row>
     <row r="11" spans="1:21">
       <c r="A11" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D11" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="I11" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="K11" t="s">
-        <v>156</v>
+        <v>164</v>
       </c>
       <c r="O11" t="s">
-        <v>230</v>
+        <v>241</v>
       </c>
       <c r="Q11" t="s">
-        <v>276</v>
+        <v>292</v>
       </c>
       <c r="S11" t="s">
-        <v>277</v>
+        <v>293</v>
       </c>
       <c r="U11" t="s">
-        <v>278</v>
+        <v>294</v>
       </c>
     </row>
     <row r="12" spans="1:21">
       <c r="A12" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="D12" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="I12" t="s">
-        <v>137</v>
+        <v>144</v>
       </c>
       <c r="K12" t="s">
-        <v>157</v>
+        <v>165</v>
       </c>
       <c r="O12" t="s">
-        <v>231</v>
+        <v>242</v>
       </c>
       <c r="Q12" t="s">
-        <v>276</v>
+        <v>292</v>
       </c>
       <c r="S12" t="s">
-        <v>277</v>
+        <v>293</v>
       </c>
       <c r="U12" t="s">
-        <v>278</v>
+        <v>294</v>
       </c>
     </row>
     <row r="13" spans="1:21">
       <c r="A13" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="D13" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="I13" t="s">
-        <v>138</v>
+        <v>145</v>
       </c>
       <c r="K13" t="s">
-        <v>158</v>
+        <v>166</v>
       </c>
       <c r="O13" t="s">
-        <v>232</v>
-      </c>
-      <c r="Q13" t="s">
-        <v>276</v>
+        <v>243</v>
       </c>
       <c r="S13" t="s">
-        <v>277</v>
+        <v>293</v>
       </c>
       <c r="U13" t="s">
-        <v>278</v>
+        <v>294</v>
       </c>
     </row>
     <row r="14" spans="1:21">
       <c r="A14" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D14" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="I14" t="s">
-        <v>129</v>
+        <v>145</v>
       </c>
       <c r="K14" t="s">
-        <v>159</v>
+        <v>167</v>
       </c>
       <c r="O14" t="s">
-        <v>233</v>
+        <v>244</v>
       </c>
       <c r="S14" t="s">
-        <v>277</v>
+        <v>293</v>
       </c>
       <c r="U14" t="s">
-        <v>278</v>
+        <v>294</v>
       </c>
     </row>
     <row r="15" spans="1:21">
       <c r="A15" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="D15" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="I15" t="s">
-        <v>137</v>
+        <v>144</v>
       </c>
       <c r="K15" t="s">
-        <v>160</v>
+        <v>168</v>
       </c>
       <c r="O15" t="s">
-        <v>234</v>
+        <v>245</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>292</v>
       </c>
       <c r="S15" t="s">
-        <v>277</v>
+        <v>293</v>
       </c>
       <c r="U15" t="s">
-        <v>278</v>
+        <v>294</v>
       </c>
     </row>
     <row r="16" spans="1:21">
       <c r="A16" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="D16" t="s">
-        <v>48</v>
+        <v>70</v>
       </c>
       <c r="I16" t="s">
-        <v>133</v>
+        <v>145</v>
       </c>
       <c r="K16" t="s">
-        <v>161</v>
+        <v>169</v>
       </c>
       <c r="O16" t="s">
-        <v>235</v>
+        <v>246</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>292</v>
       </c>
       <c r="S16" t="s">
-        <v>277</v>
+        <v>293</v>
       </c>
       <c r="U16" t="s">
-        <v>278</v>
+        <v>294</v>
       </c>
     </row>
     <row r="17" spans="1:21">
       <c r="A17" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="D17" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="I17" t="s">
-        <v>129</v>
+        <v>140</v>
       </c>
       <c r="K17" t="s">
-        <v>162</v>
+        <v>170</v>
       </c>
       <c r="O17" t="s">
-        <v>236</v>
+        <v>247</v>
       </c>
       <c r="Q17" t="s">
-        <v>276</v>
+        <v>292</v>
       </c>
       <c r="S17" t="s">
-        <v>277</v>
+        <v>293</v>
       </c>
       <c r="U17" t="s">
-        <v>278</v>
+        <v>294</v>
       </c>
     </row>
     <row r="18" spans="1:21">
@@ -1673,117 +1728,120 @@
         <v>20</v>
       </c>
       <c r="D18" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="I18" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="K18" t="s">
-        <v>163</v>
+        <v>171</v>
       </c>
       <c r="O18" t="s">
-        <v>237</v>
+        <v>248</v>
       </c>
       <c r="Q18" t="s">
-        <v>276</v>
+        <v>292</v>
       </c>
       <c r="S18" t="s">
-        <v>277</v>
+        <v>293</v>
       </c>
       <c r="U18" t="s">
-        <v>278</v>
+        <v>294</v>
       </c>
     </row>
     <row r="19" spans="1:21">
       <c r="A19" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="D19" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="I19" t="s">
-        <v>140</v>
+        <v>146</v>
       </c>
       <c r="K19" t="s">
-        <v>164</v>
+        <v>172</v>
       </c>
       <c r="O19" t="s">
-        <v>238</v>
+        <v>249</v>
       </c>
       <c r="S19" t="s">
-        <v>277</v>
+        <v>293</v>
       </c>
       <c r="U19" t="s">
-        <v>278</v>
+        <v>294</v>
       </c>
     </row>
     <row r="20" spans="1:21">
       <c r="A20" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="D20" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="I20" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="K20" t="s">
-        <v>165</v>
+        <v>173</v>
       </c>
       <c r="O20" t="s">
-        <v>239</v>
+        <v>250</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>292</v>
       </c>
       <c r="S20" t="s">
-        <v>277</v>
+        <v>293</v>
       </c>
       <c r="U20" t="s">
-        <v>278</v>
+        <v>294</v>
       </c>
     </row>
     <row r="21" spans="1:21">
       <c r="A21" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="D21" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="I21" t="s">
-        <v>129</v>
+        <v>146</v>
       </c>
       <c r="K21" t="s">
-        <v>166</v>
+        <v>172</v>
       </c>
       <c r="O21" t="s">
-        <v>240</v>
+        <v>249</v>
       </c>
       <c r="S21" t="s">
-        <v>277</v>
+        <v>293</v>
       </c>
       <c r="U21" t="s">
-        <v>278</v>
+        <v>294</v>
       </c>
     </row>
     <row r="22" spans="1:21">
       <c r="A22" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D22" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="I22" t="s">
-        <v>140</v>
+        <v>147</v>
       </c>
       <c r="K22" t="s">
-        <v>167</v>
+        <v>174</v>
       </c>
       <c r="O22" t="s">
-        <v>241</v>
+        <v>251</v>
       </c>
       <c r="S22" t="s">
-        <v>277</v>
+        <v>293</v>
       </c>
       <c r="U22" t="s">
-        <v>278</v>
+        <v>294</v>
       </c>
     </row>
     <row r="23" spans="1:21">
@@ -1791,25 +1849,25 @@
         <v>20</v>
       </c>
       <c r="D23" t="s">
-        <v>52</v>
+        <v>76</v>
       </c>
       <c r="I23" t="s">
-        <v>129</v>
+        <v>139</v>
       </c>
       <c r="K23" t="s">
-        <v>147</v>
+        <v>175</v>
       </c>
       <c r="O23" t="s">
-        <v>221</v>
+        <v>252</v>
       </c>
       <c r="Q23" t="s">
-        <v>276</v>
+        <v>292</v>
       </c>
       <c r="S23" t="s">
-        <v>277</v>
+        <v>293</v>
       </c>
       <c r="U23" t="s">
-        <v>278</v>
+        <v>294</v>
       </c>
     </row>
     <row r="24" spans="1:21">
@@ -1817,25 +1875,22 @@
         <v>28</v>
       </c>
       <c r="D24" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="I24" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="K24" t="s">
-        <v>168</v>
+        <v>176</v>
       </c>
       <c r="O24" t="s">
-        <v>238</v>
-      </c>
-      <c r="Q24" t="s">
-        <v>276</v>
+        <v>253</v>
       </c>
       <c r="S24" t="s">
-        <v>277</v>
+        <v>293</v>
       </c>
       <c r="U24" t="s">
-        <v>278</v>
+        <v>294</v>
       </c>
     </row>
     <row r="25" spans="1:21">
@@ -1843,316 +1898,313 @@
         <v>20</v>
       </c>
       <c r="D25" t="s">
-        <v>48</v>
+        <v>78</v>
       </c>
       <c r="I25" t="s">
-        <v>133</v>
+        <v>145</v>
       </c>
       <c r="K25" t="s">
-        <v>161</v>
+        <v>177</v>
       </c>
       <c r="O25" t="s">
-        <v>235</v>
+        <v>253</v>
       </c>
       <c r="S25" t="s">
-        <v>277</v>
+        <v>293</v>
       </c>
       <c r="U25" t="s">
-        <v>278</v>
+        <v>294</v>
       </c>
     </row>
     <row r="26" spans="1:21">
       <c r="A26" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D26" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="I26" t="s">
-        <v>135</v>
+        <v>145</v>
       </c>
       <c r="K26" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="O26" t="s">
-        <v>242</v>
-      </c>
-      <c r="Q26" t="s">
-        <v>276</v>
+        <v>244</v>
       </c>
       <c r="S26" t="s">
-        <v>277</v>
+        <v>293</v>
       </c>
       <c r="U26" t="s">
-        <v>278</v>
+        <v>294</v>
       </c>
     </row>
     <row r="27" spans="1:21">
       <c r="A27" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D27" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="I27" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="K27" t="s">
-        <v>170</v>
+        <v>178</v>
       </c>
       <c r="O27" t="s">
-        <v>243</v>
+        <v>254</v>
       </c>
       <c r="S27" t="s">
-        <v>277</v>
+        <v>293</v>
       </c>
       <c r="U27" t="s">
-        <v>278</v>
+        <v>294</v>
       </c>
     </row>
     <row r="28" spans="1:21">
       <c r="A28" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D28" t="s">
-        <v>56</v>
+        <v>80</v>
       </c>
       <c r="I28" t="s">
-        <v>133</v>
+        <v>144</v>
       </c>
       <c r="K28" t="s">
-        <v>151</v>
+        <v>179</v>
       </c>
       <c r="O28" t="s">
-        <v>225</v>
+        <v>255</v>
+      </c>
+      <c r="Q28" t="s">
+        <v>292</v>
       </c>
       <c r="S28" t="s">
-        <v>277</v>
+        <v>293</v>
       </c>
       <c r="U28" t="s">
-        <v>278</v>
+        <v>294</v>
       </c>
     </row>
     <row r="29" spans="1:21">
       <c r="A29" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="D29" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="I29" t="s">
-        <v>138</v>
+        <v>145</v>
       </c>
       <c r="K29" t="s">
-        <v>165</v>
+        <v>180</v>
       </c>
       <c r="O29" t="s">
-        <v>244</v>
-      </c>
-      <c r="Q29" t="s">
-        <v>276</v>
+        <v>256</v>
       </c>
       <c r="S29" t="s">
-        <v>277</v>
+        <v>293</v>
       </c>
       <c r="U29" t="s">
-        <v>278</v>
+        <v>294</v>
       </c>
     </row>
     <row r="30" spans="1:21">
       <c r="A30" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D30" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="I30" t="s">
-        <v>129</v>
+        <v>148</v>
       </c>
       <c r="K30" t="s">
-        <v>171</v>
+        <v>181</v>
       </c>
       <c r="O30" t="s">
-        <v>245</v>
-      </c>
-      <c r="Q30" t="s">
-        <v>276</v>
+        <v>257</v>
       </c>
       <c r="S30" t="s">
-        <v>277</v>
+        <v>293</v>
       </c>
       <c r="U30" t="s">
-        <v>278</v>
+        <v>294</v>
       </c>
     </row>
     <row r="31" spans="1:21">
       <c r="A31" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D31" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="I31" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="K31" t="s">
-        <v>172</v>
+        <v>182</v>
       </c>
       <c r="O31" t="s">
-        <v>246</v>
+        <v>258</v>
       </c>
       <c r="Q31" t="s">
-        <v>276</v>
+        <v>292</v>
       </c>
       <c r="S31" t="s">
-        <v>277</v>
+        <v>293</v>
       </c>
       <c r="U31" t="s">
-        <v>278</v>
+        <v>294</v>
       </c>
     </row>
     <row r="32" spans="1:21">
       <c r="A32" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D32" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="I32" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="K32" t="s">
-        <v>173</v>
+        <v>183</v>
       </c>
       <c r="O32" t="s">
-        <v>247</v>
+        <v>259</v>
+      </c>
+      <c r="Q32" t="s">
+        <v>292</v>
       </c>
       <c r="S32" t="s">
-        <v>277</v>
+        <v>293</v>
       </c>
       <c r="U32" t="s">
-        <v>278</v>
+        <v>294</v>
       </c>
     </row>
     <row r="33" spans="1:21">
       <c r="A33" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D33" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="I33" t="s">
-        <v>129</v>
+        <v>149</v>
       </c>
       <c r="K33" t="s">
-        <v>174</v>
+        <v>184</v>
       </c>
       <c r="O33" t="s">
-        <v>248</v>
+        <v>260</v>
+      </c>
+      <c r="Q33" t="s">
+        <v>292</v>
       </c>
       <c r="S33" t="s">
-        <v>277</v>
+        <v>293</v>
       </c>
       <c r="U33" t="s">
-        <v>278</v>
+        <v>294</v>
       </c>
     </row>
     <row r="34" spans="1:21">
       <c r="A34" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D34" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="I34" t="s">
-        <v>130</v>
+        <v>149</v>
       </c>
       <c r="K34" t="s">
-        <v>175</v>
+        <v>185</v>
       </c>
       <c r="O34" t="s">
-        <v>249</v>
+        <v>260</v>
+      </c>
+      <c r="Q34" t="s">
+        <v>292</v>
       </c>
       <c r="S34" t="s">
-        <v>277</v>
+        <v>293</v>
       </c>
       <c r="U34" t="s">
-        <v>278</v>
+        <v>294</v>
       </c>
     </row>
     <row r="35" spans="1:21">
       <c r="A35" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D35" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="I35" t="s">
-        <v>142</v>
+        <v>150</v>
       </c>
       <c r="K35" t="s">
-        <v>176</v>
+        <v>186</v>
       </c>
       <c r="O35" t="s">
-        <v>250</v>
+        <v>261</v>
       </c>
       <c r="S35" t="s">
-        <v>277</v>
+        <v>293</v>
       </c>
       <c r="U35" t="s">
-        <v>278</v>
+        <v>294</v>
       </c>
     </row>
     <row r="36" spans="1:21">
       <c r="A36" t="s">
-        <v>20</v>
+        <v>37</v>
       </c>
       <c r="D36" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="I36" t="s">
-        <v>131</v>
+        <v>140</v>
       </c>
       <c r="K36" t="s">
-        <v>177</v>
+        <v>187</v>
       </c>
       <c r="O36" t="s">
-        <v>251</v>
-      </c>
-      <c r="Q36" t="s">
-        <v>276</v>
+        <v>262</v>
       </c>
       <c r="S36" t="s">
-        <v>277</v>
+        <v>293</v>
       </c>
       <c r="U36" t="s">
-        <v>278</v>
+        <v>294</v>
       </c>
     </row>
     <row r="37" spans="1:21">
       <c r="A37" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="D37" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="I37" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="K37" t="s">
-        <v>158</v>
+        <v>188</v>
       </c>
       <c r="O37" t="s">
-        <v>252</v>
-      </c>
-      <c r="Q37" t="s">
-        <v>276</v>
+        <v>263</v>
       </c>
       <c r="S37" t="s">
-        <v>277</v>
+        <v>293</v>
       </c>
       <c r="U37" t="s">
-        <v>278</v>
+        <v>294</v>
       </c>
     </row>
     <row r="38" spans="1:21">
@@ -2160,68 +2212,71 @@
         <v>37</v>
       </c>
       <c r="D38" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="I38" t="s">
-        <v>129</v>
+        <v>140</v>
       </c>
       <c r="K38" t="s">
-        <v>178</v>
+        <v>187</v>
       </c>
       <c r="O38" t="s">
-        <v>241</v>
+        <v>262</v>
       </c>
       <c r="S38" t="s">
-        <v>277</v>
+        <v>293</v>
       </c>
       <c r="U38" t="s">
-        <v>278</v>
+        <v>294</v>
       </c>
     </row>
     <row r="39" spans="1:21">
       <c r="A39" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="D39" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="I39" t="s">
-        <v>129</v>
+        <v>147</v>
       </c>
       <c r="K39" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="O39" t="s">
-        <v>241</v>
+        <v>251</v>
       </c>
       <c r="S39" t="s">
-        <v>277</v>
+        <v>293</v>
       </c>
       <c r="U39" t="s">
-        <v>278</v>
+        <v>294</v>
       </c>
     </row>
     <row r="40" spans="1:21">
       <c r="A40" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="D40" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="I40" t="s">
-        <v>130</v>
+        <v>144</v>
       </c>
       <c r="K40" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="O40" t="s">
-        <v>235</v>
+        <v>250</v>
+      </c>
+      <c r="Q40" t="s">
+        <v>292</v>
       </c>
       <c r="S40" t="s">
-        <v>277</v>
+        <v>293</v>
       </c>
       <c r="U40" t="s">
-        <v>278</v>
+        <v>294</v>
       </c>
     </row>
     <row r="41" spans="1:21">
@@ -2229,97 +2284,94 @@
         <v>20</v>
       </c>
       <c r="D41" t="s">
-        <v>20</v>
+        <v>90</v>
       </c>
       <c r="I41" t="s">
-        <v>137</v>
+        <v>151</v>
       </c>
       <c r="K41" t="s">
-        <v>181</v>
+        <v>189</v>
       </c>
       <c r="O41" t="s">
-        <v>241</v>
+        <v>264</v>
       </c>
       <c r="S41" t="s">
-        <v>277</v>
+        <v>293</v>
       </c>
       <c r="U41" t="s">
-        <v>278</v>
+        <v>294</v>
       </c>
     </row>
     <row r="42" spans="1:21">
       <c r="A42" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D42" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="I42" t="s">
-        <v>143</v>
+        <v>152</v>
       </c>
       <c r="K42" t="s">
-        <v>182</v>
+        <v>190</v>
       </c>
       <c r="O42" t="s">
-        <v>253</v>
-      </c>
-      <c r="Q42" t="s">
-        <v>276</v>
+        <v>265</v>
       </c>
       <c r="S42" t="s">
-        <v>277</v>
+        <v>293</v>
       </c>
       <c r="U42" t="s">
-        <v>278</v>
+        <v>294</v>
       </c>
     </row>
     <row r="43" spans="1:21">
       <c r="A43" t="s">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="D43" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="I43" t="s">
-        <v>137</v>
+        <v>150</v>
       </c>
       <c r="K43" t="s">
-        <v>183</v>
+        <v>191</v>
       </c>
       <c r="O43" t="s">
-        <v>254</v>
+        <v>242</v>
       </c>
       <c r="S43" t="s">
-        <v>277</v>
+        <v>293</v>
       </c>
       <c r="U43" t="s">
-        <v>278</v>
+        <v>294</v>
       </c>
     </row>
     <row r="44" spans="1:21">
       <c r="A44" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D44" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="I44" t="s">
-        <v>138</v>
+        <v>150</v>
       </c>
       <c r="K44" t="s">
-        <v>162</v>
+        <v>192</v>
       </c>
       <c r="O44" t="s">
-        <v>255</v>
+        <v>266</v>
       </c>
       <c r="Q44" t="s">
-        <v>276</v>
+        <v>292</v>
       </c>
       <c r="S44" t="s">
-        <v>277</v>
+        <v>293</v>
       </c>
       <c r="U44" t="s">
-        <v>278</v>
+        <v>294</v>
       </c>
     </row>
     <row r="45" spans="1:21">
@@ -2327,143 +2379,146 @@
         <v>20</v>
       </c>
       <c r="D45" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="I45" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="K45" t="s">
-        <v>184</v>
+        <v>193</v>
       </c>
       <c r="O45" t="s">
-        <v>253</v>
+        <v>264</v>
+      </c>
+      <c r="Q45" t="s">
+        <v>292</v>
       </c>
       <c r="S45" t="s">
-        <v>277</v>
+        <v>293</v>
       </c>
       <c r="U45" t="s">
-        <v>278</v>
+        <v>294</v>
       </c>
     </row>
     <row r="46" spans="1:21">
       <c r="A46" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="D46" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="I46" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="K46" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="O46" t="s">
-        <v>256</v>
+        <v>259</v>
+      </c>
+      <c r="Q46" t="s">
+        <v>292</v>
       </c>
       <c r="S46" t="s">
-        <v>277</v>
+        <v>293</v>
       </c>
       <c r="U46" t="s">
-        <v>278</v>
+        <v>294</v>
       </c>
     </row>
     <row r="47" spans="1:21">
       <c r="A47" t="s">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="D47" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="I47" t="s">
-        <v>129</v>
+        <v>150</v>
       </c>
       <c r="K47" t="s">
-        <v>174</v>
+        <v>194</v>
       </c>
       <c r="O47" t="s">
-        <v>241</v>
+        <v>267</v>
       </c>
       <c r="S47" t="s">
-        <v>277</v>
+        <v>293</v>
       </c>
       <c r="U47" t="s">
-        <v>278</v>
+        <v>294</v>
       </c>
     </row>
     <row r="48" spans="1:21">
       <c r="A48" t="s">
-        <v>20</v>
+        <v>39</v>
       </c>
       <c r="D48" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="I48" t="s">
-        <v>132</v>
+        <v>143</v>
       </c>
       <c r="K48" t="s">
-        <v>186</v>
+        <v>195</v>
       </c>
       <c r="O48" t="s">
-        <v>257</v>
+        <v>258</v>
+      </c>
+      <c r="Q48" t="s">
+        <v>292</v>
       </c>
       <c r="S48" t="s">
-        <v>277</v>
+        <v>293</v>
       </c>
       <c r="U48" t="s">
-        <v>278</v>
+        <v>294</v>
       </c>
     </row>
     <row r="49" spans="1:21">
       <c r="A49" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D49" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="I49" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="K49" t="s">
-        <v>187</v>
+        <v>196</v>
       </c>
       <c r="O49" t="s">
-        <v>241</v>
-      </c>
-      <c r="Q49" t="s">
-        <v>276</v>
+        <v>268</v>
       </c>
       <c r="S49" t="s">
-        <v>277</v>
+        <v>293</v>
       </c>
       <c r="U49" t="s">
-        <v>278</v>
+        <v>294</v>
       </c>
     </row>
     <row r="50" spans="1:21">
       <c r="A50" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D50" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="I50" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="K50" t="s">
-        <v>188</v>
+        <v>197</v>
       </c>
       <c r="O50" t="s">
-        <v>258</v>
-      </c>
-      <c r="Q50" t="s">
-        <v>276</v>
+        <v>253</v>
       </c>
       <c r="S50" t="s">
-        <v>277</v>
+        <v>293</v>
       </c>
       <c r="U50" t="s">
-        <v>278</v>
+        <v>294</v>
       </c>
     </row>
     <row r="51" spans="1:21">
@@ -2471,264 +2526,264 @@
         <v>20</v>
       </c>
       <c r="D51" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="I51" t="s">
-        <v>134</v>
+        <v>144</v>
       </c>
       <c r="K51" t="s">
-        <v>189</v>
+        <v>198</v>
       </c>
       <c r="O51" t="s">
-        <v>241</v>
+        <v>269</v>
       </c>
       <c r="S51" t="s">
-        <v>277</v>
+        <v>293</v>
       </c>
       <c r="U51" t="s">
-        <v>278</v>
+        <v>294</v>
       </c>
     </row>
     <row r="52" spans="1:21">
       <c r="A52" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D52" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="I52" t="s">
-        <v>129</v>
+        <v>150</v>
       </c>
       <c r="K52" t="s">
-        <v>190</v>
+        <v>199</v>
       </c>
       <c r="O52" t="s">
-        <v>241</v>
+        <v>270</v>
+      </c>
+      <c r="Q52" t="s">
+        <v>292</v>
       </c>
       <c r="S52" t="s">
-        <v>277</v>
+        <v>293</v>
       </c>
       <c r="U52" t="s">
-        <v>278</v>
+        <v>294</v>
       </c>
     </row>
     <row r="53" spans="1:21">
       <c r="A53" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D53" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="I53" t="s">
-        <v>129</v>
+        <v>143</v>
       </c>
       <c r="K53" t="s">
-        <v>191</v>
+        <v>200</v>
       </c>
       <c r="O53" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="S53" t="s">
-        <v>277</v>
+        <v>293</v>
       </c>
       <c r="U53" t="s">
-        <v>278</v>
+        <v>294</v>
       </c>
     </row>
     <row r="54" spans="1:21">
       <c r="A54" t="s">
-        <v>42</v>
+        <v>23</v>
       </c>
       <c r="D54" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="I54" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
       <c r="K54" t="s">
-        <v>192</v>
+        <v>201</v>
       </c>
       <c r="O54" t="s">
-        <v>260</v>
+        <v>271</v>
       </c>
       <c r="Q54" t="s">
-        <v>276</v>
+        <v>292</v>
       </c>
       <c r="S54" t="s">
-        <v>277</v>
+        <v>293</v>
       </c>
       <c r="U54" t="s">
-        <v>278</v>
+        <v>294</v>
       </c>
     </row>
     <row r="55" spans="1:21">
       <c r="A55" t="s">
-        <v>43</v>
+        <v>20</v>
       </c>
       <c r="D55" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="I55" t="s">
-        <v>129</v>
+        <v>147</v>
       </c>
       <c r="K55" t="s">
-        <v>193</v>
+        <v>202</v>
       </c>
       <c r="O55" t="s">
-        <v>243</v>
+        <v>265</v>
+      </c>
+      <c r="Q55" t="s">
+        <v>292</v>
       </c>
       <c r="S55" t="s">
-        <v>277</v>
+        <v>293</v>
       </c>
       <c r="U55" t="s">
-        <v>278</v>
+        <v>294</v>
       </c>
     </row>
     <row r="56" spans="1:21">
       <c r="A56" t="s">
-        <v>20</v>
+        <v>41</v>
       </c>
       <c r="D56" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="I56" t="s">
-        <v>129</v>
+        <v>139</v>
       </c>
       <c r="K56" t="s">
-        <v>194</v>
+        <v>159</v>
       </c>
       <c r="O56" t="s">
-        <v>261</v>
+        <v>272</v>
+      </c>
+      <c r="Q56" t="s">
+        <v>292</v>
       </c>
       <c r="S56" t="s">
-        <v>277</v>
+        <v>293</v>
       </c>
       <c r="U56" t="s">
-        <v>278</v>
+        <v>294</v>
       </c>
     </row>
     <row r="57" spans="1:21">
       <c r="A57" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
       <c r="D57" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="I57" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="K57" t="s">
-        <v>195</v>
+        <v>203</v>
       </c>
       <c r="O57" t="s">
-        <v>262</v>
-      </c>
-      <c r="Q57" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="S57" t="s">
-        <v>277</v>
+        <v>293</v>
       </c>
       <c r="U57" t="s">
-        <v>278</v>
+        <v>294</v>
       </c>
     </row>
     <row r="58" spans="1:21">
       <c r="A58" t="s">
-        <v>20</v>
+        <v>43</v>
       </c>
       <c r="D58" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="I58" t="s">
-        <v>134</v>
+        <v>151</v>
       </c>
       <c r="K58" t="s">
-        <v>196</v>
+        <v>204</v>
       </c>
       <c r="O58" t="s">
-        <v>235</v>
+        <v>253</v>
       </c>
       <c r="S58" t="s">
-        <v>277</v>
+        <v>293</v>
       </c>
       <c r="U58" t="s">
-        <v>278</v>
+        <v>294</v>
       </c>
     </row>
     <row r="59" spans="1:21">
       <c r="A59" t="s">
-        <v>23</v>
+        <v>44</v>
       </c>
       <c r="D59" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="I59" t="s">
-        <v>133</v>
+        <v>140</v>
       </c>
       <c r="K59" t="s">
-        <v>197</v>
+        <v>155</v>
       </c>
       <c r="O59" t="s">
-        <v>263</v>
-      </c>
-      <c r="Q59" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="S59" t="s">
-        <v>277</v>
+        <v>293</v>
       </c>
       <c r="U59" t="s">
-        <v>278</v>
+        <v>294</v>
       </c>
     </row>
     <row r="60" spans="1:21">
       <c r="A60" t="s">
-        <v>20</v>
+        <v>45</v>
       </c>
       <c r="D60" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="I60" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="K60" t="s">
-        <v>198</v>
+        <v>205</v>
       </c>
       <c r="O60" t="s">
-        <v>251</v>
+        <v>275</v>
       </c>
       <c r="S60" t="s">
-        <v>277</v>
+        <v>293</v>
       </c>
       <c r="U60" t="s">
-        <v>278</v>
+        <v>294</v>
       </c>
     </row>
     <row r="61" spans="1:21">
       <c r="A61" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D61" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="I61" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
       <c r="K61" t="s">
-        <v>199</v>
+        <v>206</v>
       </c>
       <c r="O61" t="s">
-        <v>264</v>
-      </c>
-      <c r="Q61" t="s">
-        <v>276</v>
+        <v>260</v>
       </c>
       <c r="S61" t="s">
-        <v>277</v>
+        <v>293</v>
       </c>
       <c r="U61" t="s">
-        <v>278</v>
+        <v>294</v>
       </c>
     </row>
     <row r="62" spans="1:21">
@@ -2736,25 +2791,22 @@
         <v>20</v>
       </c>
       <c r="D62" t="s">
-        <v>82</v>
+        <v>110</v>
       </c>
       <c r="I62" t="s">
-        <v>131</v>
+        <v>144</v>
       </c>
       <c r="K62" t="s">
-        <v>177</v>
+        <v>207</v>
       </c>
       <c r="O62" t="s">
-        <v>251</v>
-      </c>
-      <c r="Q62" t="s">
-        <v>276</v>
+        <v>264</v>
       </c>
       <c r="S62" t="s">
-        <v>277</v>
+        <v>293</v>
       </c>
       <c r="U62" t="s">
-        <v>278</v>
+        <v>294</v>
       </c>
     </row>
     <row r="63" spans="1:21">
@@ -2762,25 +2814,22 @@
         <v>20</v>
       </c>
       <c r="D63" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="I63" t="s">
-        <v>134</v>
+        <v>144</v>
       </c>
       <c r="K63" t="s">
-        <v>200</v>
+        <v>208</v>
       </c>
       <c r="O63" t="s">
-        <v>242</v>
-      </c>
-      <c r="Q63" t="s">
         <v>276</v>
       </c>
       <c r="S63" t="s">
-        <v>277</v>
+        <v>293</v>
       </c>
       <c r="U63" t="s">
-        <v>278</v>
+        <v>294</v>
       </c>
     </row>
     <row r="64" spans="1:21">
@@ -2788,22 +2837,22 @@
         <v>20</v>
       </c>
       <c r="D64" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="I64" t="s">
-        <v>134</v>
+        <v>143</v>
       </c>
       <c r="K64" t="s">
-        <v>201</v>
+        <v>209</v>
       </c>
       <c r="O64" t="s">
-        <v>241</v>
+        <v>253</v>
       </c>
       <c r="S64" t="s">
-        <v>277</v>
+        <v>293</v>
       </c>
       <c r="U64" t="s">
-        <v>278</v>
+        <v>294</v>
       </c>
     </row>
     <row r="65" spans="1:21">
@@ -2811,241 +2860,247 @@
         <v>20</v>
       </c>
       <c r="D65" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="I65" t="s">
-        <v>137</v>
+        <v>147</v>
       </c>
       <c r="K65" t="s">
         <v>202</v>
       </c>
       <c r="O65" t="s">
-        <v>241</v>
+        <v>265</v>
+      </c>
+      <c r="Q65" t="s">
+        <v>292</v>
       </c>
       <c r="S65" t="s">
-        <v>277</v>
+        <v>293</v>
       </c>
       <c r="U65" t="s">
-        <v>278</v>
+        <v>294</v>
       </c>
     </row>
     <row r="66" spans="1:21">
       <c r="A66" t="s">
-        <v>39</v>
+        <v>20</v>
       </c>
       <c r="D66" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="I66" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="K66" t="s">
-        <v>203</v>
+        <v>210</v>
       </c>
       <c r="O66" t="s">
-        <v>253</v>
-      </c>
-      <c r="Q66" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="S66" t="s">
-        <v>277</v>
+        <v>293</v>
       </c>
       <c r="U66" t="s">
-        <v>278</v>
+        <v>294</v>
       </c>
     </row>
     <row r="67" spans="1:21">
       <c r="A67" t="s">
-        <v>20</v>
+        <v>46</v>
       </c>
       <c r="D67" t="s">
-        <v>71</v>
+        <v>114</v>
       </c>
       <c r="I67" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="K67" t="s">
-        <v>167</v>
+        <v>211</v>
       </c>
       <c r="O67" t="s">
-        <v>241</v>
+        <v>253</v>
       </c>
       <c r="S67" t="s">
-        <v>277</v>
+        <v>293</v>
       </c>
       <c r="U67" t="s">
-        <v>278</v>
+        <v>294</v>
       </c>
     </row>
     <row r="68" spans="1:21">
       <c r="A68" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="D68" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="I68" t="s">
-        <v>140</v>
+        <v>153</v>
       </c>
       <c r="K68" t="s">
-        <v>204</v>
+        <v>212</v>
       </c>
       <c r="O68" t="s">
-        <v>265</v>
+        <v>277</v>
+      </c>
+      <c r="Q68" t="s">
+        <v>292</v>
       </c>
       <c r="S68" t="s">
-        <v>277</v>
+        <v>293</v>
       </c>
       <c r="U68" t="s">
-        <v>278</v>
+        <v>294</v>
       </c>
     </row>
     <row r="69" spans="1:21">
       <c r="A69" t="s">
-        <v>20</v>
+        <v>44</v>
       </c>
       <c r="D69" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="I69" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="K69" t="s">
-        <v>205</v>
+        <v>213</v>
       </c>
       <c r="O69" t="s">
-        <v>266</v>
+        <v>278</v>
       </c>
       <c r="Q69" t="s">
-        <v>276</v>
+        <v>292</v>
       </c>
       <c r="S69" t="s">
-        <v>277</v>
+        <v>293</v>
       </c>
       <c r="U69" t="s">
-        <v>278</v>
+        <v>294</v>
       </c>
     </row>
     <row r="70" spans="1:21">
       <c r="A70" t="s">
-        <v>25</v>
+        <v>48</v>
       </c>
       <c r="D70" t="s">
-        <v>70</v>
+        <v>117</v>
       </c>
       <c r="I70" t="s">
-        <v>129</v>
+        <v>153</v>
       </c>
       <c r="K70" t="s">
-        <v>166</v>
+        <v>214</v>
       </c>
       <c r="O70" t="s">
-        <v>240</v>
+        <v>279</v>
+      </c>
+      <c r="Q70" t="s">
+        <v>292</v>
       </c>
       <c r="S70" t="s">
-        <v>277</v>
+        <v>293</v>
       </c>
       <c r="U70" t="s">
-        <v>278</v>
+        <v>294</v>
       </c>
     </row>
     <row r="71" spans="1:21">
       <c r="A71" t="s">
-        <v>45</v>
+        <v>22</v>
       </c>
       <c r="D71" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="I71" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="K71" t="s">
-        <v>206</v>
+        <v>215</v>
       </c>
       <c r="O71" t="s">
-        <v>267</v>
-      </c>
-      <c r="Q71" t="s">
-        <v>276</v>
+        <v>264</v>
       </c>
       <c r="S71" t="s">
-        <v>277</v>
+        <v>293</v>
       </c>
       <c r="U71" t="s">
-        <v>278</v>
+        <v>294</v>
       </c>
     </row>
     <row r="72" spans="1:21">
       <c r="A72" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D72" t="s">
-        <v>98</v>
+        <v>119</v>
       </c>
       <c r="I72" t="s">
-        <v>129</v>
+        <v>153</v>
       </c>
       <c r="K72" t="s">
-        <v>191</v>
+        <v>216</v>
       </c>
       <c r="O72" t="s">
-        <v>259</v>
+        <v>280</v>
       </c>
       <c r="S72" t="s">
-        <v>277</v>
+        <v>293</v>
       </c>
       <c r="U72" t="s">
-        <v>278</v>
+        <v>294</v>
       </c>
     </row>
     <row r="73" spans="1:21">
       <c r="A73" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D73" t="s">
-        <v>85</v>
+        <v>120</v>
       </c>
       <c r="I73" t="s">
-        <v>129</v>
+        <v>146</v>
       </c>
       <c r="K73" t="s">
-        <v>179</v>
+        <v>217</v>
       </c>
       <c r="O73" t="s">
-        <v>241</v>
+        <v>280</v>
+      </c>
+      <c r="Q73" t="s">
+        <v>292</v>
       </c>
       <c r="S73" t="s">
-        <v>277</v>
+        <v>293</v>
       </c>
       <c r="U73" t="s">
-        <v>278</v>
+        <v>294</v>
       </c>
     </row>
     <row r="74" spans="1:21">
       <c r="A74" t="s">
-        <v>22</v>
+        <v>49</v>
       </c>
       <c r="D74" t="s">
-        <v>106</v>
+        <v>121</v>
       </c>
       <c r="I74" t="s">
-        <v>134</v>
+        <v>153</v>
       </c>
       <c r="K74" t="s">
-        <v>199</v>
+        <v>218</v>
       </c>
       <c r="O74" t="s">
-        <v>264</v>
+        <v>281</v>
       </c>
       <c r="Q74" t="s">
-        <v>276</v>
+        <v>292</v>
       </c>
       <c r="S74" t="s">
-        <v>277</v>
+        <v>293</v>
       </c>
       <c r="U74" t="s">
-        <v>278</v>
+        <v>294</v>
       </c>
     </row>
     <row r="75" spans="1:21">
@@ -3053,25 +3108,22 @@
         <v>20</v>
       </c>
       <c r="D75" t="s">
-        <v>107</v>
+        <v>122</v>
       </c>
       <c r="I75" t="s">
-        <v>134</v>
+        <v>146</v>
       </c>
       <c r="K75" t="s">
-        <v>200</v>
+        <v>219</v>
       </c>
       <c r="O75" t="s">
-        <v>242</v>
-      </c>
-      <c r="Q75" t="s">
-        <v>276</v>
+        <v>282</v>
       </c>
       <c r="S75" t="s">
-        <v>277</v>
+        <v>293</v>
       </c>
       <c r="U75" t="s">
-        <v>278</v>
+        <v>294</v>
       </c>
     </row>
     <row r="76" spans="1:21">
@@ -3079,97 +3131,97 @@
         <v>20</v>
       </c>
       <c r="D76" t="s">
-        <v>114</v>
+        <v>123</v>
       </c>
       <c r="I76" t="s">
-        <v>134</v>
+        <v>143</v>
       </c>
       <c r="K76" t="s">
-        <v>207</v>
+        <v>220</v>
       </c>
       <c r="O76" t="s">
-        <v>241</v>
+        <v>253</v>
       </c>
       <c r="S76" t="s">
-        <v>277</v>
+        <v>293</v>
       </c>
       <c r="U76" t="s">
-        <v>278</v>
+        <v>294</v>
       </c>
     </row>
     <row r="77" spans="1:21">
       <c r="A77" t="s">
-        <v>41</v>
+        <v>20</v>
       </c>
       <c r="D77" t="s">
-        <v>115</v>
+        <v>124</v>
       </c>
       <c r="I77" t="s">
-        <v>136</v>
+        <v>153</v>
       </c>
       <c r="K77" t="s">
-        <v>208</v>
+        <v>221</v>
       </c>
       <c r="O77" t="s">
-        <v>241</v>
+        <v>283</v>
       </c>
       <c r="Q77" t="s">
-        <v>276</v>
+        <v>292</v>
       </c>
       <c r="S77" t="s">
-        <v>277</v>
+        <v>293</v>
       </c>
       <c r="U77" t="s">
-        <v>278</v>
+        <v>294</v>
       </c>
     </row>
     <row r="78" spans="1:21">
       <c r="A78" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="D78" t="s">
-        <v>116</v>
+        <v>125</v>
       </c>
       <c r="I78" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="K78" t="s">
-        <v>209</v>
+        <v>222</v>
       </c>
       <c r="O78" t="s">
-        <v>235</v>
+        <v>246</v>
+      </c>
+      <c r="Q78" t="s">
+        <v>292</v>
       </c>
       <c r="S78" t="s">
-        <v>277</v>
+        <v>293</v>
       </c>
       <c r="U78" t="s">
-        <v>278</v>
+        <v>294</v>
       </c>
     </row>
     <row r="79" spans="1:21">
       <c r="A79" t="s">
-        <v>47</v>
+        <v>20</v>
       </c>
       <c r="D79" t="s">
-        <v>117</v>
+        <v>126</v>
       </c>
       <c r="I79" t="s">
-        <v>137</v>
+        <v>150</v>
       </c>
       <c r="K79" t="s">
-        <v>173</v>
+        <v>223</v>
       </c>
       <c r="O79" t="s">
-        <v>268</v>
-      </c>
-      <c r="Q79" t="s">
-        <v>276</v>
+        <v>253</v>
       </c>
       <c r="S79" t="s">
-        <v>277</v>
+        <v>293</v>
       </c>
       <c r="U79" t="s">
-        <v>278</v>
+        <v>294</v>
       </c>
     </row>
     <row r="80" spans="1:21">
@@ -3177,287 +3229,293 @@
         <v>20</v>
       </c>
       <c r="D80" t="s">
-        <v>105</v>
+        <v>127</v>
       </c>
       <c r="I80" t="s">
         <v>139</v>
       </c>
       <c r="K80" t="s">
-        <v>198</v>
+        <v>224</v>
       </c>
       <c r="O80" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="S80" t="s">
-        <v>277</v>
+        <v>293</v>
       </c>
       <c r="U80" t="s">
-        <v>278</v>
+        <v>294</v>
       </c>
     </row>
     <row r="81" spans="1:21">
       <c r="A81" t="s">
-        <v>20</v>
+        <v>51</v>
       </c>
       <c r="D81" t="s">
-        <v>118</v>
+        <v>128</v>
       </c>
       <c r="I81" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
       <c r="K81" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="O81" t="s">
-        <v>241</v>
+        <v>284</v>
       </c>
       <c r="S81" t="s">
-        <v>277</v>
+        <v>293</v>
       </c>
       <c r="U81" t="s">
-        <v>278</v>
+        <v>294</v>
       </c>
     </row>
     <row r="82" spans="1:21">
       <c r="A82" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="D82" t="s">
-        <v>119</v>
+        <v>129</v>
       </c>
       <c r="I82" t="s">
-        <v>141</v>
+        <v>150</v>
       </c>
       <c r="K82" t="s">
-        <v>211</v>
+        <v>225</v>
       </c>
       <c r="O82" t="s">
-        <v>269</v>
-      </c>
-      <c r="Q82" t="s">
-        <v>276</v>
+        <v>253</v>
       </c>
       <c r="S82" t="s">
-        <v>277</v>
+        <v>293</v>
       </c>
       <c r="U82" t="s">
-        <v>278</v>
+        <v>294</v>
       </c>
     </row>
     <row r="83" spans="1:21">
       <c r="A83" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="D83" t="s">
-        <v>120</v>
+        <v>130</v>
       </c>
       <c r="I83" t="s">
-        <v>134</v>
+        <v>147</v>
       </c>
       <c r="K83" t="s">
-        <v>212</v>
+        <v>202</v>
       </c>
       <c r="O83" t="s">
-        <v>251</v>
+        <v>285</v>
+      </c>
+      <c r="Q83" t="s">
+        <v>292</v>
       </c>
       <c r="S83" t="s">
-        <v>277</v>
+        <v>293</v>
       </c>
       <c r="U83" t="s">
-        <v>278</v>
+        <v>294</v>
       </c>
     </row>
     <row r="84" spans="1:21">
       <c r="A84" t="s">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="D84" t="s">
-        <v>121</v>
+        <v>131</v>
       </c>
       <c r="I84" t="s">
-        <v>137</v>
+        <v>150</v>
       </c>
       <c r="K84" t="s">
-        <v>213</v>
+        <v>226</v>
       </c>
       <c r="O84" t="s">
-        <v>270</v>
+        <v>286</v>
       </c>
       <c r="Q84" t="s">
-        <v>276</v>
+        <v>292</v>
       </c>
       <c r="S84" t="s">
-        <v>277</v>
+        <v>293</v>
       </c>
       <c r="U84" t="s">
-        <v>278</v>
+        <v>294</v>
       </c>
     </row>
     <row r="85" spans="1:21">
       <c r="A85" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="D85" t="s">
-        <v>122</v>
+        <v>132</v>
       </c>
       <c r="I85" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="K85" t="s">
-        <v>214</v>
+        <v>227</v>
       </c>
       <c r="O85" t="s">
-        <v>271</v>
+        <v>287</v>
+      </c>
+      <c r="Q85" t="s">
+        <v>292</v>
       </c>
       <c r="S85" t="s">
-        <v>277</v>
+        <v>293</v>
       </c>
       <c r="U85" t="s">
-        <v>278</v>
+        <v>294</v>
       </c>
     </row>
     <row r="86" spans="1:21">
       <c r="A86" t="s">
-        <v>49</v>
+        <v>20</v>
       </c>
       <c r="D86" t="s">
-        <v>123</v>
+        <v>109</v>
       </c>
       <c r="I86" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="K86" t="s">
-        <v>215</v>
+        <v>206</v>
       </c>
       <c r="O86" t="s">
-        <v>233</v>
+        <v>260</v>
       </c>
       <c r="S86" t="s">
-        <v>277</v>
+        <v>293</v>
       </c>
       <c r="U86" t="s">
-        <v>278</v>
+        <v>294</v>
       </c>
     </row>
     <row r="87" spans="1:21">
       <c r="A87" t="s">
-        <v>50</v>
+        <v>22</v>
       </c>
       <c r="D87" t="s">
-        <v>124</v>
+        <v>133</v>
       </c>
       <c r="I87" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="K87" t="s">
-        <v>216</v>
+        <v>228</v>
       </c>
       <c r="O87" t="s">
-        <v>272</v>
+        <v>288</v>
       </c>
       <c r="S87" t="s">
-        <v>277</v>
+        <v>293</v>
       </c>
       <c r="U87" t="s">
-        <v>278</v>
+        <v>294</v>
       </c>
     </row>
     <row r="88" spans="1:21">
       <c r="A88" t="s">
-        <v>32</v>
+        <v>54</v>
       </c>
       <c r="D88" t="s">
-        <v>125</v>
+        <v>134</v>
       </c>
       <c r="I88" t="s">
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="K88" t="s">
-        <v>217</v>
+        <v>229</v>
       </c>
       <c r="O88" t="s">
-        <v>262</v>
+        <v>289</v>
+      </c>
+      <c r="Q88" t="s">
+        <v>292</v>
       </c>
       <c r="S88" t="s">
-        <v>277</v>
+        <v>293</v>
       </c>
       <c r="U88" t="s">
-        <v>278</v>
+        <v>294</v>
       </c>
     </row>
     <row r="89" spans="1:21">
       <c r="A89" t="s">
-        <v>20</v>
+        <v>55</v>
       </c>
       <c r="D89" t="s">
-        <v>126</v>
+        <v>135</v>
       </c>
       <c r="I89" t="s">
-        <v>146</v>
+        <v>153</v>
       </c>
       <c r="K89" t="s">
-        <v>218</v>
+        <v>230</v>
       </c>
       <c r="O89" t="s">
-        <v>273</v>
+        <v>258</v>
       </c>
       <c r="Q89" t="s">
-        <v>276</v>
+        <v>292</v>
       </c>
       <c r="S89" t="s">
-        <v>277</v>
+        <v>293</v>
       </c>
       <c r="U89" t="s">
-        <v>278</v>
+        <v>294</v>
       </c>
     </row>
     <row r="90" spans="1:21">
       <c r="A90" t="s">
-        <v>20</v>
+        <v>37</v>
       </c>
       <c r="D90" t="s">
-        <v>127</v>
+        <v>136</v>
       </c>
       <c r="I90" t="s">
-        <v>133</v>
+        <v>144</v>
       </c>
       <c r="K90" t="s">
-        <v>219</v>
+        <v>164</v>
       </c>
       <c r="O90" t="s">
-        <v>274</v>
+        <v>290</v>
+      </c>
+      <c r="Q90" t="s">
+        <v>292</v>
       </c>
       <c r="S90" t="s">
-        <v>277</v>
+        <v>293</v>
       </c>
       <c r="U90" t="s">
-        <v>278</v>
+        <v>294</v>
       </c>
     </row>
     <row r="91" spans="1:21">
       <c r="A91" t="s">
-        <v>51</v>
+        <v>20</v>
       </c>
       <c r="D91" t="s">
-        <v>128</v>
+        <v>137</v>
       </c>
       <c r="I91" t="s">
-        <v>144</v>
+        <v>154</v>
       </c>
       <c r="K91" t="s">
-        <v>220</v>
+        <v>231</v>
       </c>
       <c r="O91" t="s">
-        <v>275</v>
-      </c>
-      <c r="Q91" t="s">
-        <v>276</v>
+        <v>291</v>
       </c>
       <c r="S91" t="s">
-        <v>277</v>
+        <v>293</v>
       </c>
       <c r="U91" t="s">
-        <v>278</v>
+        <v>294</v>
       </c>
     </row>
   </sheetData>

</xml_diff>